<commit_message>
Added Zach's estimated hours
</commit_message>
<xml_diff>
--- a/Management/Burndown.xlsx
+++ b/Management/Burndown.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-15" windowWidth="25605" windowHeight="14520" activeTab="3"/>
@@ -12,7 +12,10 @@
     <sheet name="Sp2" sheetId="4" r:id="rId3"/>
     <sheet name="Sp3" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -646,12 +649,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -667,20 +664,11 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -700,16 +688,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="60% - Accent1 2" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -941,22 +975,22 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="37699968"/>
-        <c:axId val="37701504"/>
+        <c:axId val="356541920"/>
+        <c:axId val="356539568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="37699968"/>
+        <c:axId val="356541920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37701504"/>
+        <c:crossAx val="356539568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -964,7 +998,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="37701504"/>
+        <c:axId val="356539568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -975,7 +1009,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37699968"/>
+        <c:crossAx val="356541920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1232,13 +1266,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="37735040"/>
-        <c:axId val="38805888"/>
+        <c:axId val="356546232"/>
+        <c:axId val="356547016"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="37735040"/>
+        <c:axId val="356546232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1248,14 +1281,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38805888"/>
+        <c:crossAx val="356547016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="38805888"/>
+        <c:axId val="356547016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1266,7 +1299,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37735040"/>
+        <c:crossAx val="356546232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1487,13 +1520,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="103560320"/>
-        <c:axId val="103561856"/>
+        <c:axId val="356543880"/>
+        <c:axId val="356550544"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="103560320"/>
+        <c:axId val="356543880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1503,14 +1535,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103561856"/>
+        <c:crossAx val="356550544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="103561856"/>
+        <c:axId val="356550544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1521,7 +1553,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103560320"/>
+        <c:crossAx val="356543880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1802,13 +1834,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="103605760"/>
-        <c:axId val="103607296"/>
+        <c:axId val="356547408"/>
+        <c:axId val="356538392"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="103605760"/>
+        <c:axId val="356547408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1818,14 +1849,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103607296"/>
+        <c:crossAx val="356538392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="103607296"/>
+        <c:axId val="356538392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1836,14 +1867,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103605760"/>
+        <c:crossAx val="356547408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2045,7 +2075,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2080,7 +2110,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4643,7 +4673,7 @@
       <c r="A6" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="81">
+      <c r="B6" s="79">
         <v>1</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -4696,7 +4726,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="67"/>
-      <c r="B7" s="82"/>
+      <c r="B7" s="80"/>
       <c r="C7" s="45" t="s">
         <v>16</v>
       </c>
@@ -4717,7 +4747,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="67"/>
-      <c r="B8" s="82"/>
+      <c r="B8" s="80"/>
       <c r="C8" s="45" t="s">
         <v>17</v>
       </c>
@@ -4740,7 +4770,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="67"/>
-      <c r="B9" s="83"/>
+      <c r="B9" s="81"/>
       <c r="C9" s="46" t="s">
         <v>18</v>
       </c>
@@ -4761,7 +4791,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="67"/>
-      <c r="B10" s="84" t="s">
+      <c r="B10" s="82" t="s">
         <v>35</v>
       </c>
       <c r="C10" s="47" t="s">
@@ -4814,7 +4844,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="67"/>
-      <c r="B11" s="85"/>
+      <c r="B11" s="83"/>
       <c r="C11" s="45" t="s">
         <v>16</v>
       </c>
@@ -4835,7 +4865,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="67"/>
-      <c r="B12" s="85"/>
+      <c r="B12" s="83"/>
       <c r="C12" s="45" t="s">
         <v>17</v>
       </c>
@@ -4856,7 +4886,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="67"/>
-      <c r="B13" s="85"/>
+      <c r="B13" s="83"/>
       <c r="C13" s="46" t="s">
         <v>18</v>
       </c>
@@ -4879,7 +4909,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="67"/>
-      <c r="B14" s="85"/>
+      <c r="B14" s="83"/>
       <c r="C14" s="52" t="s">
         <v>33</v>
       </c>
@@ -4930,7 +4960,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="67"/>
-      <c r="B15" s="85"/>
+      <c r="B15" s="83"/>
       <c r="C15" s="45" t="s">
         <v>16</v>
       </c>
@@ -4957,7 +4987,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="67"/>
-      <c r="B16" s="85"/>
+      <c r="B16" s="83"/>
       <c r="C16" s="45" t="s">
         <v>17</v>
       </c>
@@ -4980,7 +5010,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="67"/>
-      <c r="B17" s="85"/>
+      <c r="B17" s="83"/>
       <c r="C17" s="45" t="s">
         <v>18</v>
       </c>
@@ -5123,7 +5153,7 @@
     </row>
     <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="67"/>
-      <c r="B22" s="79"/>
+      <c r="B22" s="84"/>
       <c r="C22" s="49" t="s">
         <v>31</v>
       </c>
@@ -5174,7 +5204,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="67"/>
-      <c r="B23" s="79"/>
+      <c r="B23" s="84"/>
       <c r="C23" s="45" t="s">
         <v>16</v>
       </c>
@@ -5195,7 +5225,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="67"/>
-      <c r="B24" s="79"/>
+      <c r="B24" s="84"/>
       <c r="C24" s="45" t="s">
         <v>17</v>
       </c>
@@ -5216,7 +5246,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="68"/>
-      <c r="B25" s="80"/>
+      <c r="B25" s="85"/>
       <c r="C25" s="46" t="s">
         <v>18</v>
       </c>
@@ -5297,7 +5327,7 @@
       <c r="A28" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="81">
+      <c r="B28" s="79">
         <v>1</v>
       </c>
       <c r="C28" s="10" t="s">
@@ -5347,7 +5377,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="67"/>
-      <c r="B29" s="82"/>
+      <c r="B29" s="80"/>
       <c r="C29" s="45" t="s">
         <v>16</v>
       </c>
@@ -5368,7 +5398,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="67"/>
-      <c r="B30" s="82"/>
+      <c r="B30" s="80"/>
       <c r="C30" s="45" t="s">
         <v>17</v>
       </c>
@@ -5407,7 +5437,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="67"/>
-      <c r="B31" s="83"/>
+      <c r="B31" s="81"/>
       <c r="C31" s="46" t="s">
         <v>18</v>
       </c>
@@ -5428,7 +5458,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="67"/>
-      <c r="B32" s="84" t="s">
+      <c r="B32" s="82" t="s">
         <v>35</v>
       </c>
       <c r="C32" s="47" t="s">
@@ -5478,7 +5508,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="67"/>
-      <c r="B33" s="85"/>
+      <c r="B33" s="83"/>
       <c r="C33" s="45" t="s">
         <v>16</v>
       </c>
@@ -5517,7 +5547,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="67"/>
-      <c r="B34" s="85"/>
+      <c r="B34" s="83"/>
       <c r="C34" s="45" t="s">
         <v>17</v>
       </c>
@@ -5538,7 +5568,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="67"/>
-      <c r="B35" s="85"/>
+      <c r="B35" s="83"/>
       <c r="C35" s="46" t="s">
         <v>18</v>
       </c>
@@ -5577,7 +5607,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="67"/>
-      <c r="B36" s="85"/>
+      <c r="B36" s="83"/>
       <c r="C36" s="52" t="s">
         <v>33</v>
       </c>
@@ -5625,7 +5655,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="67"/>
-      <c r="B37" s="85"/>
+      <c r="B37" s="83"/>
       <c r="C37" s="45" t="s">
         <v>16</v>
       </c>
@@ -5664,7 +5694,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="67"/>
-      <c r="B38" s="85"/>
+      <c r="B38" s="83"/>
       <c r="C38" s="45" t="s">
         <v>17</v>
       </c>
@@ -5703,7 +5733,7 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="67"/>
-      <c r="B39" s="85"/>
+      <c r="B39" s="83"/>
       <c r="C39" s="45" t="s">
         <v>18</v>
       </c>
@@ -5873,7 +5903,7 @@
     </row>
     <row r="44" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="67"/>
-      <c r="B44" s="79"/>
+      <c r="B44" s="84"/>
       <c r="C44" s="49" t="s">
         <v>31</v>
       </c>
@@ -5921,7 +5951,7 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="67"/>
-      <c r="B45" s="79"/>
+      <c r="B45" s="84"/>
       <c r="C45" s="45" t="s">
         <v>16</v>
       </c>
@@ -5942,7 +5972,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="67"/>
-      <c r="B46" s="79"/>
+      <c r="B46" s="84"/>
       <c r="C46" s="45" t="s">
         <v>17</v>
       </c>
@@ -5981,7 +6011,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="68"/>
-      <c r="B47" s="80"/>
+      <c r="B47" s="85"/>
       <c r="C47" s="46" t="s">
         <v>18</v>
       </c>
@@ -6109,6 +6139,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="A6:A17"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B17"/>
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="A28:A39"/>
@@ -6117,14 +6155,6 @@
     <mergeCell ref="A40:A47"/>
     <mergeCell ref="B40:B43"/>
     <mergeCell ref="B44:B47"/>
-    <mergeCell ref="A18:A25"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="A6:A17"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -6142,7 +6172,7 @@
   <dimension ref="A2:S81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V36" sqref="V36"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6306,15 +6336,14 @@
       <c r="A6" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="81">
+      <c r="B6" s="79">
         <v>12</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>36</v>
       </c>
       <c r="D6" s="15">
-        <f>SUM(D7:D9)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E6" s="16">
         <f t="shared" ref="E6:M6" si="0">SUM(E7:E9)</f>
@@ -6330,7 +6359,7 @@
       </c>
       <c r="H6" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I6" s="16">
         <f t="shared" si="0"/>
@@ -6374,12 +6403,12 @@
       </c>
       <c r="S6" s="14">
         <f>SUM(E6:R6)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="67"/>
-      <c r="B7" s="82"/>
+      <c r="B7" s="80"/>
       <c r="C7" s="45" t="s">
         <v>16</v>
       </c>
@@ -6405,7 +6434,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="67"/>
-      <c r="B8" s="82"/>
+      <c r="B8" s="80"/>
       <c r="C8" s="45" t="s">
         <v>17</v>
       </c>
@@ -6431,7 +6460,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="67"/>
-      <c r="B9" s="83"/>
+      <c r="B9" s="81"/>
       <c r="C9" s="46" t="s">
         <v>18</v>
       </c>
@@ -6439,7 +6468,9 @@
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
+      <c r="H9" s="29">
+        <v>1.5</v>
+      </c>
       <c r="I9" s="29"/>
       <c r="J9" s="29"/>
       <c r="K9" s="29"/>
@@ -6452,20 +6483,19 @@
       <c r="R9" s="29"/>
       <c r="S9" s="30">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="67"/>
-      <c r="B10" s="94">
+      <c r="B10" s="89">
         <v>15</v>
       </c>
       <c r="C10" s="47" t="s">
         <v>37</v>
       </c>
       <c r="D10" s="10">
-        <f>SUM(D11:D13)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E10" s="16">
         <f t="shared" ref="E10:M10" si="3">SUM(E11:E13)</f>
@@ -6509,7 +6539,7 @@
       </c>
       <c r="O10" s="16">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="P10" s="16">
         <f t="shared" si="4"/>
@@ -6525,12 +6555,12 @@
       </c>
       <c r="S10" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="67"/>
-      <c r="B11" s="95"/>
+      <c r="B11" s="90"/>
       <c r="C11" s="45" t="s">
         <v>16</v>
       </c>
@@ -6556,7 +6586,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="67"/>
-      <c r="B12" s="95"/>
+      <c r="B12" s="90"/>
       <c r="C12" s="45" t="s">
         <v>17</v>
       </c>
@@ -6582,7 +6612,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="67"/>
-      <c r="B13" s="96"/>
+      <c r="B13" s="91"/>
       <c r="C13" s="46" t="s">
         <v>18</v>
       </c>
@@ -6597,18 +6627,20 @@
       <c r="L13" s="29"/>
       <c r="M13" s="29"/>
       <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
+      <c r="O13" s="29">
+        <v>1.5</v>
+      </c>
       <c r="P13" s="29"/>
       <c r="Q13" s="29"/>
       <c r="R13" s="29"/>
       <c r="S13" s="30">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="67"/>
-      <c r="B14" s="94">
+      <c r="B14" s="89">
         <v>21</v>
       </c>
       <c r="C14" s="60" t="s">
@@ -6681,7 +6713,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="67"/>
-      <c r="B15" s="95"/>
+      <c r="B15" s="90"/>
       <c r="C15" s="45" t="s">
         <v>16</v>
       </c>
@@ -6713,7 +6745,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="67"/>
-      <c r="B16" s="95"/>
+      <c r="B16" s="90"/>
       <c r="C16" s="45" t="s">
         <v>17</v>
       </c>
@@ -6739,7 +6771,7 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="67"/>
-      <c r="B17" s="96"/>
+      <c r="B17" s="91"/>
       <c r="C17" s="46" t="s">
         <v>18</v>
       </c>
@@ -6765,7 +6797,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="67"/>
-      <c r="B18" s="94">
+      <c r="B18" s="89">
         <v>18</v>
       </c>
       <c r="C18" s="60" t="s">
@@ -6838,7 +6870,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="67"/>
-      <c r="B19" s="95"/>
+      <c r="B19" s="90"/>
       <c r="C19" s="45" t="s">
         <v>16</v>
       </c>
@@ -6868,7 +6900,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="67"/>
-      <c r="B20" s="95"/>
+      <c r="B20" s="90"/>
       <c r="C20" s="45" t="s">
         <v>17</v>
       </c>
@@ -6894,7 +6926,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="67"/>
-      <c r="B21" s="96"/>
+      <c r="B21" s="91"/>
       <c r="C21" s="46" t="s">
         <v>18</v>
       </c>
@@ -6920,7 +6952,7 @@
     </row>
     <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="67"/>
-      <c r="B22" s="86" t="s">
+      <c r="B22" s="92" t="s">
         <v>42</v>
       </c>
       <c r="C22" s="60" t="s">
@@ -6993,7 +7025,7 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="67"/>
-      <c r="B23" s="87"/>
+      <c r="B23" s="93"/>
       <c r="C23" s="45" t="s">
         <v>16</v>
       </c>
@@ -7019,7 +7051,7 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="67"/>
-      <c r="B24" s="87"/>
+      <c r="B24" s="93"/>
       <c r="C24" s="45" t="s">
         <v>17</v>
       </c>
@@ -7051,7 +7083,7 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="67"/>
-      <c r="B25" s="88"/>
+      <c r="B25" s="94"/>
       <c r="C25" s="46" t="s">
         <v>18</v>
       </c>
@@ -7077,7 +7109,7 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="67"/>
-      <c r="B26" s="86" t="s">
+      <c r="B26" s="92" t="s">
         <v>45</v>
       </c>
       <c r="C26" s="60" t="s">
@@ -7150,7 +7182,7 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="67"/>
-      <c r="B27" s="87"/>
+      <c r="B27" s="93"/>
       <c r="C27" s="45" t="s">
         <v>16</v>
       </c>
@@ -7176,7 +7208,7 @@
     </row>
     <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="67"/>
-      <c r="B28" s="87"/>
+      <c r="B28" s="93"/>
       <c r="C28" s="45" t="s">
         <v>17</v>
       </c>
@@ -7206,7 +7238,7 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="67"/>
-      <c r="B29" s="88"/>
+      <c r="B29" s="94"/>
       <c r="C29" s="46" t="s">
         <v>18</v>
       </c>
@@ -7232,7 +7264,7 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="67"/>
-      <c r="B30" s="86">
+      <c r="B30" s="92">
         <v>31</v>
       </c>
       <c r="C30" s="60" t="s">
@@ -7305,7 +7337,7 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="67"/>
-      <c r="B31" s="87"/>
+      <c r="B31" s="93"/>
       <c r="C31" s="45" t="s">
         <v>16</v>
       </c>
@@ -7331,7 +7363,7 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="67"/>
-      <c r="B32" s="87"/>
+      <c r="B32" s="93"/>
       <c r="C32" s="45" t="s">
         <v>17</v>
       </c>
@@ -7361,7 +7393,7 @@
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="68"/>
-      <c r="B33" s="88"/>
+      <c r="B33" s="94"/>
       <c r="C33" s="46" t="s">
         <v>18</v>
       </c>
@@ -7542,7 +7574,7 @@
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="67"/>
-      <c r="B38" s="91"/>
+      <c r="B38" s="86"/>
       <c r="C38" s="10" t="s">
         <v>40</v>
       </c>
@@ -7613,7 +7645,7 @@
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="67"/>
-      <c r="B39" s="92"/>
+      <c r="B39" s="87"/>
       <c r="C39" s="45" t="s">
         <v>16</v>
       </c>
@@ -7639,7 +7671,7 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="67"/>
-      <c r="B40" s="92"/>
+      <c r="B40" s="87"/>
       <c r="C40" s="45" t="s">
         <v>17</v>
       </c>
@@ -7669,7 +7701,7 @@
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="68"/>
-      <c r="B41" s="93"/>
+      <c r="B41" s="88"/>
       <c r="C41" s="46" t="s">
         <v>18</v>
       </c>
@@ -7694,13 +7726,13 @@
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B42" s="90" t="s">
+      <c r="B42" s="96" t="s">
         <v>26</v>
       </c>
-      <c r="C42" s="90"/>
+      <c r="C42" s="96"/>
       <c r="D42" s="2">
         <f>SUM(D6,D10,D14,D34,D38)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E42" s="2">
         <f t="shared" ref="E42:R42" si="21">SUM(E6,E10,E14,E34,E38,E18,E22,E26,E30)</f>
@@ -7716,7 +7748,7 @@
       </c>
       <c r="H42" s="2">
         <f t="shared" si="21"/>
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="I42" s="2">
         <f t="shared" si="21"/>
@@ -7744,7 +7776,7 @@
       </c>
       <c r="O42" s="2">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="P42" s="2">
         <f t="shared" si="21"/>
@@ -7760,14 +7792,14 @@
       </c>
       <c r="S42" s="23">
         <f>SUM(E42:R42)</f>
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="B44" s="81">
+      <c r="B44" s="79">
         <v>12</v>
       </c>
       <c r="C44" s="10" t="s">
@@ -7836,7 +7868,7 @@
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="67"/>
-      <c r="B45" s="82"/>
+      <c r="B45" s="80"/>
       <c r="C45" s="45" t="s">
         <v>16</v>
       </c>
@@ -7861,7 +7893,7 @@
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="67"/>
-      <c r="B46" s="82"/>
+      <c r="B46" s="80"/>
       <c r="C46" s="45" t="s">
         <v>17</v>
       </c>
@@ -7886,7 +7918,7 @@
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="67"/>
-      <c r="B47" s="83"/>
+      <c r="B47" s="81"/>
       <c r="C47" s="46" t="s">
         <v>18</v>
       </c>
@@ -7911,7 +7943,7 @@
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="67"/>
-      <c r="B48" s="94">
+      <c r="B48" s="89">
         <v>15</v>
       </c>
       <c r="C48" s="47" t="s">
@@ -7980,7 +8012,7 @@
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="67"/>
-      <c r="B49" s="95"/>
+      <c r="B49" s="90"/>
       <c r="C49" s="45" t="s">
         <v>16</v>
       </c>
@@ -8005,7 +8037,7 @@
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="67"/>
-      <c r="B50" s="95"/>
+      <c r="B50" s="90"/>
       <c r="C50" s="45" t="s">
         <v>17</v>
       </c>
@@ -8030,7 +8062,7 @@
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="67"/>
-      <c r="B51" s="96"/>
+      <c r="B51" s="91"/>
       <c r="C51" s="46" t="s">
         <v>18</v>
       </c>
@@ -8055,7 +8087,7 @@
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="67"/>
-      <c r="B52" s="94">
+      <c r="B52" s="89">
         <v>21</v>
       </c>
       <c r="C52" s="60" t="s">
@@ -8124,7 +8156,7 @@
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="67"/>
-      <c r="B53" s="95"/>
+      <c r="B53" s="90"/>
       <c r="C53" s="45" t="s">
         <v>16</v>
       </c>
@@ -8149,7 +8181,7 @@
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="67"/>
-      <c r="B54" s="95"/>
+      <c r="B54" s="90"/>
       <c r="C54" s="45" t="s">
         <v>17</v>
       </c>
@@ -8174,7 +8206,7 @@
     </row>
     <row r="55" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="67"/>
-      <c r="B55" s="96"/>
+      <c r="B55" s="91"/>
       <c r="C55" s="46" t="s">
         <v>18</v>
       </c>
@@ -8199,7 +8231,7 @@
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="67"/>
-      <c r="B56" s="94">
+      <c r="B56" s="89">
         <v>18</v>
       </c>
       <c r="C56" s="60" t="s">
@@ -8268,7 +8300,7 @@
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="67"/>
-      <c r="B57" s="95"/>
+      <c r="B57" s="90"/>
       <c r="C57" s="45" t="s">
         <v>16</v>
       </c>
@@ -8293,7 +8325,7 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="67"/>
-      <c r="B58" s="95"/>
+      <c r="B58" s="90"/>
       <c r="C58" s="45" t="s">
         <v>17</v>
       </c>
@@ -8318,7 +8350,7 @@
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="67"/>
-      <c r="B59" s="96"/>
+      <c r="B59" s="91"/>
       <c r="C59" s="46" t="s">
         <v>18</v>
       </c>
@@ -8343,7 +8375,7 @@
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="67"/>
-      <c r="B60" s="86" t="s">
+      <c r="B60" s="92" t="s">
         <v>42</v>
       </c>
       <c r="C60" s="60" t="s">
@@ -8412,7 +8444,7 @@
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="67"/>
-      <c r="B61" s="87"/>
+      <c r="B61" s="93"/>
       <c r="C61" s="45" t="s">
         <v>16</v>
       </c>
@@ -8437,7 +8469,7 @@
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="67"/>
-      <c r="B62" s="87"/>
+      <c r="B62" s="93"/>
       <c r="C62" s="45" t="s">
         <v>17</v>
       </c>
@@ -8461,7 +8493,7 @@
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="67"/>
-      <c r="B63" s="88"/>
+      <c r="B63" s="94"/>
       <c r="C63" s="46" t="s">
         <v>18</v>
       </c>
@@ -8486,7 +8518,7 @@
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="67"/>
-      <c r="B64" s="86" t="s">
+      <c r="B64" s="92" t="s">
         <v>45</v>
       </c>
       <c r="C64" s="60" t="s">
@@ -8555,7 +8587,7 @@
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="67"/>
-      <c r="B65" s="87"/>
+      <c r="B65" s="93"/>
       <c r="C65" s="45" t="s">
         <v>16</v>
       </c>
@@ -8580,7 +8612,7 @@
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="67"/>
-      <c r="B66" s="87"/>
+      <c r="B66" s="93"/>
       <c r="C66" s="45" t="s">
         <v>17</v>
       </c>
@@ -8604,7 +8636,7 @@
     </row>
     <row r="67" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="67"/>
-      <c r="B67" s="88"/>
+      <c r="B67" s="94"/>
       <c r="C67" s="46" t="s">
         <v>18</v>
       </c>
@@ -8629,7 +8661,7 @@
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="67"/>
-      <c r="B68" s="86">
+      <c r="B68" s="92">
         <v>31</v>
       </c>
       <c r="C68" s="60" t="s">
@@ -8698,7 +8730,7 @@
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="67"/>
-      <c r="B69" s="87"/>
+      <c r="B69" s="93"/>
       <c r="C69" s="45" t="s">
         <v>16</v>
       </c>
@@ -8723,7 +8755,7 @@
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="67"/>
-      <c r="B70" s="87"/>
+      <c r="B70" s="93"/>
       <c r="C70" s="45" t="s">
         <v>17</v>
       </c>
@@ -8747,7 +8779,7 @@
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="68"/>
-      <c r="B71" s="88"/>
+      <c r="B71" s="94"/>
       <c r="C71" s="46" t="s">
         <v>18</v>
       </c>
@@ -8774,7 +8806,7 @@
       <c r="A72" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="B72" s="81"/>
+      <c r="B72" s="79"/>
       <c r="C72" s="10" t="s">
         <v>39</v>
       </c>
@@ -8841,7 +8873,7 @@
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="67"/>
-      <c r="B73" s="82"/>
+      <c r="B73" s="80"/>
       <c r="C73" s="45" t="s">
         <v>16</v>
       </c>
@@ -8866,7 +8898,7 @@
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="67"/>
-      <c r="B74" s="82"/>
+      <c r="B74" s="80"/>
       <c r="C74" s="45" t="s">
         <v>17</v>
       </c>
@@ -8890,7 +8922,7 @@
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="67"/>
-      <c r="B75" s="83"/>
+      <c r="B75" s="81"/>
       <c r="C75" s="45" t="s">
         <v>18</v>
       </c>
@@ -8915,7 +8947,7 @@
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="67"/>
-      <c r="B76" s="91"/>
+      <c r="B76" s="86"/>
       <c r="C76" s="10" t="s">
         <v>40</v>
       </c>
@@ -8982,7 +9014,7 @@
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="67"/>
-      <c r="B77" s="92"/>
+      <c r="B77" s="87"/>
       <c r="C77" s="45" t="s">
         <v>16</v>
       </c>
@@ -9007,7 +9039,7 @@
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="67"/>
-      <c r="B78" s="92"/>
+      <c r="B78" s="87"/>
       <c r="C78" s="45" t="s">
         <v>17</v>
       </c>
@@ -9031,7 +9063,7 @@
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" s="68"/>
-      <c r="B79" s="93"/>
+      <c r="B79" s="88"/>
       <c r="C79" s="46" t="s">
         <v>18</v>
       </c>
@@ -9055,10 +9087,10 @@
       <c r="R79" s="39"/>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B80" s="89" t="s">
+      <c r="B80" s="95" t="s">
         <v>26</v>
       </c>
-      <c r="C80" s="89"/>
+      <c r="C80" s="95"/>
       <c r="D80" s="2">
         <f t="shared" ref="D80:M80" si="49">SUM(D44,D64,D68,D72,D76)</f>
         <v>0</v>
@@ -9184,6 +9216,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="E2:K2"/>
+    <mergeCell ref="L2:R2"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="B68:B71"/>
     <mergeCell ref="A72:A79"/>
     <mergeCell ref="B34:B37"/>
     <mergeCell ref="B38:B41"/>
@@ -9200,16 +9242,6 @@
     <mergeCell ref="B48:B51"/>
     <mergeCell ref="B52:B55"/>
     <mergeCell ref="B64:B67"/>
-    <mergeCell ref="E2:K2"/>
-    <mergeCell ref="L2:R2"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="B68:B71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
product and sprint 3 tab updated
</commit_message>
<xml_diff>
--- a/Management/Burndown.xlsx
+++ b/Management/Burndown.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-15" windowWidth="25605" windowHeight="14520" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="-15" windowWidth="25605" windowHeight="14520"/>
   </bookViews>
   <sheets>
     <sheet name="Product Burndown" sheetId="1" r:id="rId1"/>
@@ -646,12 +646,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -667,20 +661,11 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -699,6 +684,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -923,10 +923,13 @@
                   <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>135</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>125</c:v>
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -943,11 +946,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="37699968"/>
-        <c:axId val="37701504"/>
+        <c:axId val="37503360"/>
+        <c:axId val="37504896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="37699968"/>
+        <c:axId val="37503360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -956,7 +959,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37701504"/>
+        <c:crossAx val="37504896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -964,7 +967,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="37701504"/>
+        <c:axId val="37504896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -975,13 +978,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37699968"/>
+        <c:crossAx val="37503360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1234,11 +1238,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="37735040"/>
-        <c:axId val="38805888"/>
+        <c:axId val="37534336"/>
+        <c:axId val="37548416"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="37735040"/>
+        <c:axId val="37534336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1248,14 +1252,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38805888"/>
+        <c:crossAx val="37548416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="38805888"/>
+        <c:axId val="37548416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1266,7 +1270,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37735040"/>
+        <c:crossAx val="37534336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1489,11 +1493,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="103560320"/>
-        <c:axId val="103561856"/>
+        <c:axId val="150946944"/>
+        <c:axId val="150948480"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="103560320"/>
+        <c:axId val="150946944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1503,14 +1507,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103561856"/>
+        <c:crossAx val="150948480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="103561856"/>
+        <c:axId val="150948480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1521,13 +1525,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103560320"/>
+        <c:crossAx val="150946944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1629,49 +1634,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1745,49 +1750,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>15.555555555555555</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>13.611111111111111</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>11.666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>9.7222222222222214</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>7.7777777777777768</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>5.8333333333333321</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>3.8888888888888875</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1.9444444444444431</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>-1.9444444444444444</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>-3.8888888888888888</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>-5.833333333333333</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>-7.7777777777777777</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>-9.7222222222222214</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1804,11 +1809,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="103605760"/>
-        <c:axId val="103607296"/>
+        <c:axId val="150986112"/>
+        <c:axId val="168952960"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="103605760"/>
+        <c:axId val="150986112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1818,14 +1823,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103607296"/>
+        <c:crossAx val="168952960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="103607296"/>
+        <c:axId val="168952960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1836,7 +1841,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103605760"/>
+        <c:crossAx val="150986112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2291,8 +2296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2379,8 +2384,8 @@
         <v>131</v>
       </c>
       <c r="D4" s="4">
-        <f>H3-E4</f>
-        <v>124</v>
+        <f t="shared" ref="D4:D5" si="0">H3-F4</f>
+        <v>127</v>
       </c>
       <c r="E4" s="4">
         <v>19</v>
@@ -2392,7 +2397,8 @@
         <v>0</v>
       </c>
       <c r="H4" s="4">
-        <v>135</v>
+        <f t="shared" ref="H4:H5" si="1">H3-E4+G3</f>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2403,12 +2409,12 @@
         <v>12</v>
       </c>
       <c r="C5" s="4">
-        <f t="shared" ref="C5:C15" si="0" xml:space="preserve"> C4 - B5</f>
+        <f t="shared" ref="C5:C15" si="2" xml:space="preserve"> C4 - B5</f>
         <v>119</v>
       </c>
       <c r="D5" s="4">
-        <f>H4-E5</f>
-        <v>121</v>
+        <f t="shared" si="0"/>
+        <v>92</v>
       </c>
       <c r="E5" s="4">
         <v>14</v>
@@ -2420,26 +2426,38 @@
         <v>23</v>
       </c>
       <c r="H5" s="4">
-        <v>125</v>
+        <f t="shared" si="1"/>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="4">
         <v>12</v>
       </c>
-      <c r="C6" s="3">
-        <f t="shared" si="0"/>
+      <c r="C6" s="4">
+        <f t="shared" si="2"/>
         <v>107</v>
       </c>
-      <c r="D6" s="3">
-        <f>H5-E6</f>
-        <v>125</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="D6" s="4">
+        <f>H5-F6</f>
+        <v>70</v>
+      </c>
+      <c r="E6" s="4">
+        <v>34</v>
+      </c>
+      <c r="F6" s="4">
+        <v>40</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <f>H5-E6+G5</f>
+        <v>99</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -2449,7 +2467,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>95</v>
       </c>
       <c r="D7" s="2"/>
@@ -2464,7 +2482,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>83</v>
       </c>
       <c r="D8" s="2"/>
@@ -2479,7 +2497,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>71</v>
       </c>
       <c r="D9" s="2"/>
@@ -2494,7 +2512,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>59</v>
       </c>
       <c r="D10" s="2"/>
@@ -2509,7 +2527,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>47</v>
       </c>
       <c r="D11" s="2"/>
@@ -2524,7 +2542,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="D12" s="2"/>
@@ -2539,7 +2557,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="D13" s="2"/>
@@ -2554,7 +2572,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="D14" s="2"/>
@@ -2569,7 +2587,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D15" s="2"/>
@@ -2621,8 +2639,8 @@
     <mergeCell ref="B1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4643,7 +4661,7 @@
       <c r="A6" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="81">
+      <c r="B6" s="79">
         <v>1</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -4696,7 +4714,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="67"/>
-      <c r="B7" s="82"/>
+      <c r="B7" s="80"/>
       <c r="C7" s="45" t="s">
         <v>16</v>
       </c>
@@ -4717,7 +4735,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="67"/>
-      <c r="B8" s="82"/>
+      <c r="B8" s="80"/>
       <c r="C8" s="45" t="s">
         <v>17</v>
       </c>
@@ -4740,7 +4758,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="67"/>
-      <c r="B9" s="83"/>
+      <c r="B9" s="81"/>
       <c r="C9" s="46" t="s">
         <v>18</v>
       </c>
@@ -4761,7 +4779,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="67"/>
-      <c r="B10" s="84" t="s">
+      <c r="B10" s="82" t="s">
         <v>35</v>
       </c>
       <c r="C10" s="47" t="s">
@@ -4814,7 +4832,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="67"/>
-      <c r="B11" s="85"/>
+      <c r="B11" s="83"/>
       <c r="C11" s="45" t="s">
         <v>16</v>
       </c>
@@ -4835,7 +4853,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="67"/>
-      <c r="B12" s="85"/>
+      <c r="B12" s="83"/>
       <c r="C12" s="45" t="s">
         <v>17</v>
       </c>
@@ -4856,7 +4874,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="67"/>
-      <c r="B13" s="85"/>
+      <c r="B13" s="83"/>
       <c r="C13" s="46" t="s">
         <v>18</v>
       </c>
@@ -4879,7 +4897,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="67"/>
-      <c r="B14" s="85"/>
+      <c r="B14" s="83"/>
       <c r="C14" s="52" t="s">
         <v>33</v>
       </c>
@@ -4930,7 +4948,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="67"/>
-      <c r="B15" s="85"/>
+      <c r="B15" s="83"/>
       <c r="C15" s="45" t="s">
         <v>16</v>
       </c>
@@ -4957,7 +4975,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="67"/>
-      <c r="B16" s="85"/>
+      <c r="B16" s="83"/>
       <c r="C16" s="45" t="s">
         <v>17</v>
       </c>
@@ -4980,7 +4998,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="67"/>
-      <c r="B17" s="85"/>
+      <c r="B17" s="83"/>
       <c r="C17" s="45" t="s">
         <v>18</v>
       </c>
@@ -5123,7 +5141,7 @@
     </row>
     <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="67"/>
-      <c r="B22" s="79"/>
+      <c r="B22" s="84"/>
       <c r="C22" s="49" t="s">
         <v>31</v>
       </c>
@@ -5174,7 +5192,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="67"/>
-      <c r="B23" s="79"/>
+      <c r="B23" s="84"/>
       <c r="C23" s="45" t="s">
         <v>16</v>
       </c>
@@ -5195,7 +5213,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="67"/>
-      <c r="B24" s="79"/>
+      <c r="B24" s="84"/>
       <c r="C24" s="45" t="s">
         <v>17</v>
       </c>
@@ -5216,7 +5234,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="68"/>
-      <c r="B25" s="80"/>
+      <c r="B25" s="85"/>
       <c r="C25" s="46" t="s">
         <v>18</v>
       </c>
@@ -5297,7 +5315,7 @@
       <c r="A28" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="81">
+      <c r="B28" s="79">
         <v>1</v>
       </c>
       <c r="C28" s="10" t="s">
@@ -5347,7 +5365,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="67"/>
-      <c r="B29" s="82"/>
+      <c r="B29" s="80"/>
       <c r="C29" s="45" t="s">
         <v>16</v>
       </c>
@@ -5368,7 +5386,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="67"/>
-      <c r="B30" s="82"/>
+      <c r="B30" s="80"/>
       <c r="C30" s="45" t="s">
         <v>17</v>
       </c>
@@ -5407,7 +5425,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="67"/>
-      <c r="B31" s="83"/>
+      <c r="B31" s="81"/>
       <c r="C31" s="46" t="s">
         <v>18</v>
       </c>
@@ -5428,7 +5446,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="67"/>
-      <c r="B32" s="84" t="s">
+      <c r="B32" s="82" t="s">
         <v>35</v>
       </c>
       <c r="C32" s="47" t="s">
@@ -5478,7 +5496,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="67"/>
-      <c r="B33" s="85"/>
+      <c r="B33" s="83"/>
       <c r="C33" s="45" t="s">
         <v>16</v>
       </c>
@@ -5517,7 +5535,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="67"/>
-      <c r="B34" s="85"/>
+      <c r="B34" s="83"/>
       <c r="C34" s="45" t="s">
         <v>17</v>
       </c>
@@ -5538,7 +5556,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="67"/>
-      <c r="B35" s="85"/>
+      <c r="B35" s="83"/>
       <c r="C35" s="46" t="s">
         <v>18</v>
       </c>
@@ -5577,7 +5595,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="67"/>
-      <c r="B36" s="85"/>
+      <c r="B36" s="83"/>
       <c r="C36" s="52" t="s">
         <v>33</v>
       </c>
@@ -5625,7 +5643,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="67"/>
-      <c r="B37" s="85"/>
+      <c r="B37" s="83"/>
       <c r="C37" s="45" t="s">
         <v>16</v>
       </c>
@@ -5664,7 +5682,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="67"/>
-      <c r="B38" s="85"/>
+      <c r="B38" s="83"/>
       <c r="C38" s="45" t="s">
         <v>17</v>
       </c>
@@ -5703,7 +5721,7 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="67"/>
-      <c r="B39" s="85"/>
+      <c r="B39" s="83"/>
       <c r="C39" s="45" t="s">
         <v>18</v>
       </c>
@@ -5873,7 +5891,7 @@
     </row>
     <row r="44" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="67"/>
-      <c r="B44" s="79"/>
+      <c r="B44" s="84"/>
       <c r="C44" s="49" t="s">
         <v>31</v>
       </c>
@@ -5921,7 +5939,7 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="67"/>
-      <c r="B45" s="79"/>
+      <c r="B45" s="84"/>
       <c r="C45" s="45" t="s">
         <v>16</v>
       </c>
@@ -5942,7 +5960,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="67"/>
-      <c r="B46" s="79"/>
+      <c r="B46" s="84"/>
       <c r="C46" s="45" t="s">
         <v>17</v>
       </c>
@@ -5981,7 +5999,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="68"/>
-      <c r="B47" s="80"/>
+      <c r="B47" s="85"/>
       <c r="C47" s="46" t="s">
         <v>18</v>
       </c>
@@ -6109,6 +6127,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="A6:A17"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B17"/>
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="A28:A39"/>
@@ -6117,14 +6143,6 @@
     <mergeCell ref="A40:A47"/>
     <mergeCell ref="B40:B43"/>
     <mergeCell ref="B44:B47"/>
-    <mergeCell ref="A18:A25"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="A6:A17"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -6141,8 +6159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V36" sqref="V36"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="O78" sqref="O78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6306,7 +6324,7 @@
       <c r="A6" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="81">
+      <c r="B6" s="79">
         <v>12</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -6314,7 +6332,7 @@
       </c>
       <c r="D6" s="15">
         <f>SUM(D7:D9)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E6" s="16">
         <f t="shared" ref="E6:M6" si="0">SUM(E7:E9)</f>
@@ -6330,7 +6348,7 @@
       </c>
       <c r="H6" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I6" s="16">
         <f t="shared" si="0"/>
@@ -6374,12 +6392,12 @@
       </c>
       <c r="S6" s="14">
         <f>SUM(E6:R6)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="67"/>
-      <c r="B7" s="82"/>
+      <c r="B7" s="80"/>
       <c r="C7" s="45" t="s">
         <v>16</v>
       </c>
@@ -6405,7 +6423,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="67"/>
-      <c r="B8" s="82"/>
+      <c r="B8" s="80"/>
       <c r="C8" s="45" t="s">
         <v>17</v>
       </c>
@@ -6431,15 +6449,19 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="67"/>
-      <c r="B9" s="83"/>
+      <c r="B9" s="81"/>
       <c r="C9" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="26"/>
+      <c r="D9" s="26">
+        <v>1.5</v>
+      </c>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
+      <c r="H9" s="29">
+        <v>1.5</v>
+      </c>
       <c r="I9" s="29"/>
       <c r="J9" s="29"/>
       <c r="K9" s="29"/>
@@ -6452,12 +6474,12 @@
       <c r="R9" s="29"/>
       <c r="S9" s="30">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="67"/>
-      <c r="B10" s="94">
+      <c r="B10" s="89">
         <v>15</v>
       </c>
       <c r="C10" s="47" t="s">
@@ -6465,7 +6487,7 @@
       </c>
       <c r="D10" s="10">
         <f>SUM(D11:D13)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E10" s="16">
         <f t="shared" ref="E10:M10" si="3">SUM(E11:E13)</f>
@@ -6509,7 +6531,7 @@
       </c>
       <c r="O10" s="16">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="P10" s="16">
         <f t="shared" si="4"/>
@@ -6525,12 +6547,12 @@
       </c>
       <c r="S10" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="67"/>
-      <c r="B11" s="95"/>
+      <c r="B11" s="90"/>
       <c r="C11" s="45" t="s">
         <v>16</v>
       </c>
@@ -6556,7 +6578,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="67"/>
-      <c r="B12" s="95"/>
+      <c r="B12" s="90"/>
       <c r="C12" s="45" t="s">
         <v>17</v>
       </c>
@@ -6582,11 +6604,13 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="67"/>
-      <c r="B13" s="96"/>
+      <c r="B13" s="91"/>
       <c r="C13" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="26"/>
+      <c r="D13" s="26">
+        <v>1.5</v>
+      </c>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
       <c r="G13" s="29"/>
@@ -6597,18 +6621,20 @@
       <c r="L13" s="29"/>
       <c r="M13" s="29"/>
       <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
+      <c r="O13" s="29">
+        <v>1.5</v>
+      </c>
       <c r="P13" s="29"/>
       <c r="Q13" s="29"/>
       <c r="R13" s="29"/>
       <c r="S13" s="30">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="67"/>
-      <c r="B14" s="94">
+      <c r="B14" s="89">
         <v>21</v>
       </c>
       <c r="C14" s="60" t="s">
@@ -6681,7 +6707,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="67"/>
-      <c r="B15" s="95"/>
+      <c r="B15" s="90"/>
       <c r="C15" s="45" t="s">
         <v>16</v>
       </c>
@@ -6713,7 +6739,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="67"/>
-      <c r="B16" s="95"/>
+      <c r="B16" s="90"/>
       <c r="C16" s="45" t="s">
         <v>17</v>
       </c>
@@ -6739,7 +6765,7 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="67"/>
-      <c r="B17" s="96"/>
+      <c r="B17" s="91"/>
       <c r="C17" s="46" t="s">
         <v>18</v>
       </c>
@@ -6765,7 +6791,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="67"/>
-      <c r="B18" s="94">
+      <c r="B18" s="89">
         <v>18</v>
       </c>
       <c r="C18" s="60" t="s">
@@ -6838,7 +6864,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="67"/>
-      <c r="B19" s="95"/>
+      <c r="B19" s="90"/>
       <c r="C19" s="45" t="s">
         <v>16</v>
       </c>
@@ -6868,7 +6894,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="67"/>
-      <c r="B20" s="95"/>
+      <c r="B20" s="90"/>
       <c r="C20" s="45" t="s">
         <v>17</v>
       </c>
@@ -6894,7 +6920,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="67"/>
-      <c r="B21" s="96"/>
+      <c r="B21" s="91"/>
       <c r="C21" s="46" t="s">
         <v>18</v>
       </c>
@@ -6920,7 +6946,7 @@
     </row>
     <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="67"/>
-      <c r="B22" s="86" t="s">
+      <c r="B22" s="92" t="s">
         <v>42</v>
       </c>
       <c r="C22" s="60" t="s">
@@ -6993,7 +7019,7 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="67"/>
-      <c r="B23" s="87"/>
+      <c r="B23" s="93"/>
       <c r="C23" s="45" t="s">
         <v>16</v>
       </c>
@@ -7019,7 +7045,7 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="67"/>
-      <c r="B24" s="87"/>
+      <c r="B24" s="93"/>
       <c r="C24" s="45" t="s">
         <v>17</v>
       </c>
@@ -7051,7 +7077,7 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="67"/>
-      <c r="B25" s="88"/>
+      <c r="B25" s="94"/>
       <c r="C25" s="46" t="s">
         <v>18</v>
       </c>
@@ -7077,7 +7103,7 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="67"/>
-      <c r="B26" s="86" t="s">
+      <c r="B26" s="92" t="s">
         <v>45</v>
       </c>
       <c r="C26" s="60" t="s">
@@ -7150,7 +7176,7 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="67"/>
-      <c r="B27" s="87"/>
+      <c r="B27" s="93"/>
       <c r="C27" s="45" t="s">
         <v>16</v>
       </c>
@@ -7176,7 +7202,7 @@
     </row>
     <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="67"/>
-      <c r="B28" s="87"/>
+      <c r="B28" s="93"/>
       <c r="C28" s="45" t="s">
         <v>17</v>
       </c>
@@ -7206,7 +7232,7 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="67"/>
-      <c r="B29" s="88"/>
+      <c r="B29" s="94"/>
       <c r="C29" s="46" t="s">
         <v>18</v>
       </c>
@@ -7232,7 +7258,7 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="67"/>
-      <c r="B30" s="86">
+      <c r="B30" s="92">
         <v>31</v>
       </c>
       <c r="C30" s="60" t="s">
@@ -7305,7 +7331,7 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="67"/>
-      <c r="B31" s="87"/>
+      <c r="B31" s="93"/>
       <c r="C31" s="45" t="s">
         <v>16</v>
       </c>
@@ -7331,7 +7357,7 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="67"/>
-      <c r="B32" s="87"/>
+      <c r="B32" s="93"/>
       <c r="C32" s="45" t="s">
         <v>17</v>
       </c>
@@ -7361,7 +7387,7 @@
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="68"/>
-      <c r="B33" s="88"/>
+      <c r="B33" s="94"/>
       <c r="C33" s="46" t="s">
         <v>18</v>
       </c>
@@ -7542,7 +7568,7 @@
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="67"/>
-      <c r="B38" s="91"/>
+      <c r="B38" s="86"/>
       <c r="C38" s="10" t="s">
         <v>40</v>
       </c>
@@ -7613,7 +7639,7 @@
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="67"/>
-      <c r="B39" s="92"/>
+      <c r="B39" s="87"/>
       <c r="C39" s="45" t="s">
         <v>16</v>
       </c>
@@ -7639,7 +7665,7 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="67"/>
-      <c r="B40" s="92"/>
+      <c r="B40" s="87"/>
       <c r="C40" s="45" t="s">
         <v>17</v>
       </c>
@@ -7669,7 +7695,7 @@
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="68"/>
-      <c r="B41" s="93"/>
+      <c r="B41" s="88"/>
       <c r="C41" s="46" t="s">
         <v>18</v>
       </c>
@@ -7694,13 +7720,13 @@
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B42" s="90" t="s">
+      <c r="B42" s="96" t="s">
         <v>26</v>
       </c>
-      <c r="C42" s="90"/>
+      <c r="C42" s="96"/>
       <c r="D42" s="2">
         <f>SUM(D6,D10,D14,D34,D38)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E42" s="2">
         <f t="shared" ref="E42:R42" si="21">SUM(E6,E10,E14,E34,E38,E18,E22,E26,E30)</f>
@@ -7716,7 +7742,7 @@
       </c>
       <c r="H42" s="2">
         <f t="shared" si="21"/>
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="I42" s="2">
         <f t="shared" si="21"/>
@@ -7744,7 +7770,7 @@
       </c>
       <c r="O42" s="2">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="P42" s="2">
         <f t="shared" si="21"/>
@@ -7760,14 +7786,14 @@
       </c>
       <c r="S42" s="23">
         <f>SUM(E42:R42)</f>
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="B44" s="81">
+      <c r="B44" s="79">
         <v>12</v>
       </c>
       <c r="C44" s="10" t="s">
@@ -7775,68 +7801,68 @@
       </c>
       <c r="D44" s="15">
         <f>SUM(D45:D47)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E44" s="16">
         <f t="shared" ref="E44:M44" si="22">SUM(E45:E47)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="F44" s="16">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="G44" s="16">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="H44" s="16">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I44" s="16">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J44" s="16">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K44" s="16">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L44" s="16">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M44" s="16">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="N44" s="16">
         <f t="shared" ref="N44:R44" si="23">SUM(N45:N47)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O44" s="16">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P44" s="16">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Q44" s="16">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R44" s="35">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="67"/>
-      <c r="B45" s="82"/>
+      <c r="B45" s="80"/>
       <c r="C45" s="45" t="s">
         <v>16</v>
       </c>
@@ -7861,7 +7887,7 @@
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="67"/>
-      <c r="B46" s="82"/>
+      <c r="B46" s="80"/>
       <c r="C46" s="45" t="s">
         <v>17</v>
       </c>
@@ -7886,32 +7912,60 @@
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="67"/>
-      <c r="B47" s="83"/>
+      <c r="B47" s="81"/>
       <c r="C47" s="46" t="s">
         <v>18</v>
       </c>
       <c r="D47" s="24">
         <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="E47" s="31"/>
-      <c r="F47" s="31"/>
-      <c r="G47" s="31"/>
-      <c r="H47" s="31"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
-      <c r="K47" s="31"/>
-      <c r="L47" s="31"/>
-      <c r="M47" s="31"/>
-      <c r="N47" s="31"/>
-      <c r="O47" s="31"/>
-      <c r="P47" s="31"/>
-      <c r="Q47" s="31"/>
-      <c r="R47" s="36"/>
+        <v>1.5</v>
+      </c>
+      <c r="E47" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="F47" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="G47" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="H47" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="I47" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="J47" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="K47" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="L47" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="M47" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="N47" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="O47" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="P47" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="Q47" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="R47" s="31">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="67"/>
-      <c r="B48" s="94">
+      <c r="B48" s="89">
         <v>15</v>
       </c>
       <c r="C48" s="47" t="s">
@@ -7919,68 +7973,68 @@
       </c>
       <c r="D48" s="10">
         <f>SUM(D49:D51)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E48" s="16">
         <f t="shared" ref="E48:M48" si="25">SUM(E49:E51)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="F48" s="16">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="G48" s="16">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="H48" s="16">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I48" s="16">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="J48" s="16">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="K48" s="16">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="L48" s="16">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="M48" s="16">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="N48" s="16">
         <f t="shared" ref="N48:R48" si="26">SUM(N49:N51)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="O48" s="16">
         <f t="shared" si="26"/>
-        <v>0</v>
+        <v>-3.25</v>
       </c>
       <c r="P48" s="16">
         <f t="shared" si="26"/>
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="Q48" s="16">
         <f t="shared" si="26"/>
-        <v>0</v>
+        <v>-6.5</v>
       </c>
       <c r="R48" s="35">
         <f t="shared" si="26"/>
-        <v>0</v>
+        <v>-6.5</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="67"/>
-      <c r="B49" s="95"/>
+      <c r="B49" s="90"/>
       <c r="C49" s="45" t="s">
         <v>16</v>
       </c>
@@ -8005,7 +8059,7 @@
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="67"/>
-      <c r="B50" s="95"/>
+      <c r="B50" s="90"/>
       <c r="C50" s="45" t="s">
         <v>17</v>
       </c>
@@ -8030,32 +8084,63 @@
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="67"/>
-      <c r="B51" s="96"/>
+      <c r="B51" s="91"/>
       <c r="C51" s="46" t="s">
         <v>18</v>
       </c>
       <c r="D51" s="24">
         <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="E51" s="33"/>
-      <c r="F51" s="33"/>
-      <c r="G51" s="33"/>
-      <c r="H51" s="33"/>
-      <c r="I51" s="33"/>
-      <c r="J51" s="33"/>
-      <c r="K51" s="33"/>
-      <c r="L51" s="33"/>
-      <c r="M51" s="33"/>
-      <c r="N51" s="33"/>
-      <c r="O51" s="33"/>
-      <c r="P51" s="33"/>
-      <c r="Q51" s="33"/>
-      <c r="R51" s="39"/>
+        <v>1.5</v>
+      </c>
+      <c r="E51" s="33">
+        <v>1.5</v>
+      </c>
+      <c r="F51" s="33">
+        <v>1.5</v>
+      </c>
+      <c r="G51" s="33">
+        <v>1.5</v>
+      </c>
+      <c r="H51" s="33">
+        <v>1.5</v>
+      </c>
+      <c r="I51" s="33">
+        <v>1.5</v>
+      </c>
+      <c r="J51" s="33">
+        <v>1.5</v>
+      </c>
+      <c r="K51" s="33">
+        <v>1.5</v>
+      </c>
+      <c r="L51" s="33">
+        <v>1.5</v>
+      </c>
+      <c r="M51" s="33">
+        <v>1.5</v>
+      </c>
+      <c r="N51" s="33">
+        <v>1.5</v>
+      </c>
+      <c r="O51" s="33">
+        <f>1.5-4.75</f>
+        <v>-3.25</v>
+      </c>
+      <c r="P51" s="33">
+        <f>O51-2.75</f>
+        <v>-6</v>
+      </c>
+      <c r="Q51" s="33">
+        <f>P51-0.5</f>
+        <v>-6.5</v>
+      </c>
+      <c r="R51" s="39">
+        <v>-6.5</v>
+      </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="67"/>
-      <c r="B52" s="94">
+      <c r="B52" s="89">
         <v>21</v>
       </c>
       <c r="C52" s="60" t="s">
@@ -8067,31 +8152,31 @@
       </c>
       <c r="E52" s="16">
         <f t="shared" ref="E52:M52" si="28">SUM(E53:E55)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F52" s="16">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G52" s="16">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H52" s="16">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I52" s="16">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J52" s="16">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K52" s="16">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L52" s="16">
         <f t="shared" si="28"/>
@@ -8124,7 +8209,7 @@
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="67"/>
-      <c r="B53" s="95"/>
+      <c r="B53" s="90"/>
       <c r="C53" s="45" t="s">
         <v>16</v>
       </c>
@@ -8132,24 +8217,52 @@
         <f>D15</f>
         <v>4</v>
       </c>
-      <c r="E53" s="31"/>
-      <c r="F53" s="31"/>
-      <c r="G53" s="31"/>
-      <c r="H53" s="31"/>
-      <c r="I53" s="31"/>
-      <c r="J53" s="32"/>
-      <c r="K53" s="32"/>
-      <c r="L53" s="32"/>
-      <c r="M53" s="32"/>
-      <c r="N53" s="32"/>
-      <c r="O53" s="32"/>
-      <c r="P53" s="32"/>
-      <c r="Q53" s="32"/>
-      <c r="R53" s="37"/>
+      <c r="E53" s="31">
+        <v>4</v>
+      </c>
+      <c r="F53" s="31">
+        <v>4</v>
+      </c>
+      <c r="G53" s="31">
+        <v>4</v>
+      </c>
+      <c r="H53" s="31">
+        <v>4</v>
+      </c>
+      <c r="I53" s="31">
+        <v>4</v>
+      </c>
+      <c r="J53" s="31">
+        <v>3</v>
+      </c>
+      <c r="K53" s="31">
+        <v>2</v>
+      </c>
+      <c r="L53" s="32">
+        <v>0</v>
+      </c>
+      <c r="M53" s="32">
+        <v>0</v>
+      </c>
+      <c r="N53" s="32">
+        <v>0</v>
+      </c>
+      <c r="O53" s="32">
+        <v>0</v>
+      </c>
+      <c r="P53" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="32">
+        <v>0</v>
+      </c>
+      <c r="R53" s="32">
+        <v>0</v>
+      </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="67"/>
-      <c r="B54" s="95"/>
+      <c r="B54" s="90"/>
       <c r="C54" s="45" t="s">
         <v>17</v>
       </c>
@@ -8174,7 +8287,7 @@
     </row>
     <row r="55" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="67"/>
-      <c r="B55" s="96"/>
+      <c r="B55" s="91"/>
       <c r="C55" s="46" t="s">
         <v>18</v>
       </c>
@@ -8199,7 +8312,7 @@
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="67"/>
-      <c r="B56" s="94">
+      <c r="B56" s="89">
         <v>18</v>
       </c>
       <c r="C56" s="60" t="s">
@@ -8211,31 +8324,31 @@
       </c>
       <c r="E56" s="16">
         <f t="shared" ref="E56:M56" si="31">SUM(E57:E59)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F56" s="16">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G56" s="16">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H56" s="16">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I56" s="16">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J56" s="16">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K56" s="16">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L56" s="16">
         <f t="shared" si="31"/>
@@ -8243,32 +8356,32 @@
       </c>
       <c r="M56" s="16">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="N56" s="16">
         <f t="shared" ref="N56:R56" si="32">SUM(N57:N59)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="O56" s="16">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P56" s="16">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Q56" s="16">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="R56" s="35">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="67"/>
-      <c r="B57" s="95"/>
+      <c r="B57" s="90"/>
       <c r="C57" s="45" t="s">
         <v>16</v>
       </c>
@@ -8276,24 +8389,52 @@
         <f>D19</f>
         <v>3</v>
       </c>
-      <c r="E57" s="31"/>
-      <c r="F57" s="31"/>
-      <c r="G57" s="31"/>
-      <c r="H57" s="31"/>
-      <c r="I57" s="31"/>
-      <c r="J57" s="31"/>
-      <c r="K57" s="31"/>
-      <c r="L57" s="31"/>
-      <c r="M57" s="31"/>
-      <c r="N57" s="31"/>
-      <c r="O57" s="31"/>
-      <c r="P57" s="31"/>
-      <c r="Q57" s="31"/>
-      <c r="R57" s="36"/>
+      <c r="E57" s="31">
+        <v>3</v>
+      </c>
+      <c r="F57" s="31">
+        <v>3</v>
+      </c>
+      <c r="G57" s="31">
+        <v>3</v>
+      </c>
+      <c r="H57" s="31">
+        <v>3</v>
+      </c>
+      <c r="I57" s="31">
+        <v>3</v>
+      </c>
+      <c r="J57" s="31">
+        <v>3</v>
+      </c>
+      <c r="K57" s="31">
+        <v>2</v>
+      </c>
+      <c r="L57" s="31">
+        <v>0</v>
+      </c>
+      <c r="M57" s="31">
+        <v>-1</v>
+      </c>
+      <c r="N57" s="31">
+        <v>-1</v>
+      </c>
+      <c r="O57" s="31">
+        <v>-1</v>
+      </c>
+      <c r="P57" s="31">
+        <v>-1</v>
+      </c>
+      <c r="Q57" s="31">
+        <v>-1</v>
+      </c>
+      <c r="R57" s="31">
+        <v>-1</v>
+      </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="67"/>
-      <c r="B58" s="95"/>
+      <c r="B58" s="90"/>
       <c r="C58" s="45" t="s">
         <v>17</v>
       </c>
@@ -8318,7 +8459,7 @@
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="67"/>
-      <c r="B59" s="96"/>
+      <c r="B59" s="91"/>
       <c r="C59" s="46" t="s">
         <v>18</v>
       </c>
@@ -8343,7 +8484,7 @@
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="67"/>
-      <c r="B60" s="86" t="s">
+      <c r="B60" s="92" t="s">
         <v>42</v>
       </c>
       <c r="C60" s="60" t="s">
@@ -8351,68 +8492,68 @@
       </c>
       <c r="D60" s="10">
         <f>SUM(D61:D63)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E60" s="21">
         <f t="shared" ref="E60:M60" si="34">SUM(E61:E63)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F60" s="21">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G60" s="21">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H60" s="21">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I60" s="21">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J60" s="21">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K60" s="21">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L60" s="21">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M60" s="21">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N60" s="21">
         <f t="shared" ref="N60:R60" si="35">SUM(N61:N63)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O60" s="21">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P60" s="21">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q60" s="21">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R60" s="13">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="67"/>
-      <c r="B61" s="87"/>
+      <c r="B61" s="93"/>
       <c r="C61" s="45" t="s">
         <v>16</v>
       </c>
@@ -8437,31 +8578,60 @@
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="67"/>
-      <c r="B62" s="87"/>
+      <c r="B62" s="93"/>
       <c r="C62" s="45" t="s">
         <v>17</v>
       </c>
       <c r="D62" s="24">
-        <v>0</v>
-      </c>
-      <c r="E62" s="31"/>
-      <c r="F62" s="31"/>
-      <c r="G62" s="31"/>
-      <c r="H62" s="31"/>
-      <c r="I62" s="31"/>
-      <c r="J62" s="31"/>
-      <c r="K62" s="31"/>
-      <c r="L62" s="31"/>
-      <c r="M62" s="31"/>
-      <c r="N62" s="31"/>
-      <c r="O62" s="31"/>
-      <c r="P62" s="31"/>
-      <c r="Q62" s="31"/>
-      <c r="R62" s="36"/>
+        <f>D24</f>
+        <v>8</v>
+      </c>
+      <c r="E62" s="31">
+        <v>8</v>
+      </c>
+      <c r="F62" s="31">
+        <v>8</v>
+      </c>
+      <c r="G62" s="31">
+        <v>8</v>
+      </c>
+      <c r="H62" s="31">
+        <v>8</v>
+      </c>
+      <c r="I62" s="31">
+        <v>8</v>
+      </c>
+      <c r="J62" s="31">
+        <v>8</v>
+      </c>
+      <c r="K62" s="31">
+        <v>4</v>
+      </c>
+      <c r="L62" s="31">
+        <v>4</v>
+      </c>
+      <c r="M62" s="31">
+        <v>4</v>
+      </c>
+      <c r="N62" s="31">
+        <v>4</v>
+      </c>
+      <c r="O62" s="31">
+        <v>4</v>
+      </c>
+      <c r="P62" s="31">
+        <v>4</v>
+      </c>
+      <c r="Q62" s="31">
+        <v>4</v>
+      </c>
+      <c r="R62" s="36">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="67"/>
-      <c r="B63" s="88"/>
+      <c r="B63" s="94"/>
       <c r="C63" s="46" t="s">
         <v>18</v>
       </c>
@@ -8486,7 +8656,7 @@
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="67"/>
-      <c r="B64" s="86" t="s">
+      <c r="B64" s="92" t="s">
         <v>45</v>
       </c>
       <c r="C64" s="60" t="s">
@@ -8494,68 +8664,68 @@
       </c>
       <c r="D64" s="10">
         <f>SUM(D65:D67)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E64" s="16">
         <f t="shared" ref="E64:M64" si="37">SUM(E65:E67)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F64" s="16">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G64" s="16">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H64" s="16">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I64" s="16">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J64" s="16">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K64" s="16">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L64" s="16">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M64" s="16">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N64" s="16">
         <f t="shared" ref="N64:R64" si="38">SUM(N65:N67)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O64" s="16">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P64" s="16">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q64" s="16">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R64" s="35">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="67"/>
-      <c r="B65" s="87"/>
+      <c r="B65" s="93"/>
       <c r="C65" s="45" t="s">
         <v>16</v>
       </c>
@@ -8580,31 +8750,60 @@
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="67"/>
-      <c r="B66" s="87"/>
+      <c r="B66" s="93"/>
       <c r="C66" s="45" t="s">
         <v>17</v>
       </c>
       <c r="D66" s="24">
-        <v>0</v>
-      </c>
-      <c r="E66" s="31"/>
-      <c r="F66" s="31"/>
-      <c r="G66" s="31"/>
-      <c r="H66" s="31"/>
-      <c r="I66" s="31"/>
-      <c r="J66" s="31"/>
-      <c r="K66" s="31"/>
-      <c r="L66" s="31"/>
-      <c r="M66" s="31"/>
-      <c r="N66" s="31"/>
-      <c r="O66" s="31"/>
-      <c r="P66" s="31"/>
-      <c r="Q66" s="31"/>
-      <c r="R66" s="36"/>
+        <f>D28</f>
+        <v>5</v>
+      </c>
+      <c r="E66" s="31">
+        <v>5</v>
+      </c>
+      <c r="F66" s="31">
+        <v>5</v>
+      </c>
+      <c r="G66" s="31">
+        <v>5</v>
+      </c>
+      <c r="H66" s="31">
+        <v>5</v>
+      </c>
+      <c r="I66" s="31">
+        <v>5</v>
+      </c>
+      <c r="J66" s="31">
+        <v>5</v>
+      </c>
+      <c r="K66" s="31">
+        <v>5</v>
+      </c>
+      <c r="L66" s="31">
+        <v>5</v>
+      </c>
+      <c r="M66" s="31">
+        <v>5</v>
+      </c>
+      <c r="N66" s="31">
+        <v>5</v>
+      </c>
+      <c r="O66" s="31">
+        <v>5</v>
+      </c>
+      <c r="P66" s="31">
+        <v>5</v>
+      </c>
+      <c r="Q66" s="31">
+        <v>5</v>
+      </c>
+      <c r="R66" s="36">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="67" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="67"/>
-      <c r="B67" s="88"/>
+      <c r="B67" s="94"/>
       <c r="C67" s="46" t="s">
         <v>18</v>
       </c>
@@ -8629,7 +8828,7 @@
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="67"/>
-      <c r="B68" s="86">
+      <c r="B68" s="92">
         <v>31</v>
       </c>
       <c r="C68" s="60" t="s">
@@ -8637,68 +8836,68 @@
       </c>
       <c r="D68" s="10">
         <f>SUM(D69:D71)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E68" s="16">
         <f t="shared" ref="E68:M68" si="40">SUM(E69:E71)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F68" s="16">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G68" s="16">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H68" s="16">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I68" s="16">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J68" s="16">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K68" s="16">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L68" s="16">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="M68" s="16">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="N68" s="16">
         <f t="shared" ref="N68:R68" si="41">SUM(N69:N71)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="O68" s="16">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P68" s="16">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Q68" s="16">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="R68" s="35">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="67"/>
-      <c r="B69" s="87"/>
+      <c r="B69" s="93"/>
       <c r="C69" s="45" t="s">
         <v>16</v>
       </c>
@@ -8723,31 +8922,60 @@
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="67"/>
-      <c r="B70" s="87"/>
+      <c r="B70" s="93"/>
       <c r="C70" s="45" t="s">
         <v>17</v>
       </c>
       <c r="D70" s="24">
-        <v>0</v>
-      </c>
-      <c r="E70" s="31"/>
-      <c r="F70" s="31"/>
-      <c r="G70" s="31"/>
-      <c r="H70" s="31"/>
-      <c r="I70" s="31"/>
-      <c r="J70" s="32"/>
-      <c r="K70" s="32"/>
-      <c r="L70" s="32"/>
-      <c r="M70" s="32"/>
-      <c r="N70" s="32"/>
-      <c r="O70" s="32"/>
-      <c r="P70" s="32"/>
-      <c r="Q70" s="32"/>
-      <c r="R70" s="37"/>
+        <f>D32</f>
+        <v>3</v>
+      </c>
+      <c r="E70" s="31">
+        <v>3</v>
+      </c>
+      <c r="F70" s="31">
+        <v>3</v>
+      </c>
+      <c r="G70" s="31">
+        <v>2</v>
+      </c>
+      <c r="H70" s="31">
+        <v>-1</v>
+      </c>
+      <c r="I70" s="31">
+        <v>-1</v>
+      </c>
+      <c r="J70" s="31">
+        <v>-1</v>
+      </c>
+      <c r="K70" s="31">
+        <v>-1</v>
+      </c>
+      <c r="L70" s="31">
+        <v>-1</v>
+      </c>
+      <c r="M70" s="31">
+        <v>-1</v>
+      </c>
+      <c r="N70" s="31">
+        <v>-1</v>
+      </c>
+      <c r="O70" s="31">
+        <v>-1</v>
+      </c>
+      <c r="P70" s="31">
+        <v>-1</v>
+      </c>
+      <c r="Q70" s="31">
+        <v>-1</v>
+      </c>
+      <c r="R70" s="31">
+        <v>-1</v>
+      </c>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="68"/>
-      <c r="B71" s="88"/>
+      <c r="B71" s="94"/>
       <c r="C71" s="46" t="s">
         <v>18</v>
       </c>
@@ -8774,74 +9002,74 @@
       <c r="A72" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="B72" s="81"/>
+      <c r="B72" s="79"/>
       <c r="C72" s="10" t="s">
         <v>39</v>
       </c>
       <c r="D72" s="10">
         <f>SUM(D73:D75)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E72" s="16">
         <f t="shared" ref="E72:M72" si="43">SUM(E73:E75)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F72" s="16">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G72" s="16">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H72" s="16">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I72" s="16">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J72" s="16">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K72" s="16">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L72" s="16">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M72" s="16">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N72" s="16">
         <f t="shared" ref="N72:R72" si="44">SUM(N73:N75)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O72" s="16">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P72" s="16">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q72" s="16">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R72" s="35">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="67"/>
-      <c r="B73" s="82"/>
+      <c r="B73" s="80"/>
       <c r="C73" s="45" t="s">
         <v>16</v>
       </c>
@@ -8866,31 +9094,60 @@
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="67"/>
-      <c r="B74" s="82"/>
+      <c r="B74" s="80"/>
       <c r="C74" s="45" t="s">
         <v>17</v>
       </c>
       <c r="D74" s="24">
-        <v>0</v>
-      </c>
-      <c r="E74" s="31"/>
-      <c r="F74" s="31"/>
-      <c r="G74" s="31"/>
-      <c r="H74" s="31"/>
-      <c r="I74" s="31"/>
-      <c r="J74" s="32"/>
-      <c r="K74" s="32"/>
-      <c r="L74" s="32"/>
-      <c r="M74" s="32"/>
-      <c r="N74" s="32"/>
-      <c r="O74" s="32"/>
-      <c r="P74" s="32"/>
-      <c r="Q74" s="32"/>
-      <c r="R74" s="37"/>
+        <f>D36</f>
+        <v>2</v>
+      </c>
+      <c r="E74" s="31">
+        <v>2</v>
+      </c>
+      <c r="F74" s="31">
+        <v>1</v>
+      </c>
+      <c r="G74" s="31">
+        <v>1</v>
+      </c>
+      <c r="H74" s="31">
+        <v>1</v>
+      </c>
+      <c r="I74" s="31">
+        <v>1</v>
+      </c>
+      <c r="J74" s="31">
+        <v>1</v>
+      </c>
+      <c r="K74" s="31">
+        <v>1</v>
+      </c>
+      <c r="L74" s="31">
+        <v>1</v>
+      </c>
+      <c r="M74" s="31">
+        <v>1</v>
+      </c>
+      <c r="N74" s="31">
+        <v>1</v>
+      </c>
+      <c r="O74" s="31">
+        <v>1</v>
+      </c>
+      <c r="P74" s="31">
+        <v>1</v>
+      </c>
+      <c r="Q74" s="31">
+        <v>1</v>
+      </c>
+      <c r="R74" s="31">
+        <v>1</v>
+      </c>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="67"/>
-      <c r="B75" s="83"/>
+      <c r="B75" s="81"/>
       <c r="C75" s="45" t="s">
         <v>18</v>
       </c>
@@ -8915,74 +9172,74 @@
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="67"/>
-      <c r="B76" s="91"/>
+      <c r="B76" s="86"/>
       <c r="C76" s="10" t="s">
         <v>40</v>
       </c>
       <c r="D76" s="10">
         <f>SUM(D77:D79)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E76" s="21">
         <f t="shared" ref="E76:M76" si="46">SUM(E77:E79)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F76" s="21">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G76" s="21">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="H76" s="21">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="I76" s="21">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="J76" s="21">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="K76" s="21">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="L76" s="21">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="M76" s="21">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="N76" s="21">
         <f t="shared" ref="N76:R76" si="47">SUM(N77:N79)</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="O76" s="21">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="P76" s="21">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="Q76" s="21">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="R76" s="13">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="67"/>
-      <c r="B77" s="92"/>
+      <c r="B77" s="87"/>
       <c r="C77" s="45" t="s">
         <v>16</v>
       </c>
@@ -9007,31 +9264,60 @@
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="67"/>
-      <c r="B78" s="92"/>
+      <c r="B78" s="87"/>
       <c r="C78" s="45" t="s">
         <v>17</v>
       </c>
       <c r="D78" s="24">
-        <v>0</v>
-      </c>
-      <c r="E78" s="31"/>
-      <c r="F78" s="31"/>
-      <c r="G78" s="31"/>
-      <c r="H78" s="31"/>
-      <c r="I78" s="31"/>
-      <c r="J78" s="31"/>
-      <c r="K78" s="31"/>
-      <c r="L78" s="31"/>
-      <c r="M78" s="31"/>
-      <c r="N78" s="31"/>
-      <c r="O78" s="31"/>
-      <c r="P78" s="31"/>
-      <c r="Q78" s="31"/>
-      <c r="R78" s="36"/>
+        <f>D40</f>
+        <v>6</v>
+      </c>
+      <c r="E78" s="31">
+        <v>6</v>
+      </c>
+      <c r="F78" s="31">
+        <v>2</v>
+      </c>
+      <c r="G78" s="31">
+        <v>-3</v>
+      </c>
+      <c r="H78" s="31">
+        <v>-3</v>
+      </c>
+      <c r="I78" s="31">
+        <v>-3</v>
+      </c>
+      <c r="J78" s="31">
+        <v>-3</v>
+      </c>
+      <c r="K78" s="31">
+        <v>-3</v>
+      </c>
+      <c r="L78" s="31">
+        <v>-3</v>
+      </c>
+      <c r="M78" s="31">
+        <v>-3</v>
+      </c>
+      <c r="N78" s="31">
+        <v>-3</v>
+      </c>
+      <c r="O78" s="31">
+        <v>-3</v>
+      </c>
+      <c r="P78" s="31">
+        <v>-3</v>
+      </c>
+      <c r="Q78" s="31">
+        <v>-3</v>
+      </c>
+      <c r="R78" s="31">
+        <v>-3</v>
+      </c>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" s="68"/>
-      <c r="B79" s="93"/>
+      <c r="B79" s="88"/>
       <c r="C79" s="46" t="s">
         <v>18</v>
       </c>
@@ -9055,107 +9341,107 @@
       <c r="R79" s="39"/>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B80" s="89" t="s">
+      <c r="B80" s="95" t="s">
         <v>26</v>
       </c>
-      <c r="C80" s="89"/>
+      <c r="C80" s="95"/>
       <c r="D80" s="2">
         <f t="shared" ref="D80:M80" si="49">SUM(D44,D64,D68,D72,D76)</f>
-        <v>0</v>
+        <v>17.5</v>
       </c>
       <c r="E80" s="2">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>17.5</v>
       </c>
       <c r="F80" s="2">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="G80" s="2">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="H80" s="2">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="I80" s="2">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="J80" s="2">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="K80" s="2">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="L80" s="2">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="M80" s="2">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="N80" s="2">
         <f t="shared" ref="N80:R80" si="50">SUM(N44,N64,N68,N72,N76)</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="O80" s="2">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="P80" s="2">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="Q80" s="2">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="R80" s="2">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D81">
         <f>D80</f>
-        <v>0</v>
+        <v>17.5</v>
       </c>
       <c r="E81">
         <f t="shared" ref="E81:M81" si="51" xml:space="preserve"> D81 - ($D$81/COUNT($D$4:$M$4))</f>
-        <v>0</v>
+        <v>15.555555555555555</v>
       </c>
       <c r="F81">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>13.611111111111111</v>
       </c>
       <c r="G81">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>11.666666666666666</v>
       </c>
       <c r="H81">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>9.7222222222222214</v>
       </c>
       <c r="I81">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>7.7777777777777768</v>
       </c>
       <c r="J81">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>5.8333333333333321</v>
       </c>
       <c r="K81">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>3.8888888888888875</v>
       </c>
       <c r="L81">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>1.9444444444444431</v>
       </c>
       <c r="M81">
         <f t="shared" si="51"/>
@@ -9163,27 +9449,37 @@
       </c>
       <c r="N81">
         <f t="shared" ref="N81:R81" si="52" xml:space="preserve"> M81 - ($D$81/COUNT($D$4:$M$4))</f>
-        <v>0</v>
+        <v>-1.9444444444444444</v>
       </c>
       <c r="O81">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>-3.8888888888888888</v>
       </c>
       <c r="P81">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>-5.833333333333333</v>
       </c>
       <c r="Q81">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>-7.7777777777777777</v>
       </c>
       <c r="R81">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>-9.7222222222222214</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="E2:K2"/>
+    <mergeCell ref="L2:R2"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="B68:B71"/>
     <mergeCell ref="A72:A79"/>
     <mergeCell ref="B34:B37"/>
     <mergeCell ref="B38:B41"/>
@@ -9200,16 +9496,6 @@
     <mergeCell ref="B48:B51"/>
     <mergeCell ref="B52:B55"/>
     <mergeCell ref="B64:B67"/>
-    <mergeCell ref="E2:K2"/>
-    <mergeCell ref="L2:R2"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="B68:B71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Added my estimated hours for sprint 6
</commit_message>
<xml_diff>
--- a/Management/Burndown.xlsx
+++ b/Management/Burndown.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="15" yWindow="-30" windowWidth="14265" windowHeight="13020" activeTab="6"/>
@@ -15,7 +15,10 @@
     <sheet name="Sp5" sheetId="6" r:id="rId6"/>
     <sheet name="Sp6" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -25,7 +28,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="G2" authorId="0">
+    <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -791,6 +794,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -839,12 +845,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -860,20 +860,11 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -892,6 +883,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -922,9 +928,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -964,6 +967,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1135,11 +1141,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="68380928"/>
-        <c:axId val="68039040"/>
+        <c:axId val="268191096"/>
+        <c:axId val="268185216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="68380928"/>
+        <c:axId val="268191096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1164,10 +1170,11 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68039040"/>
+        <c:crossAx val="268185216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1175,7 +1182,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68039040"/>
+        <c:axId val="268185216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1205,7 +1212,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68380928"/>
+        <c:crossAx val="268191096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1463,13 +1470,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="68388736"/>
-        <c:axId val="68390272"/>
+        <c:axId val="268187568"/>
+        <c:axId val="268191880"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="68388736"/>
+        <c:axId val="268187568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1479,14 +1485,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68390272"/>
+        <c:crossAx val="268191880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="68390272"/>
+        <c:axId val="268191880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1497,7 +1503,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68388736"/>
+        <c:crossAx val="268187568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1718,13 +1724,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="68874624"/>
-        <c:axId val="68876160"/>
+        <c:axId val="268187176"/>
+        <c:axId val="268186784"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="68874624"/>
+        <c:axId val="268187176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1734,14 +1739,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68876160"/>
+        <c:crossAx val="268186784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="68876160"/>
+        <c:axId val="268186784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1752,7 +1757,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68874624"/>
+        <c:crossAx val="268187176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2033,13 +2038,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="68766336"/>
-        <c:axId val="68796800"/>
+        <c:axId val="268189136"/>
+        <c:axId val="268186000"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="68766336"/>
+        <c:axId val="268189136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2049,14 +2053,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68796800"/>
+        <c:crossAx val="268186000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="68796800"/>
+        <c:axId val="268186000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2067,7 +2071,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68766336"/>
+        <c:crossAx val="268189136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2352,23 +2356,22 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="69116672"/>
-        <c:axId val="69118208"/>
+        <c:axId val="268186392"/>
+        <c:axId val="268187960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69116672"/>
+        <c:axId val="268186392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="[$-409]d\-mmm;@" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69118208"/>
+        <c:crossAx val="268187960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2376,7 +2379,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69118208"/>
+        <c:axId val="268187960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2387,7 +2390,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69116672"/>
+        <c:crossAx val="268186392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2668,13 +2671,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="82799616"/>
-        <c:axId val="82805504"/>
+        <c:axId val="267792184"/>
+        <c:axId val="267792576"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="82799616"/>
+        <c:axId val="267792184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2684,14 +2686,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82805504"/>
+        <c:crossAx val="267792576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="82805504"/>
+        <c:axId val="267792576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2702,14 +2704,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82799616"/>
+        <c:crossAx val="267792184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2900,13 +2901,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="99461760"/>
-        <c:axId val="99471744"/>
+        <c:axId val="334335624"/>
+        <c:axId val="334338368"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="99461760"/>
+        <c:axId val="334335624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2916,14 +2916,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99471744"/>
+        <c:crossAx val="334338368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="99471744"/>
+        <c:axId val="334338368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2934,14 +2934,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99461760"/>
+        <c:crossAx val="334335624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3254,7 +3253,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3289,7 +3288,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3516,13 +3515,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="79" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
+      <c r="B1" s="80" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
     </row>
     <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -3857,22 +3856,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E2" s="89" t="s">
+      <c r="E2" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="80" t="s">
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="80"/>
-      <c r="P2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="82"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C3" s="5" t="s">
@@ -3987,10 +3986,10 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="92">
+      <c r="B6" s="93">
         <v>2</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -4054,8 +4053,8 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="83"/>
-      <c r="B7" s="93"/>
+      <c r="A7" s="84"/>
+      <c r="B7" s="94"/>
       <c r="C7" s="7" t="s">
         <v>16</v>
       </c>
@@ -4084,8 +4083,8 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="83"/>
-      <c r="B8" s="93"/>
+      <c r="A8" s="84"/>
+      <c r="B8" s="94"/>
       <c r="C8" s="7" t="s">
         <v>17</v>
       </c>
@@ -4112,8 +4111,8 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="83"/>
-      <c r="B9" s="93"/>
+      <c r="A9" s="84"/>
+      <c r="B9" s="94"/>
       <c r="C9" s="8" t="s">
         <v>18</v>
       </c>
@@ -4142,8 +4141,8 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="83"/>
-      <c r="B10" s="93"/>
+      <c r="A10" s="84"/>
+      <c r="B10" s="94"/>
       <c r="C10" s="9" t="s">
         <v>19</v>
       </c>
@@ -4205,8 +4204,8 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="83"/>
-      <c r="B11" s="93"/>
+      <c r="A11" s="84"/>
+      <c r="B11" s="94"/>
       <c r="C11" s="7" t="s">
         <v>16</v>
       </c>
@@ -4229,8 +4228,8 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="83"/>
-      <c r="B12" s="93"/>
+      <c r="A12" s="84"/>
+      <c r="B12" s="94"/>
       <c r="C12" s="7" t="s">
         <v>17</v>
       </c>
@@ -4259,8 +4258,8 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="83"/>
-      <c r="B13" s="93"/>
+      <c r="A13" s="84"/>
+      <c r="B13" s="94"/>
       <c r="C13" s="8" t="s">
         <v>18</v>
       </c>
@@ -4283,8 +4282,8 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="83"/>
-      <c r="B14" s="93"/>
+      <c r="A14" s="84"/>
+      <c r="B14" s="94"/>
       <c r="C14" s="9" t="s">
         <v>20</v>
       </c>
@@ -4346,8 +4345,8 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="83"/>
-      <c r="B15" s="93"/>
+      <c r="A15" s="84"/>
+      <c r="B15" s="94"/>
       <c r="C15" s="7" t="s">
         <v>16</v>
       </c>
@@ -4370,8 +4369,8 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="83"/>
-      <c r="B16" s="93"/>
+      <c r="A16" s="84"/>
+      <c r="B16" s="94"/>
       <c r="C16" s="7" t="s">
         <v>17</v>
       </c>
@@ -4394,8 +4393,8 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="83"/>
-      <c r="B17" s="94"/>
+      <c r="A17" s="84"/>
+      <c r="B17" s="95"/>
       <c r="C17" s="8" t="s">
         <v>18</v>
       </c>
@@ -4422,8 +4421,8 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="83"/>
-      <c r="B18" s="92">
+      <c r="A18" s="84"/>
+      <c r="B18" s="93">
         <v>3</v>
       </c>
       <c r="C18" s="9" t="s">
@@ -4487,8 +4486,8 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="83"/>
-      <c r="B19" s="93"/>
+      <c r="A19" s="84"/>
+      <c r="B19" s="94"/>
       <c r="C19" s="7" t="s">
         <v>16</v>
       </c>
@@ -4517,8 +4516,8 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="83"/>
-      <c r="B20" s="93"/>
+      <c r="A20" s="84"/>
+      <c r="B20" s="94"/>
       <c r="C20" s="7" t="s">
         <v>17</v>
       </c>
@@ -4541,8 +4540,8 @@
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="84"/>
-      <c r="B21" s="94"/>
+      <c r="A21" s="85"/>
+      <c r="B21" s="95"/>
       <c r="C21" s="8" t="s">
         <v>18</v>
       </c>
@@ -4565,10 +4564,10 @@
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="82" t="s">
+      <c r="A22" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="85"/>
+      <c r="B22" s="86"/>
       <c r="C22" s="9" t="s">
         <v>24</v>
       </c>
@@ -4630,8 +4629,8 @@
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="83"/>
-      <c r="B23" s="86"/>
+      <c r="A23" s="84"/>
+      <c r="B23" s="87"/>
       <c r="C23" s="7" t="s">
         <v>16</v>
       </c>
@@ -4654,8 +4653,8 @@
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="83"/>
-      <c r="B24" s="86"/>
+      <c r="A24" s="84"/>
+      <c r="B24" s="87"/>
       <c r="C24" s="7" t="s">
         <v>17</v>
       </c>
@@ -4682,8 +4681,8 @@
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="84"/>
-      <c r="B25" s="87"/>
+      <c r="A25" s="85"/>
+      <c r="B25" s="88"/>
       <c r="C25" s="8" t="s">
         <v>18</v>
       </c>
@@ -4706,10 +4705,10 @@
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B26" s="88" t="s">
+      <c r="B26" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="88"/>
+      <c r="C26" s="89"/>
       <c r="D26" s="2">
         <f>SUM(D6,D10,D14,D18,D22)</f>
         <v>19</v>
@@ -4774,10 +4773,10 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="82" t="s">
+      <c r="A28" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="92">
+      <c r="B28" s="93">
         <v>2</v>
       </c>
       <c r="C28" s="6" t="s">
@@ -4838,8 +4837,8 @@
       <c r="Q28" s="23"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="83"/>
-      <c r="B29" s="93"/>
+      <c r="A29" s="84"/>
+      <c r="B29" s="94"/>
       <c r="C29" s="7" t="s">
         <v>16</v>
       </c>
@@ -4885,8 +4884,8 @@
       <c r="Q29" s="24"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="83"/>
-      <c r="B30" s="93"/>
+      <c r="A30" s="84"/>
+      <c r="B30" s="94"/>
       <c r="C30" s="7" t="s">
         <v>17</v>
       </c>
@@ -4932,8 +4931,8 @@
       <c r="Q30" s="24"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="83"/>
-      <c r="B31" s="93"/>
+      <c r="A31" s="84"/>
+      <c r="B31" s="94"/>
       <c r="C31" s="8" t="s">
         <v>18</v>
       </c>
@@ -4979,8 +4978,8 @@
       <c r="Q31" s="24"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="83"/>
-      <c r="B32" s="93"/>
+      <c r="A32" s="84"/>
+      <c r="B32" s="94"/>
       <c r="C32" s="9" t="s">
         <v>19</v>
       </c>
@@ -5039,8 +5038,8 @@
       <c r="Q32" s="23"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="83"/>
-      <c r="B33" s="93"/>
+      <c r="A33" s="84"/>
+      <c r="B33" s="94"/>
       <c r="C33" s="7" t="s">
         <v>16</v>
       </c>
@@ -5060,8 +5059,8 @@
       <c r="Q33" s="24"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="83"/>
-      <c r="B34" s="93"/>
+      <c r="A34" s="84"/>
+      <c r="B34" s="94"/>
       <c r="C34" s="7" t="s">
         <v>17</v>
       </c>
@@ -5107,8 +5106,8 @@
       <c r="Q34" s="24"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" s="83"/>
-      <c r="B35" s="93"/>
+      <c r="A35" s="84"/>
+      <c r="B35" s="94"/>
       <c r="C35" s="8" t="s">
         <v>18</v>
       </c>
@@ -5128,8 +5127,8 @@
       <c r="Q35" s="24"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="83"/>
-      <c r="B36" s="93"/>
+      <c r="A36" s="84"/>
+      <c r="B36" s="94"/>
       <c r="C36" s="9" t="s">
         <v>20</v>
       </c>
@@ -5188,8 +5187,8 @@
       <c r="Q36" s="23"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="83"/>
-      <c r="B37" s="93"/>
+      <c r="A37" s="84"/>
+      <c r="B37" s="94"/>
       <c r="C37" s="7" t="s">
         <v>16</v>
       </c>
@@ -5209,8 +5208,8 @@
       <c r="Q37" s="24"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A38" s="83"/>
-      <c r="B38" s="93"/>
+      <c r="A38" s="84"/>
+      <c r="B38" s="94"/>
       <c r="C38" s="7" t="s">
         <v>17</v>
       </c>
@@ -5230,8 +5229,8 @@
       <c r="Q38" s="24"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="83"/>
-      <c r="B39" s="94"/>
+      <c r="A39" s="84"/>
+      <c r="B39" s="95"/>
       <c r="C39" s="8" t="s">
         <v>18</v>
       </c>
@@ -5277,8 +5276,8 @@
       <c r="Q39" s="24"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="83"/>
-      <c r="B40" s="92">
+      <c r="A40" s="84"/>
+      <c r="B40" s="93">
         <v>3</v>
       </c>
       <c r="C40" s="9" t="s">
@@ -5339,8 +5338,8 @@
       <c r="Q40" s="23"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="83"/>
-      <c r="B41" s="93"/>
+      <c r="A41" s="84"/>
+      <c r="B41" s="94"/>
       <c r="C41" s="7" t="s">
         <v>16</v>
       </c>
@@ -5386,8 +5385,8 @@
       <c r="Q41" s="24"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A42" s="83"/>
-      <c r="B42" s="93"/>
+      <c r="A42" s="84"/>
+      <c r="B42" s="94"/>
       <c r="C42" s="7" t="s">
         <v>17</v>
       </c>
@@ -5407,8 +5406,8 @@
       <c r="Q42" s="24"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="84"/>
-      <c r="B43" s="94"/>
+      <c r="A43" s="85"/>
+      <c r="B43" s="95"/>
       <c r="C43" s="8" t="s">
         <v>18</v>
       </c>
@@ -5428,10 +5427,10 @@
       <c r="Q43" s="24"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="82" t="s">
+      <c r="A44" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="B44" s="85"/>
+      <c r="B44" s="86"/>
       <c r="C44" s="9" t="s">
         <v>24</v>
       </c>
@@ -5490,8 +5489,8 @@
       <c r="Q44" s="23"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A45" s="83"/>
-      <c r="B45" s="86"/>
+      <c r="A45" s="84"/>
+      <c r="B45" s="87"/>
       <c r="C45" s="7" t="s">
         <v>16</v>
       </c>
@@ -5511,8 +5510,8 @@
       <c r="Q45" s="24"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A46" s="83"/>
-      <c r="B46" s="86"/>
+      <c r="A46" s="84"/>
+      <c r="B46" s="87"/>
       <c r="C46" s="7" t="s">
         <v>17</v>
       </c>
@@ -5558,8 +5557,8 @@
       <c r="Q46" s="24"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="84"/>
-      <c r="B47" s="87"/>
+      <c r="A47" s="85"/>
+      <c r="B47" s="88"/>
       <c r="C47" s="8" t="s">
         <v>18</v>
       </c>
@@ -5579,10 +5578,10 @@
       <c r="Q47" s="24"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B48" s="88" t="s">
+      <c r="B48" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="C48" s="88"/>
+      <c r="C48" s="89"/>
       <c r="D48" s="2">
         <f>SUM(D28,D32,D36,D40,D44)</f>
         <v>19</v>
@@ -5743,19 +5742,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E2" s="89" t="s">
+      <c r="E2" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="89" t="s">
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="91"/>
+      <c r="M2" s="92"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D3" s="5" t="s">
@@ -5845,10 +5844,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="97">
+      <c r="B6" s="96">
         <v>1</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -5900,8 +5899,8 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="83"/>
-      <c r="B7" s="98"/>
+      <c r="A7" s="84"/>
+      <c r="B7" s="97"/>
       <c r="C7" s="45" t="s">
         <v>16</v>
       </c>
@@ -5921,8 +5920,8 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="83"/>
-      <c r="B8" s="98"/>
+      <c r="A8" s="84"/>
+      <c r="B8" s="97"/>
       <c r="C8" s="45" t="s">
         <v>17</v>
       </c>
@@ -5946,8 +5945,8 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="83"/>
-      <c r="B9" s="99"/>
+      <c r="A9" s="84"/>
+      <c r="B9" s="98"/>
       <c r="C9" s="46" t="s">
         <v>18</v>
       </c>
@@ -5967,8 +5966,8 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="83"/>
-      <c r="B10" s="100" t="s">
+      <c r="A10" s="84"/>
+      <c r="B10" s="99" t="s">
         <v>35</v>
       </c>
       <c r="C10" s="47" t="s">
@@ -6020,8 +6019,8 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="83"/>
-      <c r="B11" s="101"/>
+      <c r="A11" s="84"/>
+      <c r="B11" s="100"/>
       <c r="C11" s="45" t="s">
         <v>16</v>
       </c>
@@ -6045,8 +6044,8 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="83"/>
-      <c r="B12" s="101"/>
+      <c r="A12" s="84"/>
+      <c r="B12" s="100"/>
       <c r="C12" s="45" t="s">
         <v>17</v>
       </c>
@@ -6066,8 +6065,8 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="83"/>
-      <c r="B13" s="101"/>
+      <c r="A13" s="84"/>
+      <c r="B13" s="100"/>
       <c r="C13" s="46" t="s">
         <v>18</v>
       </c>
@@ -6087,8 +6086,8 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="83"/>
-      <c r="B14" s="101"/>
+      <c r="A14" s="84"/>
+      <c r="B14" s="100"/>
       <c r="C14" s="52" t="s">
         <v>33</v>
       </c>
@@ -6138,8 +6137,8 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="83"/>
-      <c r="B15" s="101"/>
+      <c r="A15" s="84"/>
+      <c r="B15" s="100"/>
       <c r="C15" s="45" t="s">
         <v>16</v>
       </c>
@@ -6165,8 +6164,8 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="83"/>
-      <c r="B16" s="101"/>
+      <c r="A16" s="84"/>
+      <c r="B16" s="100"/>
       <c r="C16" s="45" t="s">
         <v>17</v>
       </c>
@@ -6190,8 +6189,8 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="83"/>
-      <c r="B17" s="101"/>
+      <c r="A17" s="84"/>
+      <c r="B17" s="100"/>
       <c r="C17" s="45" t="s">
         <v>18</v>
       </c>
@@ -6211,10 +6210,10 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="82" t="s">
+      <c r="A18" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="92"/>
+      <c r="B18" s="93"/>
       <c r="C18" s="10" t="s">
         <v>34</v>
       </c>
@@ -6264,8 +6263,8 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="83"/>
-      <c r="B19" s="93"/>
+      <c r="A19" s="84"/>
+      <c r="B19" s="94"/>
       <c r="C19" s="45" t="s">
         <v>16</v>
       </c>
@@ -6289,8 +6288,8 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="83"/>
-      <c r="B20" s="93"/>
+      <c r="A20" s="84"/>
+      <c r="B20" s="94"/>
       <c r="C20" s="45" t="s">
         <v>17</v>
       </c>
@@ -6314,8 +6313,8 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="83"/>
-      <c r="B21" s="93"/>
+      <c r="A21" s="84"/>
+      <c r="B21" s="94"/>
       <c r="C21" s="46" t="s">
         <v>18</v>
       </c>
@@ -6335,8 +6334,8 @@
       </c>
     </row>
     <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="83"/>
-      <c r="B22" s="95"/>
+      <c r="A22" s="84"/>
+      <c r="B22" s="101"/>
       <c r="C22" s="49" t="s">
         <v>31</v>
       </c>
@@ -6386,8 +6385,8 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="83"/>
-      <c r="B23" s="95"/>
+      <c r="A23" s="84"/>
+      <c r="B23" s="101"/>
       <c r="C23" s="45" t="s">
         <v>16</v>
       </c>
@@ -6407,8 +6406,8 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="83"/>
-      <c r="B24" s="95"/>
+      <c r="A24" s="84"/>
+      <c r="B24" s="101"/>
       <c r="C24" s="45" t="s">
         <v>17</v>
       </c>
@@ -6432,8 +6431,8 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="84"/>
-      <c r="B25" s="96"/>
+      <c r="A25" s="85"/>
+      <c r="B25" s="102"/>
       <c r="C25" s="46" t="s">
         <v>18</v>
       </c>
@@ -6453,10 +6452,10 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="88" t="s">
+      <c r="B26" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="88"/>
+      <c r="C26" s="89"/>
       <c r="D26" s="2">
         <f>SUM(D6,D10,D14,D18,D22)</f>
         <v>14</v>
@@ -6509,10 +6508,10 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="82" t="s">
+      <c r="A28" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="97">
+      <c r="B28" s="96">
         <v>1</v>
       </c>
       <c r="C28" s="10" t="s">
@@ -6561,8 +6560,8 @@
       <c r="N28" s="23"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="83"/>
-      <c r="B29" s="98"/>
+      <c r="A29" s="84"/>
+      <c r="B29" s="97"/>
       <c r="C29" s="45" t="s">
         <v>16</v>
       </c>
@@ -6582,8 +6581,8 @@
       <c r="N29" s="24"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="83"/>
-      <c r="B30" s="98"/>
+      <c r="A30" s="84"/>
+      <c r="B30" s="97"/>
       <c r="C30" s="45" t="s">
         <v>17</v>
       </c>
@@ -6621,8 +6620,8 @@
       <c r="N30" s="24"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="83"/>
-      <c r="B31" s="99"/>
+      <c r="A31" s="84"/>
+      <c r="B31" s="98"/>
       <c r="C31" s="46" t="s">
         <v>18</v>
       </c>
@@ -6642,8 +6641,8 @@
       <c r="N31" s="24"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="83"/>
-      <c r="B32" s="100" t="s">
+      <c r="A32" s="84"/>
+      <c r="B32" s="99" t="s">
         <v>35</v>
       </c>
       <c r="C32" s="47" t="s">
@@ -6692,8 +6691,8 @@
       <c r="N32" s="23"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="83"/>
-      <c r="B33" s="101"/>
+      <c r="A33" s="84"/>
+      <c r="B33" s="100"/>
       <c r="C33" s="45" t="s">
         <v>16</v>
       </c>
@@ -6731,8 +6730,8 @@
       <c r="N33" s="24"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="83"/>
-      <c r="B34" s="101"/>
+      <c r="A34" s="84"/>
+      <c r="B34" s="100"/>
       <c r="C34" s="45" t="s">
         <v>17</v>
       </c>
@@ -6752,8 +6751,8 @@
       <c r="N34" s="24"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="83"/>
-      <c r="B35" s="101"/>
+      <c r="A35" s="84"/>
+      <c r="B35" s="100"/>
       <c r="C35" s="46" t="s">
         <v>18</v>
       </c>
@@ -6791,8 +6790,8 @@
       <c r="N35" s="24"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="83"/>
-      <c r="B36" s="101"/>
+      <c r="A36" s="84"/>
+      <c r="B36" s="100"/>
       <c r="C36" s="52" t="s">
         <v>33</v>
       </c>
@@ -6839,8 +6838,8 @@
       <c r="N36" s="23"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="83"/>
-      <c r="B37" s="101"/>
+      <c r="A37" s="84"/>
+      <c r="B37" s="100"/>
       <c r="C37" s="45" t="s">
         <v>16</v>
       </c>
@@ -6878,8 +6877,8 @@
       <c r="N37" s="24"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="83"/>
-      <c r="B38" s="101"/>
+      <c r="A38" s="84"/>
+      <c r="B38" s="100"/>
       <c r="C38" s="45" t="s">
         <v>17</v>
       </c>
@@ -6917,8 +6916,8 @@
       <c r="N38" s="24"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="83"/>
-      <c r="B39" s="101"/>
+      <c r="A39" s="84"/>
+      <c r="B39" s="100"/>
       <c r="C39" s="45" t="s">
         <v>18</v>
       </c>
@@ -6938,10 +6937,10 @@
       <c r="N39" s="24"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="82" t="s">
+      <c r="A40" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="B40" s="92"/>
+      <c r="B40" s="93"/>
       <c r="C40" s="10" t="s">
         <v>34</v>
       </c>
@@ -6988,8 +6987,8 @@
       <c r="N40" s="23"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="83"/>
-      <c r="B41" s="93"/>
+      <c r="A41" s="84"/>
+      <c r="B41" s="94"/>
       <c r="C41" s="45" t="s">
         <v>16</v>
       </c>
@@ -7027,8 +7026,8 @@
       <c r="N41" s="24"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="83"/>
-      <c r="B42" s="93"/>
+      <c r="A42" s="84"/>
+      <c r="B42" s="94"/>
       <c r="C42" s="45" t="s">
         <v>17</v>
       </c>
@@ -7066,8 +7065,8 @@
       <c r="N42" s="24"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="83"/>
-      <c r="B43" s="93"/>
+      <c r="A43" s="84"/>
+      <c r="B43" s="94"/>
       <c r="C43" s="46" t="s">
         <v>18</v>
       </c>
@@ -7087,8 +7086,8 @@
       <c r="N43" s="24"/>
     </row>
     <row r="44" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="83"/>
-      <c r="B44" s="95"/>
+      <c r="A44" s="84"/>
+      <c r="B44" s="101"/>
       <c r="C44" s="49" t="s">
         <v>31</v>
       </c>
@@ -7135,8 +7134,8 @@
       <c r="N44" s="23"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="83"/>
-      <c r="B45" s="95"/>
+      <c r="A45" s="84"/>
+      <c r="B45" s="101"/>
       <c r="C45" s="45" t="s">
         <v>16</v>
       </c>
@@ -7156,8 +7155,8 @@
       <c r="N45" s="24"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="83"/>
-      <c r="B46" s="95"/>
+      <c r="A46" s="84"/>
+      <c r="B46" s="101"/>
       <c r="C46" s="45" t="s">
         <v>17</v>
       </c>
@@ -7195,8 +7194,8 @@
       <c r="N46" s="24"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="84"/>
-      <c r="B47" s="96"/>
+      <c r="A47" s="85"/>
+      <c r="B47" s="102"/>
       <c r="C47" s="46" t="s">
         <v>18</v>
       </c>
@@ -7234,10 +7233,10 @@
       <c r="N47" s="24"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B48" s="88" t="s">
+      <c r="B48" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="C48" s="88"/>
+      <c r="C48" s="89"/>
       <c r="D48" s="2">
         <f>SUM(D28,D32,D36,D40,D44)</f>
         <v>14</v>
@@ -7324,6 +7323,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="A6:A17"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B17"/>
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="A28:A39"/>
@@ -7332,14 +7339,6 @@
     <mergeCell ref="A40:A47"/>
     <mergeCell ref="B40:B43"/>
     <mergeCell ref="B44:B47"/>
-    <mergeCell ref="A18:A25"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="A6:A17"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -7376,24 +7375,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E2" s="89" t="s">
+      <c r="E2" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="89" t="s">
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
-      <c r="P2" s="90"/>
-      <c r="Q2" s="90"/>
-      <c r="R2" s="91"/>
+      <c r="M2" s="91"/>
+      <c r="N2" s="91"/>
+      <c r="O2" s="91"/>
+      <c r="P2" s="91"/>
+      <c r="Q2" s="91"/>
+      <c r="R2" s="92"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D3" s="5" t="s">
@@ -7518,10 +7517,10 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="97">
+      <c r="B6" s="96">
         <v>12</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -7593,8 +7592,8 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="83"/>
-      <c r="B7" s="98"/>
+      <c r="A7" s="84"/>
+      <c r="B7" s="97"/>
       <c r="C7" s="45" t="s">
         <v>16</v>
       </c>
@@ -7619,8 +7618,8 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="83"/>
-      <c r="B8" s="98"/>
+      <c r="A8" s="84"/>
+      <c r="B8" s="97"/>
       <c r="C8" s="45" t="s">
         <v>17</v>
       </c>
@@ -7645,8 +7644,8 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="83"/>
-      <c r="B9" s="99"/>
+      <c r="A9" s="84"/>
+      <c r="B9" s="98"/>
       <c r="C9" s="46" t="s">
         <v>18</v>
       </c>
@@ -7675,8 +7674,8 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="83"/>
-      <c r="B10" s="110">
+      <c r="A10" s="84"/>
+      <c r="B10" s="106">
         <v>15</v>
       </c>
       <c r="C10" s="47" t="s">
@@ -7748,8 +7747,8 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="83"/>
-      <c r="B11" s="111"/>
+      <c r="A11" s="84"/>
+      <c r="B11" s="107"/>
       <c r="C11" s="45" t="s">
         <v>16</v>
       </c>
@@ -7774,8 +7773,8 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="83"/>
-      <c r="B12" s="111"/>
+      <c r="A12" s="84"/>
+      <c r="B12" s="107"/>
       <c r="C12" s="45" t="s">
         <v>17</v>
       </c>
@@ -7800,8 +7799,8 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="83"/>
-      <c r="B13" s="112"/>
+      <c r="A13" s="84"/>
+      <c r="B13" s="108"/>
       <c r="C13" s="46" t="s">
         <v>18</v>
       </c>
@@ -7830,8 +7829,8 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="83"/>
-      <c r="B14" s="110">
+      <c r="A14" s="84"/>
+      <c r="B14" s="106">
         <v>21</v>
       </c>
       <c r="C14" s="60" t="s">
@@ -7903,8 +7902,8 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="83"/>
-      <c r="B15" s="111"/>
+      <c r="A15" s="84"/>
+      <c r="B15" s="107"/>
       <c r="C15" s="45" t="s">
         <v>16</v>
       </c>
@@ -7937,8 +7936,8 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="83"/>
-      <c r="B16" s="111"/>
+      <c r="A16" s="84"/>
+      <c r="B16" s="107"/>
       <c r="C16" s="45" t="s">
         <v>17</v>
       </c>
@@ -7963,8 +7962,8 @@
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="83"/>
-      <c r="B17" s="112"/>
+      <c r="A17" s="84"/>
+      <c r="B17" s="108"/>
       <c r="C17" s="46" t="s">
         <v>18</v>
       </c>
@@ -7989,8 +7988,8 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="83"/>
-      <c r="B18" s="110">
+      <c r="A18" s="84"/>
+      <c r="B18" s="106">
         <v>18</v>
       </c>
       <c r="C18" s="60" t="s">
@@ -8062,8 +8061,8 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="83"/>
-      <c r="B19" s="111"/>
+      <c r="A19" s="84"/>
+      <c r="B19" s="107"/>
       <c r="C19" s="45" t="s">
         <v>16</v>
       </c>
@@ -8092,8 +8091,8 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="83"/>
-      <c r="B20" s="111"/>
+      <c r="A20" s="84"/>
+      <c r="B20" s="107"/>
       <c r="C20" s="45" t="s">
         <v>17</v>
       </c>
@@ -8118,8 +8117,8 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="83"/>
-      <c r="B21" s="112"/>
+      <c r="A21" s="84"/>
+      <c r="B21" s="108"/>
       <c r="C21" s="46" t="s">
         <v>18</v>
       </c>
@@ -8144,8 +8143,8 @@
       </c>
     </row>
     <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="83"/>
-      <c r="B22" s="102" t="s">
+      <c r="A22" s="84"/>
+      <c r="B22" s="109" t="s">
         <v>42</v>
       </c>
       <c r="C22" s="60" t="s">
@@ -8217,8 +8216,8 @@
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="83"/>
-      <c r="B23" s="103"/>
+      <c r="A23" s="84"/>
+      <c r="B23" s="110"/>
       <c r="C23" s="45" t="s">
         <v>16</v>
       </c>
@@ -8243,8 +8242,8 @@
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="83"/>
-      <c r="B24" s="103"/>
+      <c r="A24" s="84"/>
+      <c r="B24" s="110"/>
       <c r="C24" s="45" t="s">
         <v>17</v>
       </c>
@@ -8275,8 +8274,8 @@
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="83"/>
-      <c r="B25" s="104"/>
+      <c r="A25" s="84"/>
+      <c r="B25" s="111"/>
       <c r="C25" s="46" t="s">
         <v>18</v>
       </c>
@@ -8301,8 +8300,8 @@
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="83"/>
-      <c r="B26" s="102" t="s">
+      <c r="A26" s="84"/>
+      <c r="B26" s="109" t="s">
         <v>45</v>
       </c>
       <c r="C26" s="60" t="s">
@@ -8374,8 +8373,8 @@
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="83"/>
-      <c r="B27" s="103"/>
+      <c r="A27" s="84"/>
+      <c r="B27" s="110"/>
       <c r="C27" s="45" t="s">
         <v>16</v>
       </c>
@@ -8400,8 +8399,8 @@
       </c>
     </row>
     <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="83"/>
-      <c r="B28" s="103"/>
+      <c r="A28" s="84"/>
+      <c r="B28" s="110"/>
       <c r="C28" s="45" t="s">
         <v>17</v>
       </c>
@@ -8430,8 +8429,8 @@
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="83"/>
-      <c r="B29" s="104"/>
+      <c r="A29" s="84"/>
+      <c r="B29" s="111"/>
       <c r="C29" s="46" t="s">
         <v>18</v>
       </c>
@@ -8456,8 +8455,8 @@
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="83"/>
-      <c r="B30" s="102">
+      <c r="A30" s="84"/>
+      <c r="B30" s="109">
         <v>31</v>
       </c>
       <c r="C30" s="60" t="s">
@@ -8529,8 +8528,8 @@
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="83"/>
-      <c r="B31" s="103"/>
+      <c r="A31" s="84"/>
+      <c r="B31" s="110"/>
       <c r="C31" s="45" t="s">
         <v>16</v>
       </c>
@@ -8555,8 +8554,8 @@
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="83"/>
-      <c r="B32" s="103"/>
+      <c r="A32" s="84"/>
+      <c r="B32" s="110"/>
       <c r="C32" s="45" t="s">
         <v>17</v>
       </c>
@@ -8585,8 +8584,8 @@
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" s="84"/>
-      <c r="B33" s="104"/>
+      <c r="A33" s="85"/>
+      <c r="B33" s="111"/>
       <c r="C33" s="46" t="s">
         <v>18</v>
       </c>
@@ -8611,10 +8610,10 @@
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A34" s="82" t="s">
+      <c r="A34" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="92"/>
+      <c r="B34" s="93"/>
       <c r="C34" s="10" t="s">
         <v>39</v>
       </c>
@@ -8684,8 +8683,8 @@
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="83"/>
-      <c r="B35" s="93"/>
+      <c r="A35" s="84"/>
+      <c r="B35" s="94"/>
       <c r="C35" s="45" t="s">
         <v>16</v>
       </c>
@@ -8710,8 +8709,8 @@
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A36" s="83"/>
-      <c r="B36" s="93"/>
+      <c r="A36" s="84"/>
+      <c r="B36" s="94"/>
       <c r="C36" s="45" t="s">
         <v>17</v>
       </c>
@@ -8740,8 +8739,8 @@
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="83"/>
-      <c r="B37" s="93"/>
+      <c r="A37" s="84"/>
+      <c r="B37" s="94"/>
       <c r="C37" s="45" t="s">
         <v>18</v>
       </c>
@@ -8766,8 +8765,8 @@
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A38" s="83"/>
-      <c r="B38" s="107"/>
+      <c r="A38" s="84"/>
+      <c r="B38" s="103"/>
       <c r="C38" s="10" t="s">
         <v>40</v>
       </c>
@@ -8837,8 +8836,8 @@
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A39" s="83"/>
-      <c r="B39" s="108"/>
+      <c r="A39" s="84"/>
+      <c r="B39" s="104"/>
       <c r="C39" s="45" t="s">
         <v>16</v>
       </c>
@@ -8863,8 +8862,8 @@
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A40" s="83"/>
-      <c r="B40" s="108"/>
+      <c r="A40" s="84"/>
+      <c r="B40" s="104"/>
       <c r="C40" s="45" t="s">
         <v>17</v>
       </c>
@@ -8893,8 +8892,8 @@
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A41" s="84"/>
-      <c r="B41" s="109"/>
+      <c r="A41" s="85"/>
+      <c r="B41" s="105"/>
       <c r="C41" s="46" t="s">
         <v>18</v>
       </c>
@@ -8919,10 +8918,10 @@
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B42" s="106" t="s">
+      <c r="B42" s="113" t="s">
         <v>26</v>
       </c>
-      <c r="C42" s="106"/>
+      <c r="C42" s="113"/>
       <c r="D42" s="2">
         <f t="shared" ref="D42:R42" si="21">SUM(D6,D10,D14,D34,D38,D18,D22,D26,D30)</f>
         <v>38</v>
@@ -8989,10 +8988,10 @@
       </c>
     </row>
     <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="82" t="s">
+      <c r="A44" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="B44" s="97">
+      <c r="B44" s="96">
         <v>12</v>
       </c>
       <c r="C44" s="10" t="s">
@@ -9060,8 +9059,8 @@
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A45" s="83"/>
-      <c r="B45" s="98"/>
+      <c r="A45" s="84"/>
+      <c r="B45" s="97"/>
       <c r="C45" s="45" t="s">
         <v>16</v>
       </c>
@@ -9085,8 +9084,8 @@
       <c r="R45" s="36"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A46" s="83"/>
-      <c r="B46" s="98"/>
+      <c r="A46" s="84"/>
+      <c r="B46" s="97"/>
       <c r="C46" s="45" t="s">
         <v>17</v>
       </c>
@@ -9110,8 +9109,8 @@
       <c r="R46" s="37"/>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A47" s="83"/>
-      <c r="B47" s="99"/>
+      <c r="A47" s="84"/>
+      <c r="B47" s="98"/>
       <c r="C47" s="46" t="s">
         <v>18</v>
       </c>
@@ -9163,8 +9162,8 @@
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A48" s="83"/>
-      <c r="B48" s="110">
+      <c r="A48" s="84"/>
+      <c r="B48" s="106">
         <v>15</v>
       </c>
       <c r="C48" s="47" t="s">
@@ -9232,8 +9231,8 @@
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="83"/>
-      <c r="B49" s="111"/>
+      <c r="A49" s="84"/>
+      <c r="B49" s="107"/>
       <c r="C49" s="45" t="s">
         <v>16</v>
       </c>
@@ -9257,8 +9256,8 @@
       <c r="R49" s="37"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A50" s="83"/>
-      <c r="B50" s="111"/>
+      <c r="A50" s="84"/>
+      <c r="B50" s="107"/>
       <c r="C50" s="45" t="s">
         <v>17</v>
       </c>
@@ -9282,8 +9281,8 @@
       <c r="R50" s="36"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" s="83"/>
-      <c r="B51" s="112"/>
+      <c r="A51" s="84"/>
+      <c r="B51" s="108"/>
       <c r="C51" s="46" t="s">
         <v>18</v>
       </c>
@@ -9338,8 +9337,8 @@
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" s="83"/>
-      <c r="B52" s="110">
+      <c r="A52" s="84"/>
+      <c r="B52" s="106">
         <v>21</v>
       </c>
       <c r="C52" s="60" t="s">
@@ -9407,8 +9406,8 @@
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A53" s="83"/>
-      <c r="B53" s="111"/>
+      <c r="A53" s="84"/>
+      <c r="B53" s="107"/>
       <c r="C53" s="45" t="s">
         <v>16</v>
       </c>
@@ -9460,8 +9459,8 @@
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A54" s="83"/>
-      <c r="B54" s="111"/>
+      <c r="A54" s="84"/>
+      <c r="B54" s="107"/>
       <c r="C54" s="45" t="s">
         <v>17</v>
       </c>
@@ -9485,8 +9484,8 @@
       <c r="R54" s="37"/>
     </row>
     <row r="55" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="83"/>
-      <c r="B55" s="112"/>
+      <c r="A55" s="84"/>
+      <c r="B55" s="108"/>
       <c r="C55" s="46" t="s">
         <v>18</v>
       </c>
@@ -9510,8 +9509,8 @@
       <c r="R55" s="39"/>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A56" s="83"/>
-      <c r="B56" s="110">
+      <c r="A56" s="84"/>
+      <c r="B56" s="106">
         <v>18</v>
       </c>
       <c r="C56" s="60" t="s">
@@ -9579,8 +9578,8 @@
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A57" s="83"/>
-      <c r="B57" s="111"/>
+      <c r="A57" s="84"/>
+      <c r="B57" s="107"/>
       <c r="C57" s="45" t="s">
         <v>16</v>
       </c>
@@ -9632,8 +9631,8 @@
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A58" s="83"/>
-      <c r="B58" s="111"/>
+      <c r="A58" s="84"/>
+      <c r="B58" s="107"/>
       <c r="C58" s="45" t="s">
         <v>17</v>
       </c>
@@ -9657,8 +9656,8 @@
       <c r="R58" s="37"/>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A59" s="83"/>
-      <c r="B59" s="112"/>
+      <c r="A59" s="84"/>
+      <c r="B59" s="108"/>
       <c r="C59" s="46" t="s">
         <v>18</v>
       </c>
@@ -9682,8 +9681,8 @@
       <c r="R59" s="38"/>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A60" s="83"/>
-      <c r="B60" s="102" t="s">
+      <c r="A60" s="84"/>
+      <c r="B60" s="109" t="s">
         <v>42</v>
       </c>
       <c r="C60" s="60" t="s">
@@ -9751,8 +9750,8 @@
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A61" s="83"/>
-      <c r="B61" s="103"/>
+      <c r="A61" s="84"/>
+      <c r="B61" s="110"/>
       <c r="C61" s="45" t="s">
         <v>16</v>
       </c>
@@ -9776,8 +9775,8 @@
       <c r="R61" s="37"/>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A62" s="83"/>
-      <c r="B62" s="103"/>
+      <c r="A62" s="84"/>
+      <c r="B62" s="110"/>
       <c r="C62" s="45" t="s">
         <v>17</v>
       </c>
@@ -9829,8 +9828,8 @@
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A63" s="83"/>
-      <c r="B63" s="104"/>
+      <c r="A63" s="84"/>
+      <c r="B63" s="111"/>
       <c r="C63" s="46" t="s">
         <v>18</v>
       </c>
@@ -9854,8 +9853,8 @@
       <c r="R63" s="39"/>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A64" s="83"/>
-      <c r="B64" s="102" t="s">
+      <c r="A64" s="84"/>
+      <c r="B64" s="109" t="s">
         <v>45</v>
       </c>
       <c r="C64" s="60" t="s">
@@ -9923,8 +9922,8 @@
       </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A65" s="83"/>
-      <c r="B65" s="103"/>
+      <c r="A65" s="84"/>
+      <c r="B65" s="110"/>
       <c r="C65" s="45" t="s">
         <v>16</v>
       </c>
@@ -9948,8 +9947,8 @@
       <c r="R65" s="37"/>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A66" s="83"/>
-      <c r="B66" s="103"/>
+      <c r="A66" s="84"/>
+      <c r="B66" s="110"/>
       <c r="C66" s="45" t="s">
         <v>17</v>
       </c>
@@ -10001,8 +10000,8 @@
       </c>
     </row>
     <row r="67" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="83"/>
-      <c r="B67" s="104"/>
+      <c r="A67" s="84"/>
+      <c r="B67" s="111"/>
       <c r="C67" s="46" t="s">
         <v>18</v>
       </c>
@@ -10026,8 +10025,8 @@
       <c r="R67" s="39"/>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A68" s="83"/>
-      <c r="B68" s="102">
+      <c r="A68" s="84"/>
+      <c r="B68" s="109">
         <v>31</v>
       </c>
       <c r="C68" s="60" t="s">
@@ -10095,8 +10094,8 @@
       </c>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A69" s="83"/>
-      <c r="B69" s="103"/>
+      <c r="A69" s="84"/>
+      <c r="B69" s="110"/>
       <c r="C69" s="45" t="s">
         <v>16</v>
       </c>
@@ -10120,8 +10119,8 @@
       <c r="R69" s="37"/>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A70" s="83"/>
-      <c r="B70" s="103"/>
+      <c r="A70" s="84"/>
+      <c r="B70" s="110"/>
       <c r="C70" s="45" t="s">
         <v>17</v>
       </c>
@@ -10173,8 +10172,8 @@
       </c>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A71" s="84"/>
-      <c r="B71" s="104"/>
+      <c r="A71" s="85"/>
+      <c r="B71" s="111"/>
       <c r="C71" s="46" t="s">
         <v>18</v>
       </c>
@@ -10198,10 +10197,10 @@
       <c r="R71" s="39"/>
     </row>
     <row r="72" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="82" t="s">
+      <c r="A72" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="B72" s="97"/>
+      <c r="B72" s="96"/>
       <c r="C72" s="10" t="s">
         <v>39</v>
       </c>
@@ -10267,8 +10266,8 @@
       </c>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A73" s="83"/>
-      <c r="B73" s="98"/>
+      <c r="A73" s="84"/>
+      <c r="B73" s="97"/>
       <c r="C73" s="45" t="s">
         <v>16</v>
       </c>
@@ -10292,8 +10291,8 @@
       <c r="R73" s="36"/>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A74" s="83"/>
-      <c r="B74" s="98"/>
+      <c r="A74" s="84"/>
+      <c r="B74" s="97"/>
       <c r="C74" s="45" t="s">
         <v>17</v>
       </c>
@@ -10345,8 +10344,8 @@
       </c>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A75" s="83"/>
-      <c r="B75" s="99"/>
+      <c r="A75" s="84"/>
+      <c r="B75" s="98"/>
       <c r="C75" s="45" t="s">
         <v>18</v>
       </c>
@@ -10370,8 +10369,8 @@
       <c r="R75" s="38"/>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A76" s="83"/>
-      <c r="B76" s="107"/>
+      <c r="A76" s="84"/>
+      <c r="B76" s="103"/>
       <c r="C76" s="10" t="s">
         <v>40</v>
       </c>
@@ -10437,8 +10436,8 @@
       </c>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A77" s="83"/>
-      <c r="B77" s="108"/>
+      <c r="A77" s="84"/>
+      <c r="B77" s="104"/>
       <c r="C77" s="45" t="s">
         <v>16</v>
       </c>
@@ -10462,8 +10461,8 @@
       <c r="R77" s="37"/>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A78" s="83"/>
-      <c r="B78" s="108"/>
+      <c r="A78" s="84"/>
+      <c r="B78" s="104"/>
       <c r="C78" s="45" t="s">
         <v>17</v>
       </c>
@@ -10515,8 +10514,8 @@
       </c>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A79" s="84"/>
-      <c r="B79" s="109"/>
+      <c r="A79" s="85"/>
+      <c r="B79" s="105"/>
       <c r="C79" s="46" t="s">
         <v>18</v>
       </c>
@@ -10540,10 +10539,10 @@
       <c r="R79" s="39"/>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B80" s="105" t="s">
+      <c r="B80" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="C80" s="105"/>
+      <c r="C80" s="112"/>
       <c r="D80" s="2">
         <f t="shared" ref="D80:M80" si="41">SUM(D44,D64,D68,D72,D76)</f>
         <v>17.5</v>
@@ -10669,6 +10668,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="E2:K2"/>
+    <mergeCell ref="L2:R2"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="B68:B71"/>
     <mergeCell ref="A72:A79"/>
     <mergeCell ref="B34:B37"/>
     <mergeCell ref="B38:B41"/>
@@ -10685,16 +10694,6 @@
     <mergeCell ref="B48:B51"/>
     <mergeCell ref="B52:B55"/>
     <mergeCell ref="B64:B67"/>
-    <mergeCell ref="E2:K2"/>
-    <mergeCell ref="L2:R2"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="B68:B71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -10731,24 +10730,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E2" s="89" t="s">
+      <c r="E2" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="89" t="s">
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
-      <c r="P2" s="90"/>
-      <c r="Q2" s="90"/>
-      <c r="R2" s="91"/>
+      <c r="M2" s="91"/>
+      <c r="N2" s="91"/>
+      <c r="O2" s="91"/>
+      <c r="P2" s="91"/>
+      <c r="Q2" s="91"/>
+      <c r="R2" s="92"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D3" s="5" t="s">
@@ -10873,10 +10872,10 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="97">
+      <c r="B6" s="96">
         <v>28</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -10948,8 +10947,8 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="83"/>
-      <c r="B7" s="98"/>
+      <c r="A7" s="84"/>
+      <c r="B7" s="97"/>
       <c r="C7" s="66" t="s">
         <v>16</v>
       </c>
@@ -10978,8 +10977,8 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="83"/>
-      <c r="B8" s="98"/>
+      <c r="A8" s="84"/>
+      <c r="B8" s="97"/>
       <c r="C8" s="66" t="s">
         <v>17</v>
       </c>
@@ -11004,8 +11003,8 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="83"/>
-      <c r="B9" s="99"/>
+      <c r="A9" s="84"/>
+      <c r="B9" s="98"/>
       <c r="C9" s="46" t="s">
         <v>18</v>
       </c>
@@ -11030,8 +11029,8 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="83"/>
-      <c r="B10" s="110">
+      <c r="A10" s="84"/>
+      <c r="B10" s="106">
         <v>16</v>
       </c>
       <c r="C10" s="47" t="s">
@@ -11103,8 +11102,8 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="83"/>
-      <c r="B11" s="111"/>
+      <c r="A11" s="84"/>
+      <c r="B11" s="107"/>
       <c r="C11" s="66" t="s">
         <v>16</v>
       </c>
@@ -11133,8 +11132,8 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="83"/>
-      <c r="B12" s="111"/>
+      <c r="A12" s="84"/>
+      <c r="B12" s="107"/>
       <c r="C12" s="66" t="s">
         <v>17</v>
       </c>
@@ -11159,8 +11158,8 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="83"/>
-      <c r="B13" s="112"/>
+      <c r="A13" s="84"/>
+      <c r="B13" s="108"/>
       <c r="C13" s="46" t="s">
         <v>18</v>
       </c>
@@ -11185,8 +11184,8 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="83"/>
-      <c r="B14" s="110">
+      <c r="A14" s="84"/>
+      <c r="B14" s="106">
         <v>9</v>
       </c>
       <c r="C14" s="60" t="s">
@@ -11258,8 +11257,8 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="83"/>
-      <c r="B15" s="111"/>
+      <c r="A15" s="84"/>
+      <c r="B15" s="107"/>
       <c r="C15" s="66" t="s">
         <v>16</v>
       </c>
@@ -11288,8 +11287,8 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="83"/>
-      <c r="B16" s="111"/>
+      <c r="A16" s="84"/>
+      <c r="B16" s="107"/>
       <c r="C16" s="66" t="s">
         <v>17</v>
       </c>
@@ -11318,8 +11317,8 @@
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="83"/>
-      <c r="B17" s="112"/>
+      <c r="A17" s="84"/>
+      <c r="B17" s="108"/>
       <c r="C17" s="46" t="s">
         <v>18</v>
       </c>
@@ -11344,8 +11343,8 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="83"/>
-      <c r="B18" s="110" t="s">
+      <c r="A18" s="84"/>
+      <c r="B18" s="106" t="s">
         <v>56</v>
       </c>
       <c r="C18" s="10" t="s">
@@ -11417,8 +11416,8 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="83"/>
-      <c r="B19" s="111"/>
+      <c r="A19" s="84"/>
+      <c r="B19" s="107"/>
       <c r="C19" s="66" t="s">
         <v>16</v>
       </c>
@@ -11443,8 +11442,8 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="83"/>
-      <c r="B20" s="111"/>
+      <c r="A20" s="84"/>
+      <c r="B20" s="107"/>
       <c r="C20" s="66" t="s">
         <v>17</v>
       </c>
@@ -11469,8 +11468,8 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="83"/>
-      <c r="B21" s="112"/>
+      <c r="A21" s="84"/>
+      <c r="B21" s="108"/>
       <c r="C21" s="46" t="s">
         <v>18</v>
       </c>
@@ -11499,8 +11498,8 @@
       </c>
     </row>
     <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="83"/>
-      <c r="B22" s="97" t="s">
+      <c r="A22" s="84"/>
+      <c r="B22" s="96" t="s">
         <v>57</v>
       </c>
       <c r="C22" s="10" t="s">
@@ -11572,8 +11571,8 @@
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="83"/>
-      <c r="B23" s="98"/>
+      <c r="A23" s="84"/>
+      <c r="B23" s="97"/>
       <c r="C23" s="66" t="s">
         <v>16</v>
       </c>
@@ -11602,8 +11601,8 @@
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="83"/>
-      <c r="B24" s="98"/>
+      <c r="A24" s="84"/>
+      <c r="B24" s="97"/>
       <c r="C24" s="66" t="s">
         <v>17</v>
       </c>
@@ -11632,8 +11631,8 @@
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="83"/>
-      <c r="B25" s="99"/>
+      <c r="A25" s="84"/>
+      <c r="B25" s="98"/>
       <c r="C25" s="46" t="s">
         <v>18</v>
       </c>
@@ -11658,7 +11657,7 @@
       </c>
     </row>
     <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="82" t="s">
+      <c r="A26" s="83" t="s">
         <v>23</v>
       </c>
       <c r="B26" s="63"/>
@@ -11731,7 +11730,7 @@
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="83"/>
+      <c r="A27" s="84"/>
       <c r="B27" s="64"/>
       <c r="C27" s="66" t="s">
         <v>16</v>
@@ -11761,7 +11760,7 @@
       </c>
     </row>
     <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="83"/>
+      <c r="A28" s="84"/>
       <c r="B28" s="64"/>
       <c r="C28" s="66" t="s">
         <v>17</v>
@@ -11787,7 +11786,7 @@
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="83"/>
+      <c r="A29" s="84"/>
       <c r="B29" s="65"/>
       <c r="C29" s="46" t="s">
         <v>18</v>
@@ -11813,8 +11812,8 @@
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="83"/>
-      <c r="B30" s="102"/>
+      <c r="A30" s="84"/>
+      <c r="B30" s="109"/>
       <c r="C30" s="60" t="s">
         <v>52</v>
       </c>
@@ -11884,8 +11883,8 @@
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="83"/>
-      <c r="B31" s="103"/>
+      <c r="A31" s="84"/>
+      <c r="B31" s="110"/>
       <c r="C31" s="66" t="s">
         <v>16</v>
       </c>
@@ -11914,8 +11913,8 @@
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="83"/>
-      <c r="B32" s="103"/>
+      <c r="A32" s="84"/>
+      <c r="B32" s="110"/>
       <c r="C32" s="66" t="s">
         <v>17</v>
       </c>
@@ -11940,8 +11939,8 @@
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" s="83"/>
-      <c r="B33" s="104"/>
+      <c r="A33" s="84"/>
+      <c r="B33" s="111"/>
       <c r="C33" s="46" t="s">
         <v>18</v>
       </c>
@@ -11966,8 +11965,8 @@
       </c>
     </row>
     <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="83"/>
-      <c r="B34" s="92"/>
+      <c r="A34" s="84"/>
+      <c r="B34" s="93"/>
       <c r="C34" s="60" t="s">
         <v>58</v>
       </c>
@@ -12037,8 +12036,8 @@
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="83"/>
-      <c r="B35" s="93"/>
+      <c r="A35" s="84"/>
+      <c r="B35" s="94"/>
       <c r="C35" s="66" t="s">
         <v>16</v>
       </c>
@@ -12067,8 +12066,8 @@
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A36" s="83"/>
-      <c r="B36" s="93"/>
+      <c r="A36" s="84"/>
+      <c r="B36" s="94"/>
       <c r="C36" s="66" t="s">
         <v>17</v>
       </c>
@@ -12097,8 +12096,8 @@
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="83"/>
-      <c r="B37" s="93"/>
+      <c r="A37" s="84"/>
+      <c r="B37" s="94"/>
       <c r="C37" s="66" t="s">
         <v>18</v>
       </c>
@@ -12123,8 +12122,8 @@
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A38" s="83"/>
-      <c r="B38" s="102"/>
+      <c r="A38" s="84"/>
+      <c r="B38" s="109"/>
       <c r="C38" s="60" t="s">
         <v>53</v>
       </c>
@@ -12194,8 +12193,8 @@
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A39" s="83"/>
-      <c r="B39" s="103"/>
+      <c r="A39" s="84"/>
+      <c r="B39" s="110"/>
       <c r="C39" s="66" t="s">
         <v>16</v>
       </c>
@@ -12224,8 +12223,8 @@
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A40" s="83"/>
-      <c r="B40" s="103"/>
+      <c r="A40" s="84"/>
+      <c r="B40" s="110"/>
       <c r="C40" s="66" t="s">
         <v>17</v>
       </c>
@@ -12250,8 +12249,8 @@
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A41" s="83"/>
-      <c r="B41" s="104"/>
+      <c r="A41" s="84"/>
+      <c r="B41" s="111"/>
       <c r="C41" s="46" t="s">
         <v>18</v>
       </c>
@@ -12276,8 +12275,8 @@
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A42" s="83"/>
-      <c r="B42" s="102"/>
+      <c r="A42" s="84"/>
+      <c r="B42" s="109"/>
       <c r="C42" s="60" t="s">
         <v>60</v>
       </c>
@@ -12347,8 +12346,8 @@
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A43" s="83"/>
-      <c r="B43" s="103"/>
+      <c r="A43" s="84"/>
+      <c r="B43" s="110"/>
       <c r="C43" s="66" t="s">
         <v>16</v>
       </c>
@@ -12373,8 +12372,8 @@
       </c>
     </row>
     <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="83"/>
-      <c r="B44" s="103"/>
+      <c r="A44" s="84"/>
+      <c r="B44" s="110"/>
       <c r="C44" s="66" t="s">
         <v>17</v>
       </c>
@@ -12405,8 +12404,8 @@
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A45" s="83"/>
-      <c r="B45" s="104"/>
+      <c r="A45" s="84"/>
+      <c r="B45" s="111"/>
       <c r="C45" s="46" t="s">
         <v>18</v>
       </c>
@@ -12431,8 +12430,8 @@
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A46" s="83"/>
-      <c r="B46" s="102"/>
+      <c r="A46" s="84"/>
+      <c r="B46" s="109"/>
       <c r="C46" s="60" t="s">
         <v>59</v>
       </c>
@@ -12502,8 +12501,8 @@
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A47" s="83"/>
-      <c r="B47" s="103"/>
+      <c r="A47" s="84"/>
+      <c r="B47" s="110"/>
       <c r="C47" s="66" t="s">
         <v>16</v>
       </c>
@@ -12532,8 +12531,8 @@
       </c>
     </row>
     <row r="48" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="83"/>
-      <c r="B48" s="103"/>
+      <c r="A48" s="84"/>
+      <c r="B48" s="110"/>
       <c r="C48" s="66" t="s">
         <v>17</v>
       </c>
@@ -12558,8 +12557,8 @@
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A49" s="84"/>
-      <c r="B49" s="104"/>
+      <c r="A49" s="85"/>
+      <c r="B49" s="111"/>
       <c r="C49" s="46" t="s">
         <v>18</v>
       </c>
@@ -12585,10 +12584,10 @@
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="75"/>
-      <c r="B50" s="106" t="s">
+      <c r="B50" s="113" t="s">
         <v>26</v>
       </c>
-      <c r="C50" s="106"/>
+      <c r="C50" s="113"/>
       <c r="D50" s="2">
         <f>SUM(D6,D10,D14,D34,D38,D18,D22,D26,D30,D42,D46)</f>
         <v>44</v>
@@ -12656,10 +12655,10 @@
     </row>
     <row r="51" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="52" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="82" t="s">
+      <c r="A52" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="B52" s="97">
+      <c r="B52" s="96">
         <v>28</v>
       </c>
       <c r="C52" s="10" t="s">
@@ -12727,8 +12726,8 @@
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A53" s="83"/>
-      <c r="B53" s="98"/>
+      <c r="A53" s="84"/>
+      <c r="B53" s="97"/>
       <c r="C53" s="70" t="s">
         <v>16</v>
       </c>
@@ -12780,8 +12779,8 @@
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A54" s="83"/>
-      <c r="B54" s="98"/>
+      <c r="A54" s="84"/>
+      <c r="B54" s="97"/>
       <c r="C54" s="70" t="s">
         <v>17</v>
       </c>
@@ -12805,8 +12804,8 @@
       <c r="R54" s="37"/>
     </row>
     <row r="55" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="83"/>
-      <c r="B55" s="99"/>
+      <c r="A55" s="84"/>
+      <c r="B55" s="98"/>
       <c r="C55" s="46" t="s">
         <v>18</v>
       </c>
@@ -12830,8 +12829,8 @@
       <c r="R55" s="36"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A56" s="83"/>
-      <c r="B56" s="110">
+      <c r="A56" s="84"/>
+      <c r="B56" s="106">
         <v>16</v>
       </c>
       <c r="C56" s="47" t="s">
@@ -12899,8 +12898,8 @@
       </c>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A57" s="83"/>
-      <c r="B57" s="111"/>
+      <c r="A57" s="84"/>
+      <c r="B57" s="107"/>
       <c r="C57" s="70" t="s">
         <v>16</v>
       </c>
@@ -12952,8 +12951,8 @@
       </c>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A58" s="83"/>
-      <c r="B58" s="111"/>
+      <c r="A58" s="84"/>
+      <c r="B58" s="107"/>
       <c r="C58" s="70" t="s">
         <v>17</v>
       </c>
@@ -12977,8 +12976,8 @@
       <c r="R58" s="36"/>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A59" s="83"/>
-      <c r="B59" s="112"/>
+      <c r="A59" s="84"/>
+      <c r="B59" s="108"/>
       <c r="C59" s="46" t="s">
         <v>18</v>
       </c>
@@ -13002,8 +13001,8 @@
       <c r="R59" s="39"/>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A60" s="83"/>
-      <c r="B60" s="110">
+      <c r="A60" s="84"/>
+      <c r="B60" s="106">
         <v>9</v>
       </c>
       <c r="C60" s="60" t="s">
@@ -13071,8 +13070,8 @@
       </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A61" s="83"/>
-      <c r="B61" s="111"/>
+      <c r="A61" s="84"/>
+      <c r="B61" s="107"/>
       <c r="C61" s="70" t="s">
         <v>16</v>
       </c>
@@ -13124,8 +13123,8 @@
       </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A62" s="83"/>
-      <c r="B62" s="111"/>
+      <c r="A62" s="84"/>
+      <c r="B62" s="107"/>
       <c r="C62" s="70" t="s">
         <v>17</v>
       </c>
@@ -13177,8 +13176,8 @@
       </c>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A63" s="83"/>
-      <c r="B63" s="112"/>
+      <c r="A63" s="84"/>
+      <c r="B63" s="108"/>
       <c r="C63" s="46" t="s">
         <v>18</v>
       </c>
@@ -13202,8 +13201,8 @@
       <c r="R63" s="39"/>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A64" s="83"/>
-      <c r="B64" s="110" t="s">
+      <c r="A64" s="84"/>
+      <c r="B64" s="106" t="s">
         <v>56</v>
       </c>
       <c r="C64" s="10" t="s">
@@ -13271,8 +13270,8 @@
       </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A65" s="83"/>
-      <c r="B65" s="111"/>
+      <c r="A65" s="84"/>
+      <c r="B65" s="107"/>
       <c r="C65" s="70" t="s">
         <v>16</v>
       </c>
@@ -13296,8 +13295,8 @@
       <c r="R65" s="36"/>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A66" s="83"/>
-      <c r="B66" s="111"/>
+      <c r="A66" s="84"/>
+      <c r="B66" s="107"/>
       <c r="C66" s="70" t="s">
         <v>17</v>
       </c>
@@ -13321,8 +13320,8 @@
       <c r="R66" s="37"/>
     </row>
     <row r="67" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="83"/>
-      <c r="B67" s="112"/>
+      <c r="A67" s="84"/>
+      <c r="B67" s="108"/>
       <c r="C67" s="46" t="s">
         <v>18</v>
       </c>
@@ -13374,8 +13373,8 @@
       </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A68" s="83"/>
-      <c r="B68" s="97" t="s">
+      <c r="A68" s="84"/>
+      <c r="B68" s="96" t="s">
         <v>57</v>
       </c>
       <c r="C68" s="10" t="s">
@@ -13443,8 +13442,8 @@
       </c>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A69" s="83"/>
-      <c r="B69" s="98"/>
+      <c r="A69" s="84"/>
+      <c r="B69" s="97"/>
       <c r="C69" s="70" t="s">
         <v>16</v>
       </c>
@@ -13496,8 +13495,8 @@
       </c>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A70" s="83"/>
-      <c r="B70" s="98"/>
+      <c r="A70" s="84"/>
+      <c r="B70" s="97"/>
       <c r="C70" s="70" t="s">
         <v>17</v>
       </c>
@@ -13549,8 +13548,8 @@
       </c>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A71" s="84"/>
-      <c r="B71" s="99"/>
+      <c r="A71" s="85"/>
+      <c r="B71" s="98"/>
       <c r="C71" s="46" t="s">
         <v>18</v>
       </c>
@@ -13574,7 +13573,7 @@
       <c r="R71" s="39"/>
     </row>
     <row r="72" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="113" t="s">
+      <c r="A72" s="114" t="s">
         <v>23</v>
       </c>
       <c r="B72" s="67"/>
@@ -13643,7 +13642,7 @@
       </c>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A73" s="114"/>
+      <c r="A73" s="115"/>
       <c r="B73" s="68"/>
       <c r="C73" s="70" t="s">
         <v>16</v>
@@ -13696,7 +13695,7 @@
       </c>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A74" s="114"/>
+      <c r="A74" s="115"/>
       <c r="B74" s="68"/>
       <c r="C74" s="70" t="s">
         <v>17</v>
@@ -13721,7 +13720,7 @@
       <c r="R74" s="36"/>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A75" s="114"/>
+      <c r="A75" s="115"/>
       <c r="B75" s="69"/>
       <c r="C75" s="46" t="s">
         <v>18</v>
@@ -13746,8 +13745,8 @@
       <c r="R75" s="39"/>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A76" s="114"/>
-      <c r="B76" s="102"/>
+      <c r="A76" s="115"/>
+      <c r="B76" s="109"/>
       <c r="C76" s="60" t="s">
         <v>52</v>
       </c>
@@ -13813,8 +13812,8 @@
       </c>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A77" s="114"/>
-      <c r="B77" s="103"/>
+      <c r="A77" s="115"/>
+      <c r="B77" s="110"/>
       <c r="C77" s="70" t="s">
         <v>16</v>
       </c>
@@ -13866,8 +13865,8 @@
       </c>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A78" s="114"/>
-      <c r="B78" s="103"/>
+      <c r="A78" s="115"/>
+      <c r="B78" s="110"/>
       <c r="C78" s="70" t="s">
         <v>17</v>
       </c>
@@ -13891,8 +13890,8 @@
       <c r="R78" s="36"/>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A79" s="114"/>
-      <c r="B79" s="104"/>
+      <c r="A79" s="115"/>
+      <c r="B79" s="111"/>
       <c r="C79" s="46" t="s">
         <v>18</v>
       </c>
@@ -13916,8 +13915,8 @@
       <c r="R79" s="39"/>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A80" s="114"/>
-      <c r="B80" s="97"/>
+      <c r="A80" s="115"/>
+      <c r="B80" s="96"/>
       <c r="C80" s="60" t="s">
         <v>58</v>
       </c>
@@ -13983,8 +13982,8 @@
       </c>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A81" s="114"/>
-      <c r="B81" s="98"/>
+      <c r="A81" s="115"/>
+      <c r="B81" s="97"/>
       <c r="C81" s="70" t="s">
         <v>16</v>
       </c>
@@ -14036,8 +14035,8 @@
       </c>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A82" s="114"/>
-      <c r="B82" s="98"/>
+      <c r="A82" s="115"/>
+      <c r="B82" s="97"/>
       <c r="C82" s="70" t="s">
         <v>17</v>
       </c>
@@ -14089,8 +14088,8 @@
       </c>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A83" s="114"/>
-      <c r="B83" s="99"/>
+      <c r="A83" s="115"/>
+      <c r="B83" s="98"/>
       <c r="C83" s="46" t="s">
         <v>18</v>
       </c>
@@ -14114,8 +14113,8 @@
       <c r="R83" s="38"/>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A84" s="114"/>
-      <c r="B84" s="102"/>
+      <c r="A84" s="115"/>
+      <c r="B84" s="109"/>
       <c r="C84" s="60" t="s">
         <v>53</v>
       </c>
@@ -14181,8 +14180,8 @@
       </c>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A85" s="114"/>
-      <c r="B85" s="103"/>
+      <c r="A85" s="115"/>
+      <c r="B85" s="110"/>
       <c r="C85" s="70" t="s">
         <v>16</v>
       </c>
@@ -14234,8 +14233,8 @@
       </c>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A86" s="114"/>
-      <c r="B86" s="103"/>
+      <c r="A86" s="115"/>
+      <c r="B86" s="110"/>
       <c r="C86" s="70" t="s">
         <v>17</v>
       </c>
@@ -14287,8 +14286,8 @@
       </c>
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A87" s="114"/>
-      <c r="B87" s="104"/>
+      <c r="A87" s="115"/>
+      <c r="B87" s="111"/>
       <c r="C87" s="46" t="s">
         <v>18</v>
       </c>
@@ -14312,8 +14311,8 @@
       <c r="R87" s="39"/>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A88" s="114"/>
-      <c r="B88" s="102"/>
+      <c r="A88" s="115"/>
+      <c r="B88" s="109"/>
       <c r="C88" s="60" t="s">
         <v>60</v>
       </c>
@@ -14379,8 +14378,8 @@
       </c>
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A89" s="114"/>
-      <c r="B89" s="103"/>
+      <c r="A89" s="115"/>
+      <c r="B89" s="110"/>
       <c r="C89" s="70" t="s">
         <v>16</v>
       </c>
@@ -14404,8 +14403,8 @@
       <c r="R89" s="37"/>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A90" s="114"/>
-      <c r="B90" s="103"/>
+      <c r="A90" s="115"/>
+      <c r="B90" s="110"/>
       <c r="C90" s="70" t="s">
         <v>17</v>
       </c>
@@ -14457,8 +14456,8 @@
       </c>
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A91" s="114"/>
-      <c r="B91" s="104"/>
+      <c r="A91" s="115"/>
+      <c r="B91" s="111"/>
       <c r="C91" s="46" t="s">
         <v>18</v>
       </c>
@@ -14482,8 +14481,8 @@
       <c r="R91" s="39"/>
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A92" s="114"/>
-      <c r="B92" s="102"/>
+      <c r="A92" s="115"/>
+      <c r="B92" s="109"/>
       <c r="C92" s="60" t="s">
         <v>59</v>
       </c>
@@ -14549,8 +14548,8 @@
       </c>
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A93" s="114"/>
-      <c r="B93" s="103"/>
+      <c r="A93" s="115"/>
+      <c r="B93" s="110"/>
       <c r="C93" s="70" t="s">
         <v>16</v>
       </c>
@@ -14602,8 +14601,8 @@
       </c>
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A94" s="114"/>
-      <c r="B94" s="103"/>
+      <c r="A94" s="115"/>
+      <c r="B94" s="110"/>
       <c r="C94" s="70" t="s">
         <v>17</v>
       </c>
@@ -14655,8 +14654,8 @@
       </c>
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A95" s="114"/>
-      <c r="B95" s="104"/>
+      <c r="A95" s="115"/>
+      <c r="B95" s="111"/>
       <c r="C95" s="46" t="s">
         <v>18</v>
       </c>
@@ -14680,10 +14679,10 @@
       <c r="R95" s="39"/>
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B96" s="105" t="s">
+      <c r="B96" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="C96" s="105"/>
+      <c r="C96" s="112"/>
       <c r="D96" s="2">
         <f>SUM(D52,D56,D60,D64,D68,D72,D76,D80,D84,D88,D92)</f>
         <v>44</v>
@@ -14809,18 +14808,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B92:B95"/>
-    <mergeCell ref="A72:A95"/>
-    <mergeCell ref="A52:A71"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="E2:K2"/>
-    <mergeCell ref="B84:B87"/>
-    <mergeCell ref="B88:B91"/>
-    <mergeCell ref="A6:A25"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="A26:A49"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="B18:B21"/>
     <mergeCell ref="L2:R2"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="B10:B13"/>
@@ -14837,6 +14824,18 @@
     <mergeCell ref="B38:B41"/>
     <mergeCell ref="B30:B33"/>
     <mergeCell ref="B42:B45"/>
+    <mergeCell ref="B92:B95"/>
+    <mergeCell ref="A72:A95"/>
+    <mergeCell ref="A52:A71"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="E2:K2"/>
+    <mergeCell ref="B84:B87"/>
+    <mergeCell ref="B88:B91"/>
+    <mergeCell ref="A6:A25"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="A26:A49"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="B18:B21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -14870,24 +14869,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E2" s="89" t="s">
+      <c r="E2" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="89" t="s">
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
-      <c r="P2" s="90"/>
-      <c r="Q2" s="90"/>
-      <c r="R2" s="91"/>
+      <c r="M2" s="91"/>
+      <c r="N2" s="91"/>
+      <c r="O2" s="91"/>
+      <c r="P2" s="91"/>
+      <c r="Q2" s="91"/>
+      <c r="R2" s="92"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D3" s="5" t="s">
@@ -15012,10 +15011,10 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="115" t="s">
+      <c r="B6" s="116" t="s">
         <v>62</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -15087,8 +15086,8 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="83"/>
-      <c r="B7" s="116"/>
+      <c r="A7" s="84"/>
+      <c r="B7" s="117"/>
       <c r="C7" s="70" t="s">
         <v>16</v>
       </c>
@@ -15117,8 +15116,8 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="83"/>
-      <c r="B8" s="116"/>
+      <c r="A8" s="84"/>
+      <c r="B8" s="117"/>
       <c r="C8" s="70" t="s">
         <v>17</v>
       </c>
@@ -15147,8 +15146,8 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="83"/>
-      <c r="B9" s="117"/>
+      <c r="A9" s="84"/>
+      <c r="B9" s="118"/>
       <c r="C9" s="46" t="s">
         <v>18</v>
       </c>
@@ -15173,8 +15172,8 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="83"/>
-      <c r="B10" s="118">
+      <c r="A10" s="84"/>
+      <c r="B10" s="119">
         <v>26</v>
       </c>
       <c r="C10" s="47" t="s">
@@ -15246,8 +15245,8 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="83"/>
-      <c r="B11" s="119"/>
+      <c r="A11" s="84"/>
+      <c r="B11" s="120"/>
       <c r="C11" s="70" t="s">
         <v>16</v>
       </c>
@@ -15276,8 +15275,8 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="83"/>
-      <c r="B12" s="119"/>
+      <c r="A12" s="84"/>
+      <c r="B12" s="120"/>
       <c r="C12" s="70" t="s">
         <v>17</v>
       </c>
@@ -15306,8 +15305,8 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="83"/>
-      <c r="B13" s="120"/>
+      <c r="A13" s="84"/>
+      <c r="B13" s="121"/>
       <c r="C13" s="46" t="s">
         <v>18</v>
       </c>
@@ -15332,8 +15331,8 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="83"/>
-      <c r="B14" s="118">
+      <c r="A14" s="84"/>
+      <c r="B14" s="119">
         <v>26</v>
       </c>
       <c r="C14" s="60" t="s">
@@ -15405,8 +15404,8 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="83"/>
-      <c r="B15" s="119"/>
+      <c r="A15" s="84"/>
+      <c r="B15" s="120"/>
       <c r="C15" s="70" t="s">
         <v>16</v>
       </c>
@@ -15437,8 +15436,8 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="83"/>
-      <c r="B16" s="119"/>
+      <c r="A16" s="84"/>
+      <c r="B16" s="120"/>
       <c r="C16" s="70" t="s">
         <v>17</v>
       </c>
@@ -15463,8 +15462,8 @@
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="83"/>
-      <c r="B17" s="120"/>
+      <c r="A17" s="84"/>
+      <c r="B17" s="121"/>
       <c r="C17" s="46" t="s">
         <v>18</v>
       </c>
@@ -15497,8 +15496,8 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="83"/>
-      <c r="B18" s="118" t="s">
+      <c r="A18" s="84"/>
+      <c r="B18" s="119" t="s">
         <v>66</v>
       </c>
       <c r="C18" s="10" t="s">
@@ -15570,8 +15569,8 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="83"/>
-      <c r="B19" s="119"/>
+      <c r="A19" s="84"/>
+      <c r="B19" s="120"/>
       <c r="C19" s="70" t="s">
         <v>16</v>
       </c>
@@ -15596,8 +15595,8 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="83"/>
-      <c r="B20" s="119"/>
+      <c r="A20" s="84"/>
+      <c r="B20" s="120"/>
       <c r="C20" s="70" t="s">
         <v>17</v>
       </c>
@@ -15628,8 +15627,8 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="83"/>
-      <c r="B21" s="120"/>
+      <c r="A21" s="84"/>
+      <c r="B21" s="121"/>
       <c r="C21" s="46" t="s">
         <v>18</v>
       </c>
@@ -15654,10 +15653,10 @@
       </c>
     </row>
     <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="82" t="s">
+      <c r="A22" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="115"/>
+      <c r="B22" s="116"/>
       <c r="C22" s="10" t="s">
         <v>67</v>
       </c>
@@ -15727,8 +15726,8 @@
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="83"/>
-      <c r="B23" s="116"/>
+      <c r="A23" s="84"/>
+      <c r="B23" s="117"/>
       <c r="C23" s="70" t="s">
         <v>16</v>
       </c>
@@ -15757,8 +15756,8 @@
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="83"/>
-      <c r="B24" s="116"/>
+      <c r="A24" s="84"/>
+      <c r="B24" s="117"/>
       <c r="C24" s="70" t="s">
         <v>17</v>
       </c>
@@ -15787,8 +15786,8 @@
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="83"/>
-      <c r="B25" s="117"/>
+      <c r="A25" s="84"/>
+      <c r="B25" s="118"/>
       <c r="C25" s="46" t="s">
         <v>18</v>
       </c>
@@ -15819,7 +15818,7 @@
       </c>
     </row>
     <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="83"/>
+      <c r="A26" s="84"/>
       <c r="B26" s="72"/>
       <c r="C26" s="60" t="s">
         <v>68</v>
@@ -15890,7 +15889,7 @@
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="83"/>
+      <c r="A27" s="84"/>
       <c r="B27" s="73"/>
       <c r="C27" s="70" t="s">
         <v>16</v>
@@ -15922,7 +15921,7 @@
       </c>
     </row>
     <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="83"/>
+      <c r="A28" s="84"/>
       <c r="B28" s="73"/>
       <c r="C28" s="70" t="s">
         <v>17</v>
@@ -15954,7 +15953,7 @@
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="84"/>
+      <c r="A29" s="85"/>
       <c r="B29" s="74"/>
       <c r="C29" s="46" t="s">
         <v>18</v>
@@ -15987,10 +15986,10 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="71"/>
-      <c r="B30" s="106" t="s">
+      <c r="B30" s="113" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="106"/>
+      <c r="C30" s="113"/>
       <c r="D30" s="2">
         <f>SUM(D6,D10,D14,D18,D22,D26)</f>
         <v>66</v>
@@ -16058,10 +16057,10 @@
     </row>
     <row r="31" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="82" t="s">
+      <c r="A32" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="115" t="s">
+      <c r="B32" s="116" t="s">
         <v>62</v>
       </c>
       <c r="C32" s="10" t="s">
@@ -16129,8 +16128,8 @@
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="83"/>
-      <c r="B33" s="116"/>
+      <c r="A33" s="84"/>
+      <c r="B33" s="117"/>
       <c r="C33" s="76" t="s">
         <v>16</v>
       </c>
@@ -16181,8 +16180,8 @@
       </c>
     </row>
     <row r="34" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="83"/>
-      <c r="B34" s="116"/>
+      <c r="A34" s="84"/>
+      <c r="B34" s="117"/>
       <c r="C34" s="76" t="s">
         <v>17</v>
       </c>
@@ -16233,8 +16232,8 @@
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="83"/>
-      <c r="B35" s="117"/>
+      <c r="A35" s="84"/>
+      <c r="B35" s="118"/>
       <c r="C35" s="46" t="s">
         <v>18</v>
       </c>
@@ -16255,8 +16254,8 @@
       <c r="R35" s="31"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="83"/>
-      <c r="B36" s="118">
+      <c r="A36" s="84"/>
+      <c r="B36" s="119">
         <v>26</v>
       </c>
       <c r="C36" s="47" t="s">
@@ -16324,8 +16323,8 @@
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="83"/>
-      <c r="B37" s="119"/>
+      <c r="A37" s="84"/>
+      <c r="B37" s="120"/>
       <c r="C37" s="76" t="s">
         <v>16</v>
       </c>
@@ -16383,8 +16382,8 @@
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="83"/>
-      <c r="B38" s="119"/>
+      <c r="A38" s="84"/>
+      <c r="B38" s="120"/>
       <c r="C38" s="76" t="s">
         <v>17</v>
       </c>
@@ -16449,8 +16448,8 @@
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="83"/>
-      <c r="B39" s="120"/>
+      <c r="A39" s="84"/>
+      <c r="B39" s="121"/>
       <c r="C39" s="46" t="s">
         <v>18</v>
       </c>
@@ -16471,8 +16470,8 @@
       <c r="R39" s="39"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="83"/>
-      <c r="B40" s="118">
+      <c r="A40" s="84"/>
+      <c r="B40" s="119">
         <v>26</v>
       </c>
       <c r="C40" s="60" t="s">
@@ -16540,8 +16539,8 @@
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="83"/>
-      <c r="B41" s="119"/>
+      <c r="A41" s="84"/>
+      <c r="B41" s="120"/>
       <c r="C41" s="76" t="s">
         <v>16</v>
       </c>
@@ -16599,8 +16598,8 @@
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="83"/>
-      <c r="B42" s="119"/>
+      <c r="A42" s="84"/>
+      <c r="B42" s="120"/>
       <c r="C42" s="76" t="s">
         <v>17</v>
       </c>
@@ -16623,8 +16622,8 @@
       <c r="R42" s="37"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="83"/>
-      <c r="B43" s="120"/>
+      <c r="A43" s="84"/>
+      <c r="B43" s="121"/>
       <c r="C43" s="46" t="s">
         <v>18</v>
       </c>
@@ -16647,8 +16646,8 @@
       <c r="R43" s="39"/>
     </row>
     <row r="44" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="83"/>
-      <c r="B44" s="118" t="s">
+      <c r="A44" s="84"/>
+      <c r="B44" s="119" t="s">
         <v>66</v>
       </c>
       <c r="C44" s="10" t="s">
@@ -16716,8 +16715,8 @@
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="83"/>
-      <c r="B45" s="119"/>
+      <c r="A45" s="84"/>
+      <c r="B45" s="120"/>
       <c r="C45" s="76" t="s">
         <v>16</v>
       </c>
@@ -16738,8 +16737,8 @@
       <c r="R45" s="31"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="83"/>
-      <c r="B46" s="119"/>
+      <c r="A46" s="84"/>
+      <c r="B46" s="120"/>
       <c r="C46" s="76" t="s">
         <v>17</v>
       </c>
@@ -16790,8 +16789,8 @@
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="83"/>
-      <c r="B47" s="120"/>
+      <c r="A47" s="84"/>
+      <c r="B47" s="121"/>
       <c r="C47" s="46" t="s">
         <v>18</v>
       </c>
@@ -16812,10 +16811,10 @@
       <c r="R47" s="38"/>
     </row>
     <row r="48" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="82" t="s">
+      <c r="A48" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="B48" s="115"/>
+      <c r="B48" s="116"/>
       <c r="C48" s="10" t="s">
         <v>67</v>
       </c>
@@ -16881,8 +16880,8 @@
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="83"/>
-      <c r="B49" s="116"/>
+      <c r="A49" s="84"/>
+      <c r="B49" s="117"/>
       <c r="C49" s="76" t="s">
         <v>16</v>
       </c>
@@ -16933,8 +16932,8 @@
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A50" s="83"/>
-      <c r="B50" s="116"/>
+      <c r="A50" s="84"/>
+      <c r="B50" s="117"/>
       <c r="C50" s="76" t="s">
         <v>17</v>
       </c>
@@ -16985,8 +16984,8 @@
       </c>
     </row>
     <row r="51" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="83"/>
-      <c r="B51" s="117"/>
+      <c r="A51" s="84"/>
+      <c r="B51" s="118"/>
       <c r="C51" s="46" t="s">
         <v>18</v>
       </c>
@@ -17009,7 +17008,7 @@
       <c r="R51" s="39"/>
     </row>
     <row r="52" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="83"/>
+      <c r="A52" s="84"/>
       <c r="B52" s="72"/>
       <c r="C52" s="60" t="s">
         <v>68</v>
@@ -17076,7 +17075,7 @@
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A53" s="83"/>
+      <c r="A53" s="84"/>
       <c r="B53" s="73"/>
       <c r="C53" s="76" t="s">
         <v>16</v>
@@ -17128,7 +17127,7 @@
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A54" s="83"/>
+      <c r="A54" s="84"/>
       <c r="B54" s="73"/>
       <c r="C54" s="76" t="s">
         <v>17</v>
@@ -17180,7 +17179,7 @@
       </c>
     </row>
     <row r="55" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="84"/>
+      <c r="A55" s="85"/>
       <c r="B55" s="74"/>
       <c r="C55" s="46" t="s">
         <v>18</v>
@@ -17206,10 +17205,10 @@
       <c r="R55" s="39"/>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B56" s="105" t="s">
+      <c r="B56" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="C56" s="105"/>
+      <c r="C56" s="112"/>
       <c r="D56" s="2">
         <f>SUM(D32, D36, D40, D44, D48,D52)</f>
         <v>66</v>
@@ -17337,13 +17336,6 @@
     <row r="72" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="B48:B51"/>
     <mergeCell ref="A32:A47"/>
     <mergeCell ref="A48:A55"/>
     <mergeCell ref="A22:A29"/>
@@ -17355,6 +17347,13 @@
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="A6:A21"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="B48:B51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -17366,8 +17365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17389,24 +17388,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E2" s="89" t="s">
+      <c r="E2" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="89" t="s">
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
-      <c r="P2" s="90"/>
-      <c r="Q2" s="90"/>
-      <c r="R2" s="91"/>
+      <c r="M2" s="91"/>
+      <c r="N2" s="91"/>
+      <c r="O2" s="91"/>
+      <c r="P2" s="91"/>
+      <c r="Q2" s="91"/>
+      <c r="R2" s="92"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D3" s="5" t="s">
@@ -17531,10 +17530,10 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="121" t="s">
+      <c r="A6" s="122" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="115" t="s">
+      <c r="B6" s="116" t="s">
         <v>70</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -17606,8 +17605,8 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="122"/>
-      <c r="B7" s="116"/>
+      <c r="A7" s="123"/>
+      <c r="B7" s="117"/>
       <c r="C7" s="77" t="s">
         <v>16</v>
       </c>
@@ -17634,8 +17633,8 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="122"/>
-      <c r="B8" s="116"/>
+      <c r="A8" s="123"/>
+      <c r="B8" s="117"/>
       <c r="C8" s="77" t="s">
         <v>17</v>
       </c>
@@ -17660,8 +17659,8 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="122"/>
-      <c r="B9" s="117"/>
+      <c r="A9" s="123"/>
+      <c r="B9" s="118"/>
       <c r="C9" s="46" t="s">
         <v>18</v>
       </c>
@@ -17686,8 +17685,8 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="122"/>
-      <c r="B10" s="115" t="s">
+      <c r="A10" s="123"/>
+      <c r="B10" s="116" t="s">
         <v>72</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -17759,8 +17758,8 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="122"/>
-      <c r="B11" s="116"/>
+      <c r="A11" s="123"/>
+      <c r="B11" s="117"/>
       <c r="C11" s="77" t="s">
         <v>16</v>
       </c>
@@ -17787,8 +17786,8 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="122"/>
-      <c r="B12" s="116"/>
+      <c r="A12" s="123"/>
+      <c r="B12" s="117"/>
       <c r="C12" s="77" t="s">
         <v>17</v>
       </c>
@@ -17817,8 +17816,8 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="122"/>
-      <c r="B13" s="117"/>
+      <c r="A13" s="123"/>
+      <c r="B13" s="118"/>
       <c r="C13" s="46" t="s">
         <v>18</v>
       </c>
@@ -17843,8 +17842,8 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="122"/>
-      <c r="B14" s="118" t="s">
+      <c r="A14" s="123"/>
+      <c r="B14" s="119" t="s">
         <v>79</v>
       </c>
       <c r="C14" s="47" t="s">
@@ -17852,7 +17851,7 @@
       </c>
       <c r="D14" s="10">
         <f>SUM(D15:D17)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" s="16">
         <f t="shared" ref="E14:R14" si="4">SUM(E15:E17)</f>
@@ -17888,7 +17887,7 @@
       </c>
       <c r="M14" s="16">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N14" s="16">
         <f t="shared" si="4"/>
@@ -17912,12 +17911,12 @@
       </c>
       <c r="S14" s="14">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="122"/>
-      <c r="B15" s="119"/>
+      <c r="A15" s="123"/>
+      <c r="B15" s="120"/>
       <c r="C15" s="77" t="s">
         <v>16</v>
       </c>
@@ -17942,8 +17941,8 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="122"/>
-      <c r="B16" s="119"/>
+      <c r="A16" s="123"/>
+      <c r="B16" s="120"/>
       <c r="C16" s="77" t="s">
         <v>17</v>
       </c>
@@ -17968,13 +17967,13 @@
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="122"/>
-      <c r="B17" s="120"/>
+      <c r="A17" s="123"/>
+      <c r="B17" s="121"/>
       <c r="C17" s="46" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
@@ -17984,7 +17983,9 @@
       <c r="J17" s="29"/>
       <c r="K17" s="29"/>
       <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
+      <c r="M17" s="29">
+        <v>2</v>
+      </c>
       <c r="N17" s="29"/>
       <c r="O17" s="29"/>
       <c r="P17" s="29"/>
@@ -17992,12 +17993,12 @@
       <c r="R17" s="29"/>
       <c r="S17" s="30">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="122"/>
-      <c r="B18" s="115">
+      <c r="A18" s="123"/>
+      <c r="B18" s="116">
         <v>39</v>
       </c>
       <c r="C18" s="10" t="s">
@@ -18005,7 +18006,7 @@
       </c>
       <c r="D18" s="15">
         <f>SUM(D19:D21)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" s="16">
         <f t="shared" ref="E18:R18" si="5">SUM(E19:E21)</f>
@@ -18041,7 +18042,7 @@
       </c>
       <c r="M18" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N18" s="16">
         <f t="shared" si="5"/>
@@ -18065,12 +18066,12 @@
       </c>
       <c r="S18" s="14">
         <f>SUM(E18:R18)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="122"/>
-      <c r="B19" s="116"/>
+      <c r="A19" s="123"/>
+      <c r="B19" s="117"/>
       <c r="C19" s="77" t="s">
         <v>16</v>
       </c>
@@ -18095,8 +18096,8 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="122"/>
-      <c r="B20" s="116"/>
+      <c r="A20" s="123"/>
+      <c r="B20" s="117"/>
       <c r="C20" s="77" t="s">
         <v>17</v>
       </c>
@@ -18121,13 +18122,13 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="122"/>
-      <c r="B21" s="117"/>
+      <c r="A21" s="123"/>
+      <c r="B21" s="118"/>
       <c r="C21" s="46" t="s">
         <v>18</v>
       </c>
       <c r="D21" s="26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
@@ -18137,7 +18138,9 @@
       <c r="J21" s="29"/>
       <c r="K21" s="29"/>
       <c r="L21" s="29"/>
-      <c r="M21" s="29"/>
+      <c r="M21" s="29">
+        <v>2</v>
+      </c>
       <c r="N21" s="29"/>
       <c r="O21" s="29"/>
       <c r="P21" s="29"/>
@@ -18145,12 +18148,12 @@
       <c r="R21" s="29"/>
       <c r="S21" s="30">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="122"/>
-      <c r="B22" s="115" t="s">
+      <c r="A22" s="123"/>
+      <c r="B22" s="116" t="s">
         <v>78</v>
       </c>
       <c r="C22" s="10" t="s">
@@ -18222,8 +18225,8 @@
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="122"/>
-      <c r="B23" s="116"/>
+      <c r="A23" s="123"/>
+      <c r="B23" s="117"/>
       <c r="C23" s="77" t="s">
         <v>16</v>
       </c>
@@ -18250,8 +18253,8 @@
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="122"/>
-      <c r="B24" s="116"/>
+      <c r="A24" s="123"/>
+      <c r="B24" s="117"/>
       <c r="C24" s="77" t="s">
         <v>17</v>
       </c>
@@ -18280,8 +18283,8 @@
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="122"/>
-      <c r="B25" s="117"/>
+      <c r="A25" s="123"/>
+      <c r="B25" s="118"/>
       <c r="C25" s="46" t="s">
         <v>18</v>
       </c>
@@ -18306,8 +18309,8 @@
       </c>
     </row>
     <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="122"/>
-      <c r="B26" s="118" t="s">
+      <c r="A26" s="123"/>
+      <c r="B26" s="119" t="s">
         <v>74</v>
       </c>
       <c r="C26" s="47" t="s">
@@ -18379,8 +18382,8 @@
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="122"/>
-      <c r="B27" s="119"/>
+      <c r="A27" s="123"/>
+      <c r="B27" s="120"/>
       <c r="C27" s="77" t="s">
         <v>16</v>
       </c>
@@ -18405,8 +18408,8 @@
       </c>
     </row>
     <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="122"/>
-      <c r="B28" s="119"/>
+      <c r="A28" s="123"/>
+      <c r="B28" s="120"/>
       <c r="C28" s="77" t="s">
         <v>17</v>
       </c>
@@ -18435,8 +18438,8 @@
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="122"/>
-      <c r="B29" s="120"/>
+      <c r="A29" s="123"/>
+      <c r="B29" s="121"/>
       <c r="C29" s="46" t="s">
         <v>18</v>
       </c>
@@ -18461,8 +18464,8 @@
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="122"/>
-      <c r="B30" s="118">
+      <c r="A30" s="123"/>
+      <c r="B30" s="119">
         <v>40</v>
       </c>
       <c r="C30" s="60" t="s">
@@ -18470,7 +18473,7 @@
       </c>
       <c r="D30" s="10">
         <f>SUM(D31:D33)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E30" s="16">
         <f t="shared" ref="E30:R30" si="10">SUM(E31:E33)</f>
@@ -18502,7 +18505,7 @@
       </c>
       <c r="L30" s="16">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M30" s="16">
         <f t="shared" si="10"/>
@@ -18530,12 +18533,12 @@
       </c>
       <c r="S30" s="14">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="122"/>
-      <c r="B31" s="119"/>
+      <c r="A31" s="123"/>
+      <c r="B31" s="120"/>
       <c r="C31" s="77" t="s">
         <v>16</v>
       </c>
@@ -18560,8 +18563,8 @@
       </c>
     </row>
     <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="122"/>
-      <c r="B32" s="119"/>
+      <c r="A32" s="123"/>
+      <c r="B32" s="120"/>
       <c r="C32" s="77" t="s">
         <v>17</v>
       </c>
@@ -18590,12 +18593,14 @@
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" s="122"/>
-      <c r="B33" s="120"/>
+      <c r="A33" s="123"/>
+      <c r="B33" s="121"/>
       <c r="C33" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="26"/>
+      <c r="D33" s="26">
+        <v>6</v>
+      </c>
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
       <c r="G33" s="29"/>
@@ -18603,7 +18608,9 @@
       <c r="I33" s="29"/>
       <c r="J33" s="29"/>
       <c r="K33" s="29"/>
-      <c r="L33" s="29"/>
+      <c r="L33" s="29">
+        <v>6</v>
+      </c>
       <c r="M33" s="29"/>
       <c r="N33" s="29"/>
       <c r="O33" s="29"/>
@@ -18612,12 +18619,12 @@
       <c r="R33" s="29"/>
       <c r="S33" s="30">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="122"/>
-      <c r="B34" s="118">
+      <c r="A34" s="123"/>
+      <c r="B34" s="119">
         <v>41</v>
       </c>
       <c r="C34" s="10" t="s">
@@ -18689,8 +18696,8 @@
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="122"/>
-      <c r="B35" s="119"/>
+      <c r="A35" s="123"/>
+      <c r="B35" s="120"/>
       <c r="C35" s="77" t="s">
         <v>16</v>
       </c>
@@ -18717,8 +18724,8 @@
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A36" s="122"/>
-      <c r="B36" s="119"/>
+      <c r="A36" s="123"/>
+      <c r="B36" s="120"/>
       <c r="C36" s="77" t="s">
         <v>17</v>
       </c>
@@ -18743,8 +18750,8 @@
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="122"/>
-      <c r="B37" s="120"/>
+      <c r="A37" s="123"/>
+      <c r="B37" s="121"/>
       <c r="C37" s="46" t="s">
         <v>18</v>
       </c>
@@ -18770,73 +18777,73 @@
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="75"/>
-      <c r="B38" s="106" t="s">
+      <c r="B38" s="113" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="106"/>
+      <c r="C38" s="113"/>
       <c r="D38" s="2">
-        <f>SUM(D6,D10,D14,D18, D22, D26, D30, D34)</f>
-        <v>39</v>
+        <f t="shared" ref="D38:S38" si="12">SUM(D6,D10,D14,D18, D22, D26, D30, D34)</f>
+        <v>47</v>
       </c>
       <c r="E38" s="2">
-        <f>SUM(E6,E10,E14,E18, E22, E26, E30, E34)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="F38" s="2">
-        <f>SUM(F6,F10,F14,F18, F22, F26, F30, F34)</f>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="G38" s="2">
-        <f>SUM(G6,G10,G14,G18, G22, G26, G30, G34)</f>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="H38" s="2">
-        <f>SUM(H6,H10,H14,H18, H22, H26, H30, H34)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I38" s="2">
-        <f>SUM(I6,I10,I14,I18, I22, I26, I30, I34)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="J38" s="2">
-        <f>SUM(J6,J10,J14,J18, J22, J26, J30, J34)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K38" s="2">
-        <f>SUM(K6,K10,K14,K18, K22, K26, K30, K34)</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="L38" s="2">
-        <f>SUM(L6,L10,L14,L18, L22, L26, L30, L34)</f>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>6</v>
       </c>
       <c r="M38" s="2">
-        <f>SUM(M6,M10,M14,M18, M22, M26, M30, M34)</f>
-        <v>7</v>
+        <f t="shared" si="12"/>
+        <v>11</v>
       </c>
       <c r="N38" s="2">
-        <f>SUM(N6,N10,N14,N18, N22, N26, N30, N34)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O38" s="2">
-        <f>SUM(O6,O10,O14,O18, O22, O26, O30, O34)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P38" s="2">
-        <f>SUM(P6,P10,P14,P18, P22, P26, P30, P34)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q38" s="2">
-        <f>SUM(Q6,Q10,Q14,Q18, Q22, Q26, Q30, Q34)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="R38" s="2">
-        <f>SUM(R6,R10,R14,R18, R22, R26, R30, R34)</f>
-        <v>0</v>
-      </c>
-      <c r="S38" s="123">
-        <f>SUM(S6,S10,S14,S18, S22, S26, S30, S34)</f>
-        <v>18</v>
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S38" s="79">
+        <f t="shared" si="12"/>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
@@ -18894,11 +18901,6 @@
     <row r="72" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A6:A37"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="E2:K2"/>
     <mergeCell ref="L2:R2"/>
@@ -18906,6 +18908,11 @@
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="B30:B33"/>
     <mergeCell ref="B34:B37"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A6:A37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated graphs with zachs times added
</commit_message>
<xml_diff>
--- a/Management/Burndown.xlsx
+++ b/Management/Burndown.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="-30" windowWidth="14265" windowHeight="13020" activeTab="6"/>
+    <workbookView xWindow="15" yWindow="-30" windowWidth="14265" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Product Burndown" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -28,7 +28,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="G2" authorId="0" shapeId="0">
+    <comment ref="G2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>Start</t>
-  </si>
-  <si>
-    <t>Added Requirements</t>
   </si>
   <si>
     <t>Planned Effort</t>
@@ -300,6 +297,9 @@
   </si>
   <si>
     <t>Database and interaction classes</t>
+  </si>
+  <si>
+    <t>Added Effort</t>
   </si>
 </sst>
 </file>
@@ -845,6 +845,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -860,11 +866,20 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -883,21 +898,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -1115,16 +1115,19 @@
                   <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>129</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>120</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>68.5</c:v>
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1141,11 +1144,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="268191096"/>
-        <c:axId val="268185216"/>
+        <c:axId val="110344064"/>
+        <c:axId val="110350336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="268191096"/>
+        <c:axId val="110344064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1174,7 +1177,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="268185216"/>
+        <c:crossAx val="110350336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1182,7 +1185,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="268185216"/>
+        <c:axId val="110350336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1212,7 +1215,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="268191096"/>
+        <c:crossAx val="110344064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1470,12 +1473,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="268187568"/>
-        <c:axId val="268191880"/>
+        <c:axId val="121832960"/>
+        <c:axId val="121834496"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="268187568"/>
+        <c:axId val="121832960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1485,14 +1489,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="268191880"/>
+        <c:crossAx val="121834496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="268191880"/>
+        <c:axId val="121834496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1503,7 +1507,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="268187568"/>
+        <c:crossAx val="121832960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1724,12 +1728,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="268187176"/>
-        <c:axId val="268186784"/>
+        <c:axId val="121868288"/>
+        <c:axId val="121869824"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="268187176"/>
+        <c:axId val="121868288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1739,14 +1744,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="268186784"/>
+        <c:crossAx val="121869824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="268186784"/>
+        <c:axId val="121869824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1757,7 +1762,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="268187176"/>
+        <c:crossAx val="121868288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2038,12 +2043,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="268189136"/>
-        <c:axId val="268186000"/>
+        <c:axId val="124324096"/>
+        <c:axId val="124325888"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="268189136"/>
+        <c:axId val="124324096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2053,14 +2059,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="268186000"/>
+        <c:crossAx val="124325888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="268186000"/>
+        <c:axId val="124325888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2071,7 +2077,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="268189136"/>
+        <c:crossAx val="124324096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2356,12 +2362,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="268186392"/>
-        <c:axId val="268187960"/>
+        <c:axId val="124356864"/>
+        <c:axId val="124370944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="268186392"/>
+        <c:axId val="124356864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2371,7 +2378,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="268187960"/>
+        <c:crossAx val="124370944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2379,7 +2386,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="268187960"/>
+        <c:axId val="124370944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2390,7 +2397,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="268186392"/>
+        <c:crossAx val="124356864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2671,12 +2678,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="267792184"/>
-        <c:axId val="267792576"/>
+        <c:axId val="124465920"/>
+        <c:axId val="124467456"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="267792184"/>
+        <c:axId val="124465920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2686,14 +2694,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="267792576"/>
+        <c:crossAx val="124467456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="267792576"/>
+        <c:axId val="124467456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2704,7 +2712,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="267792184"/>
+        <c:crossAx val="124465920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2901,12 +2909,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="334335624"/>
-        <c:axId val="334338368"/>
+        <c:axId val="124549760"/>
+        <c:axId val="124551552"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="334335624"/>
+        <c:axId val="124549760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2916,14 +2925,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="334338368"/>
+        <c:crossAx val="124551552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="334338368"/>
+        <c:axId val="124551552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2934,7 +2943,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="334335624"/>
+        <c:crossAx val="124549760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3253,7 +3262,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3288,7 +3297,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3499,8 +3508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3537,13 +3546,13 @@
         <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>6</v>
@@ -3600,8 +3609,8 @@
         <v>5</v>
       </c>
       <c r="H4" s="4">
-        <f>H3-E4+G4</f>
-        <v>129</v>
+        <f t="shared" ref="H4:H7" si="0">H3-E4+G3</f>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3612,12 +3621,12 @@
         <v>24</v>
       </c>
       <c r="C5" s="4">
-        <f t="shared" ref="C5:C9" si="0" xml:space="preserve"> C4 - B5</f>
+        <f t="shared" ref="C5:C9" si="1" xml:space="preserve"> C4 - B5</f>
         <v>95</v>
       </c>
       <c r="D5" s="4">
-        <f>H4-E5</f>
-        <v>115</v>
+        <f t="shared" ref="D5:D8" si="2">H4-E5</f>
+        <v>110</v>
       </c>
       <c r="E5" s="4">
         <v>14</v>
@@ -3629,8 +3638,8 @@
         <v>5</v>
       </c>
       <c r="H5" s="4">
-        <f t="shared" ref="H5:H6" si="1">H4-E5+G5</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -3641,12 +3650,12 @@
         <v>24</v>
       </c>
       <c r="C6" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>71</v>
       </c>
       <c r="D6" s="4">
-        <f>H5-E6</f>
-        <v>82</v>
+        <f t="shared" si="2"/>
+        <v>77</v>
       </c>
       <c r="E6" s="4">
         <v>38</v>
@@ -3658,8 +3667,8 @@
         <v>8</v>
       </c>
       <c r="H6" s="4">
-        <f t="shared" si="1"/>
-        <v>90</v>
+        <f t="shared" si="0"/>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -3670,12 +3679,12 @@
         <v>24</v>
       </c>
       <c r="C7" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="D7" s="4">
-        <f>H6-E7</f>
-        <v>46</v>
+        <f t="shared" si="2"/>
+        <v>38</v>
       </c>
       <c r="E7" s="4">
         <v>44</v>
@@ -3687,31 +3696,38 @@
         <v>22.5</v>
       </c>
       <c r="H7" s="4">
-        <f>H6-E7+G7</f>
-        <v>68.5</v>
+        <f t="shared" si="0"/>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="A8" s="4">
         <v>5</v>
       </c>
       <c r="B8" s="4">
         <v>24</v>
       </c>
-      <c r="C8" s="3">
-        <f t="shared" si="0"/>
+      <c r="C8" s="4">
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="D8" s="4">
-        <f>H7-E8</f>
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="E8" s="4">
+        <v>39</v>
+      </c>
+      <c r="F8" s="4">
+        <v>58.75</v>
+      </c>
+      <c r="G8" s="4">
+        <v>29</v>
+      </c>
+      <c r="H8" s="4">
+        <f>H7-E8+G7</f>
         <v>29.5</v>
       </c>
-      <c r="E8" s="2">
-        <v>39</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -3721,7 +3737,7 @@
         <v>23</v>
       </c>
       <c r="C9" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D9" s="2"/>
@@ -3857,7 +3873,7 @@
   <sheetData>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E2" s="90" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="91"/>
       <c r="G2" s="91"/>
@@ -3865,7 +3881,7 @@
       <c r="I2" s="91"/>
       <c r="J2" s="92"/>
       <c r="K2" s="81" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L2" s="81"/>
       <c r="M2" s="81"/>
@@ -3875,7 +3891,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C3" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="42"/>
       <c r="E3" s="40">
@@ -3917,7 +3933,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="42">
         <v>0</v>
@@ -3961,13 +3977,13 @@
     </row>
     <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>14</v>
-      </c>
       <c r="D5" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="44"/>
       <c r="F5" s="44"/>
@@ -3982,18 +3998,18 @@
       <c r="O5" s="44"/>
       <c r="P5" s="44"/>
       <c r="Q5" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="83" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="93">
         <v>2</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="15">
         <f>SUM(D7:D9)</f>
@@ -4056,7 +4072,7 @@
       <c r="A7" s="84"/>
       <c r="B7" s="94"/>
       <c r="C7" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="24">
         <v>2</v>
@@ -4086,7 +4102,7 @@
       <c r="A8" s="84"/>
       <c r="B8" s="94"/>
       <c r="C8" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="24">
         <v>2</v>
@@ -4114,7 +4130,7 @@
       <c r="A9" s="84"/>
       <c r="B9" s="94"/>
       <c r="C9" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="26">
         <v>2</v>
@@ -4144,7 +4160,7 @@
       <c r="A10" s="84"/>
       <c r="B10" s="94"/>
       <c r="C10" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="10">
         <f>SUM(D11:D13)</f>
@@ -4207,7 +4223,7 @@
       <c r="A11" s="84"/>
       <c r="B11" s="94"/>
       <c r="C11" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="17"/>
@@ -4231,7 +4247,7 @@
       <c r="A12" s="84"/>
       <c r="B12" s="94"/>
       <c r="C12" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="24">
         <v>3</v>
@@ -4261,7 +4277,7 @@
       <c r="A13" s="84"/>
       <c r="B13" s="94"/>
       <c r="C13" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="18"/>
@@ -4285,7 +4301,7 @@
       <c r="A14" s="84"/>
       <c r="B14" s="94"/>
       <c r="C14" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="10">
         <f>SUM(D15:D17)</f>
@@ -4348,7 +4364,7 @@
       <c r="A15" s="84"/>
       <c r="B15" s="94"/>
       <c r="C15" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="24"/>
       <c r="E15" s="17"/>
@@ -4372,7 +4388,7 @@
       <c r="A16" s="84"/>
       <c r="B16" s="94"/>
       <c r="C16" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" s="24"/>
       <c r="E16" s="17"/>
@@ -4396,7 +4412,7 @@
       <c r="A17" s="84"/>
       <c r="B17" s="95"/>
       <c r="C17" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="26">
         <v>1</v>
@@ -4426,7 +4442,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D18" s="10">
         <f>SUM(D19:D21)</f>
@@ -4489,7 +4505,7 @@
       <c r="A19" s="84"/>
       <c r="B19" s="94"/>
       <c r="C19" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D19" s="24">
         <v>4</v>
@@ -4519,7 +4535,7 @@
       <c r="A20" s="84"/>
       <c r="B20" s="94"/>
       <c r="C20" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="17"/>
@@ -4543,7 +4559,7 @@
       <c r="A21" s="85"/>
       <c r="B21" s="95"/>
       <c r="C21" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" s="26"/>
       <c r="E21" s="18"/>
@@ -4565,11 +4581,11 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="83" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="86"/>
       <c r="C22" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D22" s="10">
         <f>SUM(D23:D25)</f>
@@ -4632,7 +4648,7 @@
       <c r="A23" s="84"/>
       <c r="B23" s="87"/>
       <c r="C23" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D23" s="19"/>
       <c r="E23" s="17"/>
@@ -4656,7 +4672,7 @@
       <c r="A24" s="84"/>
       <c r="B24" s="87"/>
       <c r="C24" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D24" s="25">
         <v>5</v>
@@ -4684,7 +4700,7 @@
       <c r="A25" s="85"/>
       <c r="B25" s="88"/>
       <c r="C25" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="18"/>
@@ -4706,7 +4722,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" s="89" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="89"/>
       <c r="D26" s="2">
@@ -4774,13 +4790,13 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="83" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="93">
         <v>2</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D28" s="15">
         <f>SUM(D29:D31)</f>
@@ -4840,7 +4856,7 @@
       <c r="A29" s="84"/>
       <c r="B29" s="94"/>
       <c r="C29" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D29" s="24">
         <v>2</v>
@@ -4887,7 +4903,7 @@
       <c r="A30" s="84"/>
       <c r="B30" s="94"/>
       <c r="C30" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D30" s="24">
         <v>2</v>
@@ -4934,7 +4950,7 @@
       <c r="A31" s="84"/>
       <c r="B31" s="94"/>
       <c r="C31" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D31" s="26">
         <v>2</v>
@@ -4981,7 +4997,7 @@
       <c r="A32" s="84"/>
       <c r="B32" s="94"/>
       <c r="C32" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D32" s="10">
         <f>SUM(D33:D35)</f>
@@ -5041,7 +5057,7 @@
       <c r="A33" s="84"/>
       <c r="B33" s="94"/>
       <c r="C33" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D33" s="24"/>
       <c r="E33" s="31"/>
@@ -5062,7 +5078,7 @@
       <c r="A34" s="84"/>
       <c r="B34" s="94"/>
       <c r="C34" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D34" s="24">
         <v>3</v>
@@ -5109,7 +5125,7 @@
       <c r="A35" s="84"/>
       <c r="B35" s="94"/>
       <c r="C35" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D35" s="26"/>
       <c r="E35" s="33"/>
@@ -5130,7 +5146,7 @@
       <c r="A36" s="84"/>
       <c r="B36" s="94"/>
       <c r="C36" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D36" s="10">
         <f>SUM(D37:D39)</f>
@@ -5190,7 +5206,7 @@
       <c r="A37" s="84"/>
       <c r="B37" s="94"/>
       <c r="C37" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D37" s="24"/>
       <c r="E37" s="31"/>
@@ -5211,7 +5227,7 @@
       <c r="A38" s="84"/>
       <c r="B38" s="94"/>
       <c r="C38" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D38" s="24"/>
       <c r="E38" s="31"/>
@@ -5232,7 +5248,7 @@
       <c r="A39" s="84"/>
       <c r="B39" s="95"/>
       <c r="C39" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D39" s="26">
         <v>1</v>
@@ -5281,7 +5297,7 @@
         <v>3</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D40" s="10">
         <f>SUM(D41:D43)</f>
@@ -5341,7 +5357,7 @@
       <c r="A41" s="84"/>
       <c r="B41" s="94"/>
       <c r="C41" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D41" s="24">
         <v>4</v>
@@ -5388,7 +5404,7 @@
       <c r="A42" s="84"/>
       <c r="B42" s="94"/>
       <c r="C42" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D42" s="24"/>
       <c r="E42" s="31"/>
@@ -5409,7 +5425,7 @@
       <c r="A43" s="85"/>
       <c r="B43" s="95"/>
       <c r="C43" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D43" s="26"/>
       <c r="E43" s="33"/>
@@ -5428,11 +5444,11 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="83" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B44" s="86"/>
       <c r="C44" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D44" s="10">
         <f>SUM(D45:D47)</f>
@@ -5492,7 +5508,7 @@
       <c r="A45" s="84"/>
       <c r="B45" s="87"/>
       <c r="C45" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D45" s="19"/>
       <c r="E45" s="31"/>
@@ -5513,7 +5529,7 @@
       <c r="A46" s="84"/>
       <c r="B46" s="87"/>
       <c r="C46" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D46" s="19">
         <v>5</v>
@@ -5560,7 +5576,7 @@
       <c r="A47" s="85"/>
       <c r="B47" s="88"/>
       <c r="C47" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="33"/>
@@ -5579,7 +5595,7 @@
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B48" s="89" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C48" s="89"/>
       <c r="D48" s="2">
@@ -5743,14 +5759,14 @@
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E2" s="90" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="91"/>
       <c r="G2" s="91"/>
       <c r="H2" s="91"/>
       <c r="I2" s="91"/>
       <c r="J2" s="90" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K2" s="91"/>
       <c r="L2" s="91"/>
@@ -5758,7 +5774,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D3" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="40">
         <v>41975</v>
@@ -5790,7 +5806,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D4" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="43">
         <v>1</v>
@@ -5822,13 +5838,13 @@
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="48" t="s">
-        <v>14</v>
-      </c>
       <c r="D5" s="55" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="53"/>
       <c r="F5" s="53"/>
@@ -5840,18 +5856,18 @@
       <c r="L5" s="53"/>
       <c r="M5" s="53"/>
       <c r="N5" s="54" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="83" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="96">
+        <v>11</v>
+      </c>
+      <c r="B6" s="98">
         <v>1</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="15">
         <f>SUM(D7:D9)</f>
@@ -5900,9 +5916,9 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="84"/>
-      <c r="B7" s="97"/>
+      <c r="B7" s="99"/>
       <c r="C7" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="17"/>
@@ -5921,9 +5937,9 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="84"/>
-      <c r="B8" s="97"/>
+      <c r="B8" s="99"/>
       <c r="C8" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="24">
         <v>2</v>
@@ -5946,9 +5962,9 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="84"/>
-      <c r="B9" s="98"/>
+      <c r="B9" s="100"/>
       <c r="C9" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="26"/>
       <c r="E9" s="18"/>
@@ -5967,11 +5983,11 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="84"/>
-      <c r="B10" s="99" t="s">
-        <v>35</v>
+      <c r="B10" s="101" t="s">
+        <v>34</v>
       </c>
       <c r="C10" s="47" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="10">
         <f>SUM(D11:D13)</f>
@@ -6020,9 +6036,9 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="84"/>
-      <c r="B11" s="100"/>
+      <c r="B11" s="102"/>
       <c r="C11" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="24">
         <v>1</v>
@@ -6045,9 +6061,9 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="84"/>
-      <c r="B12" s="100"/>
+      <c r="B12" s="102"/>
       <c r="C12" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="24"/>
       <c r="E12" s="17"/>
@@ -6066,9 +6082,9 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="84"/>
-      <c r="B13" s="100"/>
+      <c r="B13" s="102"/>
       <c r="C13" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="18"/>
@@ -6087,9 +6103,9 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="84"/>
-      <c r="B14" s="100"/>
+      <c r="B14" s="102"/>
       <c r="C14" s="52" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14" s="10">
         <f>SUM(D15:D17)</f>
@@ -6138,9 +6154,9 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="84"/>
-      <c r="B15" s="100"/>
+      <c r="B15" s="102"/>
       <c r="C15" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="24">
         <v>3</v>
@@ -6165,9 +6181,9 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="84"/>
-      <c r="B16" s="100"/>
+      <c r="B16" s="102"/>
       <c r="C16" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" s="24">
         <v>3</v>
@@ -6190,9 +6206,9 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="84"/>
-      <c r="B17" s="100"/>
+      <c r="B17" s="102"/>
       <c r="C17" s="45" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="17"/>
@@ -6211,11 +6227,11 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="83" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" s="93"/>
       <c r="C18" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" s="10">
         <f>SUM(D19:D21)</f>
@@ -6266,7 +6282,7 @@
       <c r="A19" s="84"/>
       <c r="B19" s="94"/>
       <c r="C19" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D19" s="24">
         <v>2</v>
@@ -6291,7 +6307,7 @@
       <c r="A20" s="84"/>
       <c r="B20" s="94"/>
       <c r="C20" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D20" s="24">
         <v>2</v>
@@ -6316,7 +6332,7 @@
       <c r="A21" s="84"/>
       <c r="B21" s="94"/>
       <c r="C21" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" s="26"/>
       <c r="E21" s="18"/>
@@ -6335,9 +6351,9 @@
     </row>
     <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="84"/>
-      <c r="B22" s="101"/>
+      <c r="B22" s="96"/>
       <c r="C22" s="49" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D22" s="49">
         <f>SUM(D23:D25)</f>
@@ -6386,9 +6402,9 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="84"/>
-      <c r="B23" s="101"/>
+      <c r="B23" s="96"/>
       <c r="C23" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D23" s="19"/>
       <c r="E23" s="17"/>
@@ -6407,9 +6423,9 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="84"/>
-      <c r="B24" s="101"/>
+      <c r="B24" s="96"/>
       <c r="C24" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D24" s="25">
         <v>1</v>
@@ -6432,9 +6448,9 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="85"/>
-      <c r="B25" s="102"/>
+      <c r="B25" s="97"/>
       <c r="C25" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D25" s="26"/>
       <c r="E25" s="18"/>
@@ -6453,7 +6469,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B26" s="89" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="89"/>
       <c r="D26" s="2">
@@ -6509,13 +6525,13 @@
     </row>
     <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="83" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="96">
+        <v>11</v>
+      </c>
+      <c r="B28" s="98">
         <v>1</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D28" s="15">
         <f>D6</f>
@@ -6561,9 +6577,9 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="84"/>
-      <c r="B29" s="97"/>
+      <c r="B29" s="99"/>
       <c r="C29" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D29" s="57">
         <f t="shared" ref="D29:D47" si="8">D7</f>
@@ -6582,9 +6598,9 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="84"/>
-      <c r="B30" s="97"/>
+      <c r="B30" s="99"/>
       <c r="C30" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D30" s="57">
         <f>D8</f>
@@ -6621,9 +6637,9 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="84"/>
-      <c r="B31" s="98"/>
+      <c r="B31" s="100"/>
       <c r="C31" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D31" s="58">
         <f t="shared" si="8"/>
@@ -6642,11 +6658,11 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="84"/>
-      <c r="B32" s="99" t="s">
-        <v>35</v>
+      <c r="B32" s="101" t="s">
+        <v>34</v>
       </c>
       <c r="C32" s="47" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D32" s="56">
         <f t="shared" si="8"/>
@@ -6692,9 +6708,9 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="84"/>
-      <c r="B33" s="100"/>
+      <c r="B33" s="102"/>
       <c r="C33" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D33" s="57">
         <f t="shared" si="8"/>
@@ -6731,9 +6747,9 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="84"/>
-      <c r="B34" s="100"/>
+      <c r="B34" s="102"/>
       <c r="C34" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D34" s="57">
         <f t="shared" si="8"/>
@@ -6752,9 +6768,9 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="84"/>
-      <c r="B35" s="100"/>
+      <c r="B35" s="102"/>
       <c r="C35" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D35" s="58">
         <f t="shared" si="8"/>
@@ -6791,9 +6807,9 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="84"/>
-      <c r="B36" s="100"/>
+      <c r="B36" s="102"/>
       <c r="C36" s="52" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D36" s="56">
         <f t="shared" si="8"/>
@@ -6839,9 +6855,9 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="84"/>
-      <c r="B37" s="100"/>
+      <c r="B37" s="102"/>
       <c r="C37" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D37" s="57">
         <f t="shared" si="8"/>
@@ -6878,9 +6894,9 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="84"/>
-      <c r="B38" s="100"/>
+      <c r="B38" s="102"/>
       <c r="C38" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D38" s="57">
         <f t="shared" si="8"/>
@@ -6917,9 +6933,9 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="84"/>
-      <c r="B39" s="100"/>
+      <c r="B39" s="102"/>
       <c r="C39" s="45" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D39" s="58">
         <f t="shared" si="8"/>
@@ -6938,11 +6954,11 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="83" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B40" s="93"/>
       <c r="C40" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D40" s="56">
         <f t="shared" si="8"/>
@@ -6990,7 +7006,7 @@
       <c r="A41" s="84"/>
       <c r="B41" s="94"/>
       <c r="C41" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D41" s="57">
         <f t="shared" si="8"/>
@@ -7029,7 +7045,7 @@
       <c r="A42" s="84"/>
       <c r="B42" s="94"/>
       <c r="C42" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D42" s="57">
         <f t="shared" si="8"/>
@@ -7068,7 +7084,7 @@
       <c r="A43" s="84"/>
       <c r="B43" s="94"/>
       <c r="C43" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D43" s="58">
         <f t="shared" si="8"/>
@@ -7087,9 +7103,9 @@
     </row>
     <row r="44" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="84"/>
-      <c r="B44" s="101"/>
+      <c r="B44" s="96"/>
       <c r="C44" s="49" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D44" s="56">
         <f t="shared" si="8"/>
@@ -7135,9 +7151,9 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="84"/>
-      <c r="B45" s="101"/>
+      <c r="B45" s="96"/>
       <c r="C45" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D45" s="57">
         <f t="shared" si="8"/>
@@ -7156,9 +7172,9 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="84"/>
-      <c r="B46" s="101"/>
+      <c r="B46" s="96"/>
       <c r="C46" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D46" s="57">
         <f t="shared" si="8"/>
@@ -7195,9 +7211,9 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="85"/>
-      <c r="B47" s="102"/>
+      <c r="B47" s="97"/>
       <c r="C47" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D47" s="58">
         <f t="shared" si="8"/>
@@ -7234,7 +7250,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B48" s="89" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C48" s="89"/>
       <c r="D48" s="2">
@@ -7323,6 +7339,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="A28:A39"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="B32:B39"/>
+    <mergeCell ref="A40:A47"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="B44:B47"/>
     <mergeCell ref="A18:A25"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="B22:B25"/>
@@ -7331,14 +7355,6 @@
     <mergeCell ref="A6:A17"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="B10:B17"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="A28:A39"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="B32:B39"/>
-    <mergeCell ref="A40:A47"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="B44:B47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -7376,7 +7392,7 @@
   <sheetData>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E2" s="90" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="91"/>
       <c r="G2" s="91"/>
@@ -7385,7 +7401,7 @@
       <c r="J2" s="91"/>
       <c r="K2" s="91"/>
       <c r="L2" s="90" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M2" s="91"/>
       <c r="N2" s="91"/>
@@ -7396,7 +7412,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D3" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="40">
         <v>42022</v>
@@ -7443,7 +7459,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D4" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="43">
         <v>1</v>
@@ -7490,13 +7506,13 @@
     </row>
     <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="48" t="s">
-        <v>14</v>
-      </c>
       <c r="D5" s="55" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="53"/>
       <c r="F5" s="53"/>
@@ -7513,18 +7529,18 @@
       <c r="Q5" s="61"/>
       <c r="R5" s="61"/>
       <c r="S5" s="54" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="83" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="98">
         <v>12</v>
       </c>
-      <c r="B6" s="96">
-        <v>12</v>
-      </c>
       <c r="C6" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="15">
         <f>SUM(D7:D9)</f>
@@ -7593,9 +7609,9 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="84"/>
-      <c r="B7" s="97"/>
+      <c r="B7" s="99"/>
       <c r="C7" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="17"/>
@@ -7619,9 +7635,9 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="84"/>
-      <c r="B8" s="97"/>
+      <c r="B8" s="99"/>
       <c r="C8" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="24"/>
       <c r="E8" s="62"/>
@@ -7645,9 +7661,9 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="84"/>
-      <c r="B9" s="98"/>
+      <c r="B9" s="100"/>
       <c r="C9" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="26">
         <v>1.5</v>
@@ -7675,11 +7691,11 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="84"/>
-      <c r="B10" s="106">
+      <c r="B10" s="111">
         <v>15</v>
       </c>
       <c r="C10" s="47" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="10">
         <f>SUM(D11:D13)</f>
@@ -7748,9 +7764,9 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="84"/>
-      <c r="B11" s="107"/>
+      <c r="B11" s="112"/>
       <c r="C11" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="17"/>
@@ -7774,9 +7790,9 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="84"/>
-      <c r="B12" s="107"/>
+      <c r="B12" s="112"/>
       <c r="C12" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="24"/>
       <c r="E12" s="17"/>
@@ -7800,9 +7816,9 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="84"/>
-      <c r="B13" s="108"/>
+      <c r="B13" s="113"/>
       <c r="C13" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="26">
         <v>1.5</v>
@@ -7830,11 +7846,11 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="84"/>
-      <c r="B14" s="106">
+      <c r="B14" s="111">
         <v>21</v>
       </c>
       <c r="C14" s="60" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14" s="10">
         <f>SUM(D15:D17)</f>
@@ -7903,9 +7919,9 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="84"/>
-      <c r="B15" s="107"/>
+      <c r="B15" s="112"/>
       <c r="C15" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="24">
         <v>8</v>
@@ -7937,9 +7953,9 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="84"/>
-      <c r="B16" s="107"/>
+      <c r="B16" s="112"/>
       <c r="C16" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" s="24"/>
       <c r="E16" s="17"/>
@@ -7963,9 +7979,9 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="84"/>
-      <c r="B17" s="108"/>
+      <c r="B17" s="113"/>
       <c r="C17" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="26"/>
       <c r="E17" s="18"/>
@@ -7989,11 +8005,11 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="84"/>
-      <c r="B18" s="106">
+      <c r="B18" s="111">
         <v>18</v>
       </c>
       <c r="C18" s="60" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" s="10">
         <f>SUM(D19:D21)</f>
@@ -8062,9 +8078,9 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="84"/>
-      <c r="B19" s="107"/>
+      <c r="B19" s="112"/>
       <c r="C19" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D19" s="24">
         <v>3</v>
@@ -8092,9 +8108,9 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="84"/>
-      <c r="B20" s="107"/>
+      <c r="B20" s="112"/>
       <c r="C20" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="17"/>
@@ -8118,9 +8134,9 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="84"/>
-      <c r="B21" s="108"/>
+      <c r="B21" s="113"/>
       <c r="C21" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" s="26"/>
       <c r="E21" s="18"/>
@@ -8144,11 +8160,11 @@
     </row>
     <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="84"/>
-      <c r="B22" s="109" t="s">
+      <c r="B22" s="103" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="60" t="s">
         <v>42</v>
-      </c>
-      <c r="C22" s="60" t="s">
-        <v>43</v>
       </c>
       <c r="D22" s="10">
         <f>SUM(D23:D25)</f>
@@ -8217,9 +8233,9 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="84"/>
-      <c r="B23" s="110"/>
+      <c r="B23" s="104"/>
       <c r="C23" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D23" s="24"/>
       <c r="E23" s="17"/>
@@ -8243,9 +8259,9 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="84"/>
-      <c r="B24" s="110"/>
+      <c r="B24" s="104"/>
       <c r="C24" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D24" s="24">
         <v>8</v>
@@ -8275,9 +8291,9 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="84"/>
-      <c r="B25" s="111"/>
+      <c r="B25" s="105"/>
       <c r="C25" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D25" s="26"/>
       <c r="E25" s="18"/>
@@ -8301,11 +8317,11 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="84"/>
-      <c r="B26" s="109" t="s">
-        <v>45</v>
+      <c r="B26" s="103" t="s">
+        <v>44</v>
       </c>
       <c r="C26" s="60" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D26" s="10">
         <f>SUM(D27:D29)</f>
@@ -8374,9 +8390,9 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="84"/>
-      <c r="B27" s="110"/>
+      <c r="B27" s="104"/>
       <c r="C27" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D27" s="24"/>
       <c r="E27" s="17"/>
@@ -8400,9 +8416,9 @@
     </row>
     <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="84"/>
-      <c r="B28" s="110"/>
+      <c r="B28" s="104"/>
       <c r="C28" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D28" s="24">
         <v>5</v>
@@ -8430,9 +8446,9 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="84"/>
-      <c r="B29" s="111"/>
+      <c r="B29" s="105"/>
       <c r="C29" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D29" s="26"/>
       <c r="E29" s="18"/>
@@ -8456,11 +8472,11 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="84"/>
-      <c r="B30" s="109">
+      <c r="B30" s="103">
         <v>31</v>
       </c>
       <c r="C30" s="60" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D30" s="10">
         <f>SUM(D31:D33)</f>
@@ -8529,9 +8545,9 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="84"/>
-      <c r="B31" s="110"/>
+      <c r="B31" s="104"/>
       <c r="C31" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D31" s="24"/>
       <c r="E31" s="17"/>
@@ -8555,9 +8571,9 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="84"/>
-      <c r="B32" s="110"/>
+      <c r="B32" s="104"/>
       <c r="C32" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D32" s="24">
         <v>3</v>
@@ -8585,9 +8601,9 @@
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="85"/>
-      <c r="B33" s="111"/>
+      <c r="B33" s="105"/>
       <c r="C33" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D33" s="26"/>
       <c r="E33" s="18"/>
@@ -8611,11 +8627,11 @@
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="83" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B34" s="93"/>
       <c r="C34" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D34" s="10">
         <f t="shared" ref="D34:M34" si="15">SUM(D35:D37)</f>
@@ -8686,7 +8702,7 @@
       <c r="A35" s="84"/>
       <c r="B35" s="94"/>
       <c r="C35" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D35" s="24"/>
       <c r="E35" s="17"/>
@@ -8712,7 +8728,7 @@
       <c r="A36" s="84"/>
       <c r="B36" s="94"/>
       <c r="C36" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D36" s="24">
         <v>2</v>
@@ -8742,7 +8758,7 @@
       <c r="A37" s="84"/>
       <c r="B37" s="94"/>
       <c r="C37" s="45" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D37" s="24"/>
       <c r="E37" s="17"/>
@@ -8766,9 +8782,9 @@
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="84"/>
-      <c r="B38" s="103"/>
+      <c r="B38" s="108"/>
       <c r="C38" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D38" s="10">
         <f t="shared" ref="D38:M38" si="18">SUM(D39:D41)</f>
@@ -8837,9 +8853,9 @@
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="84"/>
-      <c r="B39" s="104"/>
+      <c r="B39" s="109"/>
       <c r="C39" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D39" s="19"/>
       <c r="E39" s="17"/>
@@ -8863,9 +8879,9 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="84"/>
-      <c r="B40" s="104"/>
+      <c r="B40" s="109"/>
       <c r="C40" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D40" s="25">
         <v>6</v>
@@ -8893,9 +8909,9 @@
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="85"/>
-      <c r="B41" s="105"/>
+      <c r="B41" s="110"/>
       <c r="C41" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D41" s="26"/>
       <c r="E41" s="18"/>
@@ -8918,10 +8934,10 @@
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B42" s="113" t="s">
-        <v>26</v>
-      </c>
-      <c r="C42" s="113"/>
+      <c r="B42" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" s="107"/>
       <c r="D42" s="2">
         <f t="shared" ref="D42:R42" si="21">SUM(D6,D10,D14,D34,D38,D18,D22,D26,D30)</f>
         <v>38</v>
@@ -8989,13 +9005,13 @@
     </row>
     <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="83" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" s="98">
         <v>12</v>
       </c>
-      <c r="B44" s="96">
-        <v>12</v>
-      </c>
       <c r="C44" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D44" s="15">
         <f>SUM(D45:D47)</f>
@@ -9060,9 +9076,9 @@
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="84"/>
-      <c r="B45" s="97"/>
+      <c r="B45" s="99"/>
       <c r="C45" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D45" s="24">
         <f>D7</f>
@@ -9085,9 +9101,9 @@
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="84"/>
-      <c r="B46" s="97"/>
+      <c r="B46" s="99"/>
       <c r="C46" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D46" s="24">
         <f>D8</f>
@@ -9110,9 +9126,9 @@
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="84"/>
-      <c r="B47" s="98"/>
+      <c r="B47" s="100"/>
       <c r="C47" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D47" s="24">
         <f>D9</f>
@@ -9163,11 +9179,11 @@
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="84"/>
-      <c r="B48" s="106">
+      <c r="B48" s="111">
         <v>15</v>
       </c>
       <c r="C48" s="47" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D48" s="10">
         <f>SUM(D49:D51)</f>
@@ -9232,9 +9248,9 @@
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="84"/>
-      <c r="B49" s="107"/>
+      <c r="B49" s="112"/>
       <c r="C49" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D49" s="24">
         <f>D11</f>
@@ -9257,9 +9273,9 @@
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="84"/>
-      <c r="B50" s="107"/>
+      <c r="B50" s="112"/>
       <c r="C50" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D50" s="24">
         <f>D12</f>
@@ -9282,9 +9298,9 @@
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="84"/>
-      <c r="B51" s="108"/>
+      <c r="B51" s="113"/>
       <c r="C51" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D51" s="24">
         <f>D13</f>
@@ -9338,11 +9354,11 @@
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="84"/>
-      <c r="B52" s="106">
+      <c r="B52" s="111">
         <v>21</v>
       </c>
       <c r="C52" s="60" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D52" s="10">
         <f>SUM(D53:D55)</f>
@@ -9407,9 +9423,9 @@
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="84"/>
-      <c r="B53" s="107"/>
+      <c r="B53" s="112"/>
       <c r="C53" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D53" s="24">
         <f>D15</f>
@@ -9460,9 +9476,9 @@
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="84"/>
-      <c r="B54" s="107"/>
+      <c r="B54" s="112"/>
       <c r="C54" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D54" s="24">
         <f>D16</f>
@@ -9485,9 +9501,9 @@
     </row>
     <row r="55" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="84"/>
-      <c r="B55" s="108"/>
+      <c r="B55" s="113"/>
       <c r="C55" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D55" s="24">
         <f>D17</f>
@@ -9510,11 +9526,11 @@
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="84"/>
-      <c r="B56" s="106">
+      <c r="B56" s="111">
         <v>18</v>
       </c>
       <c r="C56" s="60" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D56" s="10">
         <f>SUM(D57:D59)</f>
@@ -9579,9 +9595,9 @@
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="84"/>
-      <c r="B57" s="107"/>
+      <c r="B57" s="112"/>
       <c r="C57" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D57" s="24">
         <f>D19</f>
@@ -9632,9 +9648,9 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="84"/>
-      <c r="B58" s="107"/>
+      <c r="B58" s="112"/>
       <c r="C58" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D58" s="24">
         <f>D20</f>
@@ -9657,9 +9673,9 @@
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="84"/>
-      <c r="B59" s="108"/>
+      <c r="B59" s="113"/>
       <c r="C59" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D59" s="24">
         <f>D21</f>
@@ -9682,11 +9698,11 @@
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="84"/>
-      <c r="B60" s="109" t="s">
+      <c r="B60" s="103" t="s">
+        <v>41</v>
+      </c>
+      <c r="C60" s="60" t="s">
         <v>42</v>
-      </c>
-      <c r="C60" s="60" t="s">
-        <v>43</v>
       </c>
       <c r="D60" s="10">
         <f>SUM(D61:D63)</f>
@@ -9751,9 +9767,9 @@
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="84"/>
-      <c r="B61" s="110"/>
+      <c r="B61" s="104"/>
       <c r="C61" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D61" s="24">
         <f>D23</f>
@@ -9776,9 +9792,9 @@
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="84"/>
-      <c r="B62" s="110"/>
+      <c r="B62" s="104"/>
       <c r="C62" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D62" s="24">
         <f>D24</f>
@@ -9829,9 +9845,9 @@
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="84"/>
-      <c r="B63" s="111"/>
+      <c r="B63" s="105"/>
       <c r="C63" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D63" s="24">
         <f>D25</f>
@@ -9854,11 +9870,11 @@
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="84"/>
-      <c r="B64" s="109" t="s">
-        <v>45</v>
+      <c r="B64" s="103" t="s">
+        <v>44</v>
       </c>
       <c r="C64" s="60" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D64" s="10">
         <f>SUM(D65:D67)</f>
@@ -9923,9 +9939,9 @@
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="84"/>
-      <c r="B65" s="110"/>
+      <c r="B65" s="104"/>
       <c r="C65" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D65" s="24">
         <f>D27</f>
@@ -9948,9 +9964,9 @@
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="84"/>
-      <c r="B66" s="110"/>
+      <c r="B66" s="104"/>
       <c r="C66" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D66" s="24">
         <f>D28</f>
@@ -10001,9 +10017,9 @@
     </row>
     <row r="67" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="84"/>
-      <c r="B67" s="111"/>
+      <c r="B67" s="105"/>
       <c r="C67" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D67" s="24">
         <f>D29</f>
@@ -10026,11 +10042,11 @@
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="84"/>
-      <c r="B68" s="109">
+      <c r="B68" s="103">
         <v>31</v>
       </c>
       <c r="C68" s="60" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D68" s="10">
         <f>SUM(D69:D71)</f>
@@ -10095,9 +10111,9 @@
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="84"/>
-      <c r="B69" s="110"/>
+      <c r="B69" s="104"/>
       <c r="C69" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D69" s="24">
         <f>D31</f>
@@ -10120,9 +10136,9 @@
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="84"/>
-      <c r="B70" s="110"/>
+      <c r="B70" s="104"/>
       <c r="C70" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D70" s="24">
         <f>D32</f>
@@ -10173,9 +10189,9 @@
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="85"/>
-      <c r="B71" s="111"/>
+      <c r="B71" s="105"/>
       <c r="C71" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D71" s="24">
         <f>D33</f>
@@ -10198,11 +10214,11 @@
     </row>
     <row r="72" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="83" t="s">
-        <v>23</v>
-      </c>
-      <c r="B72" s="96"/>
+        <v>22</v>
+      </c>
+      <c r="B72" s="98"/>
       <c r="C72" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D72" s="10">
         <f>SUM(D73:D75)</f>
@@ -10267,9 +10283,9 @@
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="84"/>
-      <c r="B73" s="97"/>
+      <c r="B73" s="99"/>
       <c r="C73" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D73" s="24">
         <f>D35</f>
@@ -10292,9 +10308,9 @@
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="84"/>
-      <c r="B74" s="97"/>
+      <c r="B74" s="99"/>
       <c r="C74" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D74" s="24">
         <f>D36</f>
@@ -10345,9 +10361,9 @@
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="84"/>
-      <c r="B75" s="98"/>
+      <c r="B75" s="100"/>
       <c r="C75" s="45" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D75" s="24">
         <f>D37</f>
@@ -10370,9 +10386,9 @@
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="84"/>
-      <c r="B76" s="103"/>
+      <c r="B76" s="108"/>
       <c r="C76" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D76" s="10">
         <f>SUM(D77:D79)</f>
@@ -10437,9 +10453,9 @@
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="84"/>
-      <c r="B77" s="104"/>
+      <c r="B77" s="109"/>
       <c r="C77" s="45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D77" s="24">
         <f>D39</f>
@@ -10462,9 +10478,9 @@
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="84"/>
-      <c r="B78" s="104"/>
+      <c r="B78" s="109"/>
       <c r="C78" s="45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D78" s="24">
         <f>D40</f>
@@ -10515,9 +10531,9 @@
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" s="85"/>
-      <c r="B79" s="105"/>
+      <c r="B79" s="110"/>
       <c r="C79" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D79" s="26">
         <f t="shared" ref="D79" si="40">D41</f>
@@ -10539,10 +10555,10 @@
       <c r="R79" s="39"/>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B80" s="112" t="s">
-        <v>26</v>
-      </c>
-      <c r="C80" s="112"/>
+      <c r="B80" s="106" t="s">
+        <v>25</v>
+      </c>
+      <c r="C80" s="106"/>
       <c r="D80" s="2">
         <f t="shared" ref="D80:M80" si="41">SUM(D44,D64,D68,D72,D76)</f>
         <v>17.5</v>
@@ -10668,16 +10684,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="E2:K2"/>
-    <mergeCell ref="L2:R2"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="B68:B71"/>
     <mergeCell ref="A72:A79"/>
     <mergeCell ref="B34:B37"/>
     <mergeCell ref="B38:B41"/>
@@ -10694,6 +10700,16 @@
     <mergeCell ref="B48:B51"/>
     <mergeCell ref="B52:B55"/>
     <mergeCell ref="B64:B67"/>
+    <mergeCell ref="E2:K2"/>
+    <mergeCell ref="L2:R2"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="B68:B71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -10731,7 +10747,7 @@
   <sheetData>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E2" s="90" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="91"/>
       <c r="G2" s="91"/>
@@ -10740,7 +10756,7 @@
       <c r="J2" s="91"/>
       <c r="K2" s="91"/>
       <c r="L2" s="90" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M2" s="91"/>
       <c r="N2" s="91"/>
@@ -10751,7 +10767,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D3" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="40">
         <v>42064</v>
@@ -10798,7 +10814,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D4" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="43">
         <v>1</v>
@@ -10845,13 +10861,13 @@
     </row>
     <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="48" t="s">
-        <v>14</v>
-      </c>
       <c r="D5" s="55" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="53"/>
       <c r="F5" s="53"/>
@@ -10868,18 +10884,18 @@
       <c r="Q5" s="61"/>
       <c r="R5" s="61"/>
       <c r="S5" s="54" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="83" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="96">
+        <v>11</v>
+      </c>
+      <c r="B6" s="98">
         <v>28</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" s="15">
         <f>SUM(D7:D9)</f>
@@ -10948,9 +10964,9 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="84"/>
-      <c r="B7" s="97"/>
+      <c r="B7" s="99"/>
       <c r="C7" s="66" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="24">
         <v>2</v>
@@ -10978,9 +10994,9 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="84"/>
-      <c r="B8" s="97"/>
+      <c r="B8" s="99"/>
       <c r="C8" s="66" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="24"/>
       <c r="E8" s="62"/>
@@ -11004,9 +11020,9 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="84"/>
-      <c r="B9" s="98"/>
+      <c r="B9" s="100"/>
       <c r="C9" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="26"/>
       <c r="E9" s="18"/>
@@ -11030,11 +11046,11 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="84"/>
-      <c r="B10" s="106">
+      <c r="B10" s="111">
         <v>16</v>
       </c>
       <c r="C10" s="47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" s="10">
         <f>SUM(D11:D13)</f>
@@ -11103,9 +11119,9 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="84"/>
-      <c r="B11" s="107"/>
+      <c r="B11" s="112"/>
       <c r="C11" s="66" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="24">
         <v>2</v>
@@ -11133,9 +11149,9 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="84"/>
-      <c r="B12" s="107"/>
+      <c r="B12" s="112"/>
       <c r="C12" s="66" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="24"/>
       <c r="E12" s="17"/>
@@ -11159,9 +11175,9 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="84"/>
-      <c r="B13" s="108"/>
+      <c r="B13" s="113"/>
       <c r="C13" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="18"/>
@@ -11185,11 +11201,11 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="84"/>
-      <c r="B14" s="106">
+      <c r="B14" s="111">
         <v>9</v>
       </c>
       <c r="C14" s="60" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D14" s="10">
         <f>SUM(D15:D17)</f>
@@ -11258,9 +11274,9 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="84"/>
-      <c r="B15" s="107"/>
+      <c r="B15" s="112"/>
       <c r="C15" s="66" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="24">
         <v>4</v>
@@ -11288,9 +11304,9 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="84"/>
-      <c r="B16" s="107"/>
+      <c r="B16" s="112"/>
       <c r="C16" s="66" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" s="24">
         <v>4</v>
@@ -11318,9 +11334,9 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="84"/>
-      <c r="B17" s="108"/>
+      <c r="B17" s="113"/>
       <c r="C17" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="26"/>
       <c r="E17" s="18"/>
@@ -11344,11 +11360,11 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="84"/>
-      <c r="B18" s="106" t="s">
-        <v>56</v>
+      <c r="B18" s="111" t="s">
+        <v>55</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" s="10">
         <f>SUM(D19:D21)</f>
@@ -11417,9 +11433,9 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="84"/>
-      <c r="B19" s="107"/>
+      <c r="B19" s="112"/>
       <c r="C19" s="66" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D19" s="24"/>
       <c r="E19" s="17"/>
@@ -11443,9 +11459,9 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="84"/>
-      <c r="B20" s="107"/>
+      <c r="B20" s="112"/>
       <c r="C20" s="66" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="17"/>
@@ -11469,9 +11485,9 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="84"/>
-      <c r="B21" s="108"/>
+      <c r="B21" s="113"/>
       <c r="C21" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" s="26">
         <v>4</v>
@@ -11499,11 +11515,11 @@
     </row>
     <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="84"/>
-      <c r="B22" s="96" t="s">
-        <v>57</v>
+      <c r="B22" s="98" t="s">
+        <v>56</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D22" s="10">
         <f>SUM(D23:D25)</f>
@@ -11572,9 +11588,9 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="84"/>
-      <c r="B23" s="97"/>
+      <c r="B23" s="99"/>
       <c r="C23" s="66" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D23" s="24">
         <v>2</v>
@@ -11602,9 +11618,9 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="84"/>
-      <c r="B24" s="97"/>
+      <c r="B24" s="99"/>
       <c r="C24" s="66" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D24" s="24">
         <v>3.5</v>
@@ -11632,9 +11648,9 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="84"/>
-      <c r="B25" s="98"/>
+      <c r="B25" s="100"/>
       <c r="C25" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D25" s="26"/>
       <c r="E25" s="18"/>
@@ -11658,11 +11674,11 @@
     </row>
     <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="83" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="63"/>
       <c r="C26" s="60" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D26" s="10">
         <f>SUM(D27:D29)</f>
@@ -11733,7 +11749,7 @@
       <c r="A27" s="84"/>
       <c r="B27" s="64"/>
       <c r="C27" s="66" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D27" s="24">
         <v>2</v>
@@ -11763,7 +11779,7 @@
       <c r="A28" s="84"/>
       <c r="B28" s="64"/>
       <c r="C28" s="66" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D28" s="24"/>
       <c r="E28" s="17"/>
@@ -11789,7 +11805,7 @@
       <c r="A29" s="84"/>
       <c r="B29" s="65"/>
       <c r="C29" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D29" s="26"/>
       <c r="E29" s="18"/>
@@ -11813,9 +11829,9 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="84"/>
-      <c r="B30" s="109"/>
+      <c r="B30" s="103"/>
       <c r="C30" s="60" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D30" s="10">
         <f>SUM(D31:D33)</f>
@@ -11884,9 +11900,9 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="84"/>
-      <c r="B31" s="110"/>
+      <c r="B31" s="104"/>
       <c r="C31" s="66" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D31" s="24">
         <v>2</v>
@@ -11914,9 +11930,9 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="84"/>
-      <c r="B32" s="110"/>
+      <c r="B32" s="104"/>
       <c r="C32" s="66" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D32" s="24"/>
       <c r="E32" s="17"/>
@@ -11940,9 +11956,9 @@
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="84"/>
-      <c r="B33" s="111"/>
+      <c r="B33" s="105"/>
       <c r="C33" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D33" s="26"/>
       <c r="E33" s="18"/>
@@ -11968,7 +11984,7 @@
       <c r="A34" s="84"/>
       <c r="B34" s="93"/>
       <c r="C34" s="60" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D34" s="10">
         <f t="shared" ref="D34:R34" si="8">SUM(D35:D37)</f>
@@ -12039,7 +12055,7 @@
       <c r="A35" s="84"/>
       <c r="B35" s="94"/>
       <c r="C35" s="66" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D35" s="24">
         <v>2</v>
@@ -12069,7 +12085,7 @@
       <c r="A36" s="84"/>
       <c r="B36" s="94"/>
       <c r="C36" s="66" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D36" s="24">
         <v>8</v>
@@ -12099,7 +12115,7 @@
       <c r="A37" s="84"/>
       <c r="B37" s="94"/>
       <c r="C37" s="66" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D37" s="24"/>
       <c r="E37" s="17"/>
@@ -12123,9 +12139,9 @@
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="84"/>
-      <c r="B38" s="109"/>
+      <c r="B38" s="103"/>
       <c r="C38" s="60" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D38" s="10">
         <f t="shared" ref="D38:R38" si="10">SUM(D39:D41)</f>
@@ -12194,9 +12210,9 @@
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="84"/>
-      <c r="B39" s="110"/>
+      <c r="B39" s="104"/>
       <c r="C39" s="66" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D39" s="25">
         <v>2</v>
@@ -12224,9 +12240,9 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="84"/>
-      <c r="B40" s="110"/>
+      <c r="B40" s="104"/>
       <c r="C40" s="66" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D40" s="25"/>
       <c r="E40" s="17"/>
@@ -12250,9 +12266,9 @@
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="84"/>
-      <c r="B41" s="111"/>
+      <c r="B41" s="105"/>
       <c r="C41" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D41" s="26"/>
       <c r="E41" s="18"/>
@@ -12276,9 +12292,9 @@
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="84"/>
-      <c r="B42" s="109"/>
+      <c r="B42" s="103"/>
       <c r="C42" s="60" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D42" s="10">
         <f>SUM(D43:D45)</f>
@@ -12347,9 +12363,9 @@
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="84"/>
-      <c r="B43" s="110"/>
+      <c r="B43" s="104"/>
       <c r="C43" s="66" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D43" s="24"/>
       <c r="E43" s="17"/>
@@ -12373,9 +12389,9 @@
     </row>
     <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="84"/>
-      <c r="B44" s="110"/>
+      <c r="B44" s="104"/>
       <c r="C44" s="66" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D44" s="24">
         <v>4.5</v>
@@ -12405,9 +12421,9 @@
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="84"/>
-      <c r="B45" s="111"/>
+      <c r="B45" s="105"/>
       <c r="C45" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D45" s="26"/>
       <c r="E45" s="18"/>
@@ -12431,9 +12447,9 @@
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="84"/>
-      <c r="B46" s="109"/>
+      <c r="B46" s="103"/>
       <c r="C46" s="60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D46" s="10">
         <f>SUM(D47:D49)</f>
@@ -12502,9 +12518,9 @@
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="84"/>
-      <c r="B47" s="110"/>
+      <c r="B47" s="104"/>
       <c r="C47" s="66" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D47" s="24">
         <v>2</v>
@@ -12532,9 +12548,9 @@
     </row>
     <row r="48" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="84"/>
-      <c r="B48" s="110"/>
+      <c r="B48" s="104"/>
       <c r="C48" s="66" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D48" s="24"/>
       <c r="E48" s="17"/>
@@ -12558,9 +12574,9 @@
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="85"/>
-      <c r="B49" s="111"/>
+      <c r="B49" s="105"/>
       <c r="C49" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D49" s="26"/>
       <c r="E49" s="18"/>
@@ -12584,10 +12600,10 @@
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="75"/>
-      <c r="B50" s="113" t="s">
-        <v>26</v>
-      </c>
-      <c r="C50" s="113"/>
+      <c r="B50" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" s="107"/>
       <c r="D50" s="2">
         <f>SUM(D6,D10,D14,D34,D38,D18,D22,D26,D30,D42,D46)</f>
         <v>44</v>
@@ -12656,13 +12672,13 @@
     <row r="51" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="52" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="83" t="s">
-        <v>12</v>
-      </c>
-      <c r="B52" s="96">
+        <v>11</v>
+      </c>
+      <c r="B52" s="98">
         <v>28</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D52" s="15">
         <f>SUM(D53:D55)</f>
@@ -12727,9 +12743,9 @@
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="84"/>
-      <c r="B53" s="97"/>
+      <c r="B53" s="99"/>
       <c r="C53" s="70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D53" s="24">
         <f>D7</f>
@@ -12780,9 +12796,9 @@
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="84"/>
-      <c r="B54" s="97"/>
+      <c r="B54" s="99"/>
       <c r="C54" s="70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D54" s="24">
         <f>D8</f>
@@ -12805,9 +12821,9 @@
     </row>
     <row r="55" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="84"/>
-      <c r="B55" s="98"/>
+      <c r="B55" s="100"/>
       <c r="C55" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D55" s="24">
         <f>D9</f>
@@ -12830,11 +12846,11 @@
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="84"/>
-      <c r="B56" s="106">
+      <c r="B56" s="111">
         <v>16</v>
       </c>
       <c r="C56" s="47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D56" s="10">
         <f>SUM(D57:D59)</f>
@@ -12899,9 +12915,9 @@
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="84"/>
-      <c r="B57" s="107"/>
+      <c r="B57" s="112"/>
       <c r="C57" s="70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D57" s="24">
         <f>D11</f>
@@ -12952,9 +12968,9 @@
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="84"/>
-      <c r="B58" s="107"/>
+      <c r="B58" s="112"/>
       <c r="C58" s="70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D58" s="24">
         <f>D12</f>
@@ -12977,9 +12993,9 @@
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="84"/>
-      <c r="B59" s="108"/>
+      <c r="B59" s="113"/>
       <c r="C59" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D59" s="24">
         <f>D13</f>
@@ -13002,11 +13018,11 @@
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="84"/>
-      <c r="B60" s="106">
+      <c r="B60" s="111">
         <v>9</v>
       </c>
       <c r="C60" s="60" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D60" s="10">
         <f>SUM(D61:D63)</f>
@@ -13071,9 +13087,9 @@
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="84"/>
-      <c r="B61" s="107"/>
+      <c r="B61" s="112"/>
       <c r="C61" s="70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D61" s="24">
         <f>D15</f>
@@ -13124,9 +13140,9 @@
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="84"/>
-      <c r="B62" s="107"/>
+      <c r="B62" s="112"/>
       <c r="C62" s="70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D62" s="24">
         <f>D16</f>
@@ -13177,9 +13193,9 @@
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="84"/>
-      <c r="B63" s="108"/>
+      <c r="B63" s="113"/>
       <c r="C63" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D63" s="24">
         <f>D17</f>
@@ -13202,11 +13218,11 @@
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="84"/>
-      <c r="B64" s="106" t="s">
-        <v>56</v>
+      <c r="B64" s="111" t="s">
+        <v>55</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D64" s="10">
         <f>SUM(D65:D67)</f>
@@ -13271,9 +13287,9 @@
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="84"/>
-      <c r="B65" s="107"/>
+      <c r="B65" s="112"/>
       <c r="C65" s="70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D65" s="24">
         <f>D19</f>
@@ -13296,9 +13312,9 @@
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="84"/>
-      <c r="B66" s="107"/>
+      <c r="B66" s="112"/>
       <c r="C66" s="70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D66" s="24">
         <f>D20</f>
@@ -13321,9 +13337,9 @@
     </row>
     <row r="67" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="84"/>
-      <c r="B67" s="108"/>
+      <c r="B67" s="113"/>
       <c r="C67" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D67" s="24">
         <f>D21</f>
@@ -13374,11 +13390,11 @@
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="84"/>
-      <c r="B68" s="96" t="s">
-        <v>57</v>
+      <c r="B68" s="98" t="s">
+        <v>56</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D68" s="10">
         <f>SUM(D69:D71)</f>
@@ -13443,9 +13459,9 @@
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="84"/>
-      <c r="B69" s="97"/>
+      <c r="B69" s="99"/>
       <c r="C69" s="70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D69" s="24">
         <f>D23</f>
@@ -13496,9 +13512,9 @@
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="84"/>
-      <c r="B70" s="97"/>
+      <c r="B70" s="99"/>
       <c r="C70" s="70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D70" s="24">
         <f>D24</f>
@@ -13549,9 +13565,9 @@
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="85"/>
-      <c r="B71" s="98"/>
+      <c r="B71" s="100"/>
       <c r="C71" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D71" s="24">
         <f>D25</f>
@@ -13574,11 +13590,11 @@
     </row>
     <row r="72" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="114" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B72" s="67"/>
       <c r="C72" s="60" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D72" s="10">
         <f>SUM(D73:D75)</f>
@@ -13645,7 +13661,7 @@
       <c r="A73" s="115"/>
       <c r="B73" s="68"/>
       <c r="C73" s="70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D73" s="24">
         <f>D27</f>
@@ -13698,7 +13714,7 @@
       <c r="A74" s="115"/>
       <c r="B74" s="68"/>
       <c r="C74" s="70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D74" s="24">
         <f>D28</f>
@@ -13723,7 +13739,7 @@
       <c r="A75" s="115"/>
       <c r="B75" s="69"/>
       <c r="C75" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D75" s="24">
         <f>D29</f>
@@ -13746,9 +13762,9 @@
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="115"/>
-      <c r="B76" s="109"/>
+      <c r="B76" s="103"/>
       <c r="C76" s="60" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D76" s="10">
         <f>SUM(D77:D79)</f>
@@ -13813,9 +13829,9 @@
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="115"/>
-      <c r="B77" s="110"/>
+      <c r="B77" s="104"/>
       <c r="C77" s="70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D77" s="24">
         <f>D31</f>
@@ -13866,9 +13882,9 @@
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="115"/>
-      <c r="B78" s="110"/>
+      <c r="B78" s="104"/>
       <c r="C78" s="70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D78" s="24">
         <f>D32</f>
@@ -13891,9 +13907,9 @@
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" s="115"/>
-      <c r="B79" s="111"/>
+      <c r="B79" s="105"/>
       <c r="C79" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D79" s="24">
         <f>D33</f>
@@ -13916,9 +13932,9 @@
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" s="115"/>
-      <c r="B80" s="96"/>
+      <c r="B80" s="98"/>
       <c r="C80" s="60" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D80" s="10">
         <f>SUM(D81:D83)</f>
@@ -13983,9 +13999,9 @@
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="115"/>
-      <c r="B81" s="97"/>
+      <c r="B81" s="99"/>
       <c r="C81" s="70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D81" s="24">
         <f>D35</f>
@@ -14036,9 +14052,9 @@
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="115"/>
-      <c r="B82" s="97"/>
+      <c r="B82" s="99"/>
       <c r="C82" s="70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D82" s="24">
         <f>D36</f>
@@ -14089,9 +14105,9 @@
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="115"/>
-      <c r="B83" s="98"/>
+      <c r="B83" s="100"/>
       <c r="C83" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D83" s="26">
         <f>D37</f>
@@ -14114,9 +14130,9 @@
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="115"/>
-      <c r="B84" s="109"/>
+      <c r="B84" s="103"/>
       <c r="C84" s="60" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D84" s="10">
         <f>SUM(D85:D87)</f>
@@ -14181,9 +14197,9 @@
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="115"/>
-      <c r="B85" s="110"/>
+      <c r="B85" s="104"/>
       <c r="C85" s="70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D85" s="24">
         <f>D39</f>
@@ -14234,9 +14250,9 @@
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="115"/>
-      <c r="B86" s="110"/>
+      <c r="B86" s="104"/>
       <c r="C86" s="70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D86" s="24">
         <f>D40</f>
@@ -14287,9 +14303,9 @@
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" s="115"/>
-      <c r="B87" s="111"/>
+      <c r="B87" s="105"/>
       <c r="C87" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D87" s="26">
         <f>D41</f>
@@ -14312,9 +14328,9 @@
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" s="115"/>
-      <c r="B88" s="109"/>
+      <c r="B88" s="103"/>
       <c r="C88" s="60" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D88" s="10">
         <f>SUM(D89:D91)</f>
@@ -14379,9 +14395,9 @@
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" s="115"/>
-      <c r="B89" s="110"/>
+      <c r="B89" s="104"/>
       <c r="C89" s="70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D89" s="24">
         <f>D43</f>
@@ -14404,9 +14420,9 @@
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" s="115"/>
-      <c r="B90" s="110"/>
+      <c r="B90" s="104"/>
       <c r="C90" s="70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D90" s="24">
         <f>D44</f>
@@ -14457,9 +14473,9 @@
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" s="115"/>
-      <c r="B91" s="111"/>
+      <c r="B91" s="105"/>
       <c r="C91" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D91" s="26">
         <f>D45</f>
@@ -14482,9 +14498,9 @@
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" s="115"/>
-      <c r="B92" s="109"/>
+      <c r="B92" s="103"/>
       <c r="C92" s="60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D92" s="10">
         <f>SUM(D93:D95)</f>
@@ -14549,9 +14565,9 @@
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" s="115"/>
-      <c r="B93" s="110"/>
+      <c r="B93" s="104"/>
       <c r="C93" s="70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D93" s="24">
         <f>D47</f>
@@ -14602,9 +14618,9 @@
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" s="115"/>
-      <c r="B94" s="110"/>
+      <c r="B94" s="104"/>
       <c r="C94" s="70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D94" s="24">
         <f>D48</f>
@@ -14655,9 +14671,9 @@
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" s="115"/>
-      <c r="B95" s="111"/>
+      <c r="B95" s="105"/>
       <c r="C95" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D95" s="26">
         <f>D49</f>
@@ -14679,10 +14695,10 @@
       <c r="R95" s="39"/>
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B96" s="112" t="s">
-        <v>26</v>
-      </c>
-      <c r="C96" s="112"/>
+      <c r="B96" s="106" t="s">
+        <v>25</v>
+      </c>
+      <c r="C96" s="106"/>
       <c r="D96" s="2">
         <f>SUM(D52,D56,D60,D64,D68,D72,D76,D80,D84,D88,D92)</f>
         <v>44</v>
@@ -14808,6 +14824,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B92:B95"/>
+    <mergeCell ref="A72:A95"/>
+    <mergeCell ref="A52:A71"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="E2:K2"/>
+    <mergeCell ref="B84:B87"/>
+    <mergeCell ref="B88:B91"/>
+    <mergeCell ref="A6:A25"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="A26:A49"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="B18:B21"/>
     <mergeCell ref="L2:R2"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="B10:B13"/>
@@ -14824,18 +14852,6 @@
     <mergeCell ref="B38:B41"/>
     <mergeCell ref="B30:B33"/>
     <mergeCell ref="B42:B45"/>
-    <mergeCell ref="B92:B95"/>
-    <mergeCell ref="A72:A95"/>
-    <mergeCell ref="A52:A71"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="E2:K2"/>
-    <mergeCell ref="B84:B87"/>
-    <mergeCell ref="B88:B91"/>
-    <mergeCell ref="A6:A25"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="A26:A49"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="B18:B21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -14870,7 +14886,7 @@
   <sheetData>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E2" s="90" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="91"/>
       <c r="G2" s="91"/>
@@ -14879,7 +14895,7 @@
       <c r="J2" s="91"/>
       <c r="K2" s="91"/>
       <c r="L2" s="90" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M2" s="91"/>
       <c r="N2" s="91"/>
@@ -14890,7 +14906,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D3" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="40">
         <v>42079</v>
@@ -14937,7 +14953,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D4" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="43">
         <v>1</v>
@@ -14984,13 +15000,13 @@
     </row>
     <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="48" t="s">
-        <v>14</v>
-      </c>
       <c r="D5" s="55" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="53"/>
       <c r="F5" s="53"/>
@@ -15007,18 +15023,18 @@
       <c r="Q5" s="61"/>
       <c r="R5" s="61"/>
       <c r="S5" s="54" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="83" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="116" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D6" s="15">
         <f>SUM(D7:D9)</f>
@@ -15089,7 +15105,7 @@
       <c r="A7" s="84"/>
       <c r="B7" s="117"/>
       <c r="C7" s="70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="24">
         <v>1</v>
@@ -15119,7 +15135,7 @@
       <c r="A8" s="84"/>
       <c r="B8" s="117"/>
       <c r="C8" s="70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="24">
         <v>3</v>
@@ -15149,7 +15165,7 @@
       <c r="A9" s="84"/>
       <c r="B9" s="118"/>
       <c r="C9" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="26"/>
       <c r="E9" s="18"/>
@@ -15177,7 +15193,7 @@
         <v>26</v>
       </c>
       <c r="C10" s="47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" s="10">
         <f>SUM(D11:D13)</f>
@@ -15248,7 +15264,7 @@
       <c r="A11" s="84"/>
       <c r="B11" s="120"/>
       <c r="C11" s="70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="24">
         <v>2</v>
@@ -15278,7 +15294,7 @@
       <c r="A12" s="84"/>
       <c r="B12" s="120"/>
       <c r="C12" s="70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="24">
         <v>1</v>
@@ -15308,7 +15324,7 @@
       <c r="A13" s="84"/>
       <c r="B13" s="121"/>
       <c r="C13" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="18"/>
@@ -15336,7 +15352,7 @@
         <v>26</v>
       </c>
       <c r="C14" s="60" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14" s="10">
         <f>SUM(D15:D17)</f>
@@ -15407,7 +15423,7 @@
       <c r="A15" s="84"/>
       <c r="B15" s="120"/>
       <c r="C15" s="70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="24">
         <v>10</v>
@@ -15439,7 +15455,7 @@
       <c r="A16" s="84"/>
       <c r="B16" s="120"/>
       <c r="C16" s="70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" s="24"/>
       <c r="E16" s="17"/>
@@ -15465,7 +15481,7 @@
       <c r="A17" s="84"/>
       <c r="B17" s="121"/>
       <c r="C17" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="26">
         <v>15</v>
@@ -15498,10 +15514,10 @@
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="84"/>
       <c r="B18" s="119" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D18" s="10">
         <f>SUM(D19:D21)</f>
@@ -15572,7 +15588,7 @@
       <c r="A19" s="84"/>
       <c r="B19" s="120"/>
       <c r="C19" s="70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D19" s="24"/>
       <c r="E19" s="17"/>
@@ -15598,7 +15614,7 @@
       <c r="A20" s="84"/>
       <c r="B20" s="120"/>
       <c r="C20" s="70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D20" s="24">
         <v>7</v>
@@ -15630,7 +15646,7 @@
       <c r="A21" s="84"/>
       <c r="B21" s="121"/>
       <c r="C21" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" s="26"/>
       <c r="E21" s="18"/>
@@ -15654,11 +15670,11 @@
     </row>
     <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="83" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="116"/>
       <c r="C22" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D22" s="10">
         <f>SUM(D23:D25)</f>
@@ -15729,7 +15745,7 @@
       <c r="A23" s="84"/>
       <c r="B23" s="117"/>
       <c r="C23" s="70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D23" s="24">
         <v>5</v>
@@ -15759,7 +15775,7 @@
       <c r="A24" s="84"/>
       <c r="B24" s="117"/>
       <c r="C24" s="70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D24" s="24">
         <v>3</v>
@@ -15789,7 +15805,7 @@
       <c r="A25" s="84"/>
       <c r="B25" s="118"/>
       <c r="C25" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D25" s="26">
         <v>4</v>
@@ -15821,7 +15837,7 @@
       <c r="A26" s="84"/>
       <c r="B26" s="72"/>
       <c r="C26" s="60" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D26" s="10">
         <f>SUM(D27:D29)</f>
@@ -15892,7 +15908,7 @@
       <c r="A27" s="84"/>
       <c r="B27" s="73"/>
       <c r="C27" s="70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D27" s="24">
         <v>5</v>
@@ -15924,7 +15940,7 @@
       <c r="A28" s="84"/>
       <c r="B28" s="73"/>
       <c r="C28" s="70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D28" s="24">
         <v>5</v>
@@ -15956,7 +15972,7 @@
       <c r="A29" s="85"/>
       <c r="B29" s="74"/>
       <c r="C29" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D29" s="26">
         <v>5</v>
@@ -15986,10 +16002,10 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="71"/>
-      <c r="B30" s="113" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="113"/>
+      <c r="B30" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="107"/>
       <c r="D30" s="2">
         <f>SUM(D6,D10,D14,D18,D22,D26)</f>
         <v>66</v>
@@ -16058,13 +16074,13 @@
     <row r="31" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="83" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B32" s="116" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D32" s="15">
         <f>SUM(D33:D35)</f>
@@ -16131,7 +16147,7 @@
       <c r="A33" s="84"/>
       <c r="B33" s="117"/>
       <c r="C33" s="76" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D33" s="24">
         <v>1</v>
@@ -16183,7 +16199,7 @@
       <c r="A34" s="84"/>
       <c r="B34" s="117"/>
       <c r="C34" s="76" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D34" s="24">
         <v>3</v>
@@ -16235,7 +16251,7 @@
       <c r="A35" s="84"/>
       <c r="B35" s="118"/>
       <c r="C35" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D35" s="26"/>
       <c r="E35" s="31"/>
@@ -16259,7 +16275,7 @@
         <v>26</v>
       </c>
       <c r="C36" s="47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D36" s="10">
         <f>SUM(D37:D39)</f>
@@ -16326,7 +16342,7 @@
       <c r="A37" s="84"/>
       <c r="B37" s="120"/>
       <c r="C37" s="76" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D37" s="24">
         <v>2</v>
@@ -16385,7 +16401,7 @@
       <c r="A38" s="84"/>
       <c r="B38" s="120"/>
       <c r="C38" s="76" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D38" s="24">
         <v>1</v>
@@ -16451,7 +16467,7 @@
       <c r="A39" s="84"/>
       <c r="B39" s="121"/>
       <c r="C39" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D39" s="26"/>
       <c r="E39" s="31"/>
@@ -16475,7 +16491,7 @@
         <v>26</v>
       </c>
       <c r="C40" s="60" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D40" s="10">
         <f>SUM(D41:D43)</f>
@@ -16542,7 +16558,7 @@
       <c r="A41" s="84"/>
       <c r="B41" s="120"/>
       <c r="C41" s="76" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D41" s="24">
         <v>10</v>
@@ -16601,7 +16617,7 @@
       <c r="A42" s="84"/>
       <c r="B42" s="120"/>
       <c r="C42" s="76" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D42" s="24"/>
       <c r="E42" s="31"/>
@@ -16625,7 +16641,7 @@
       <c r="A43" s="84"/>
       <c r="B43" s="121"/>
       <c r="C43" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D43" s="26">
         <v>15</v>
@@ -16648,10 +16664,10 @@
     <row r="44" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="84"/>
       <c r="B44" s="119" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D44" s="10">
         <f>SUM(D45:D47)</f>
@@ -16718,7 +16734,7 @@
       <c r="A45" s="84"/>
       <c r="B45" s="120"/>
       <c r="C45" s="76" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D45" s="24"/>
       <c r="E45" s="31"/>
@@ -16740,7 +16756,7 @@
       <c r="A46" s="84"/>
       <c r="B46" s="120"/>
       <c r="C46" s="76" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D46" s="24">
         <v>7</v>
@@ -16792,7 +16808,7 @@
       <c r="A47" s="84"/>
       <c r="B47" s="121"/>
       <c r="C47" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D47" s="26"/>
       <c r="E47" s="33"/>
@@ -16812,11 +16828,11 @@
     </row>
     <row r="48" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="83" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B48" s="116"/>
       <c r="C48" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D48" s="10">
         <f>SUM(D49:D51)</f>
@@ -16883,7 +16899,7 @@
       <c r="A49" s="84"/>
       <c r="B49" s="117"/>
       <c r="C49" s="76" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D49" s="24">
         <v>5</v>
@@ -16935,7 +16951,7 @@
       <c r="A50" s="84"/>
       <c r="B50" s="117"/>
       <c r="C50" s="76" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D50" s="24">
         <v>3</v>
@@ -16987,7 +17003,7 @@
       <c r="A51" s="84"/>
       <c r="B51" s="118"/>
       <c r="C51" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D51" s="26">
         <v>4</v>
@@ -17011,7 +17027,7 @@
       <c r="A52" s="84"/>
       <c r="B52" s="72"/>
       <c r="C52" s="60" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D52" s="10">
         <f>SUM(D53:D55)</f>
@@ -17078,7 +17094,7 @@
       <c r="A53" s="84"/>
       <c r="B53" s="73"/>
       <c r="C53" s="76" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D53" s="24">
         <v>5</v>
@@ -17130,7 +17146,7 @@
       <c r="A54" s="84"/>
       <c r="B54" s="73"/>
       <c r="C54" s="76" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D54" s="24">
         <v>5</v>
@@ -17182,7 +17198,7 @@
       <c r="A55" s="85"/>
       <c r="B55" s="74"/>
       <c r="C55" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D55" s="26">
         <v>5</v>
@@ -17205,10 +17221,10 @@
       <c r="R55" s="39"/>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B56" s="112" t="s">
-        <v>26</v>
-      </c>
-      <c r="C56" s="112"/>
+      <c r="B56" s="106" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56" s="106"/>
       <c r="D56" s="2">
         <f>SUM(D32, D36, D40, D44, D48,D52)</f>
         <v>66</v>
@@ -17336,6 +17352,13 @@
     <row r="72" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="B48:B51"/>
     <mergeCell ref="A32:A47"/>
     <mergeCell ref="A48:A55"/>
     <mergeCell ref="A22:A29"/>
@@ -17347,13 +17370,6 @@
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="A6:A21"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="B48:B51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -17365,7 +17381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
@@ -17389,7 +17405,7 @@
   <sheetData>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E2" s="90" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="91"/>
       <c r="G2" s="91"/>
@@ -17398,7 +17414,7 @@
       <c r="J2" s="91"/>
       <c r="K2" s="91"/>
       <c r="L2" s="90" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M2" s="91"/>
       <c r="N2" s="91"/>
@@ -17409,7 +17425,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D3" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="40">
         <v>42101</v>
@@ -17456,7 +17472,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D4" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="43">
         <v>1</v>
@@ -17503,13 +17519,13 @@
     </row>
     <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="48" t="s">
-        <v>14</v>
-      </c>
       <c r="D5" s="55" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="53"/>
       <c r="F5" s="53"/>
@@ -17526,18 +17542,18 @@
       <c r="Q5" s="61"/>
       <c r="R5" s="61"/>
       <c r="S5" s="54" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="122" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="116" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D6" s="15">
         <f>SUM(D7:D9)</f>
@@ -17608,7 +17624,7 @@
       <c r="A7" s="123"/>
       <c r="B7" s="117"/>
       <c r="C7" s="77" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="24">
         <v>6</v>
@@ -17636,7 +17652,7 @@
       <c r="A8" s="123"/>
       <c r="B8" s="117"/>
       <c r="C8" s="77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="24"/>
       <c r="E8" s="62"/>
@@ -17662,7 +17678,7 @@
       <c r="A9" s="123"/>
       <c r="B9" s="118"/>
       <c r="C9" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="26"/>
       <c r="E9" s="18"/>
@@ -17687,10 +17703,10 @@
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="123"/>
       <c r="B10" s="116" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" s="15">
         <f>SUM(D11:D13)</f>
@@ -17761,7 +17777,7 @@
       <c r="A11" s="123"/>
       <c r="B11" s="117"/>
       <c r="C11" s="77" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="24">
         <v>4</v>
@@ -17789,7 +17805,7 @@
       <c r="A12" s="123"/>
       <c r="B12" s="117"/>
       <c r="C12" s="77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="24">
         <v>4</v>
@@ -17819,7 +17835,7 @@
       <c r="A13" s="123"/>
       <c r="B13" s="118"/>
       <c r="C13" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="18"/>
@@ -17844,10 +17860,10 @@
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="123"/>
       <c r="B14" s="119" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="47" t="s">
         <v>79</v>
-      </c>
-      <c r="C14" s="47" t="s">
-        <v>80</v>
       </c>
       <c r="D14" s="10">
         <f>SUM(D15:D17)</f>
@@ -17918,7 +17934,7 @@
       <c r="A15" s="123"/>
       <c r="B15" s="120"/>
       <c r="C15" s="77" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="24"/>
       <c r="E15" s="17"/>
@@ -17944,7 +17960,7 @@
       <c r="A16" s="123"/>
       <c r="B16" s="120"/>
       <c r="C16" s="77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" s="24"/>
       <c r="E16" s="17"/>
@@ -17970,7 +17986,7 @@
       <c r="A17" s="123"/>
       <c r="B17" s="121"/>
       <c r="C17" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="26">
         <v>2</v>
@@ -18002,7 +18018,7 @@
         <v>39</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D18" s="15">
         <f>SUM(D19:D21)</f>
@@ -18073,7 +18089,7 @@
       <c r="A19" s="123"/>
       <c r="B19" s="117"/>
       <c r="C19" s="77" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D19" s="24"/>
       <c r="E19" s="17"/>
@@ -18099,7 +18115,7 @@
       <c r="A20" s="123"/>
       <c r="B20" s="117"/>
       <c r="C20" s="77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="62"/>
@@ -18125,7 +18141,7 @@
       <c r="A21" s="123"/>
       <c r="B21" s="118"/>
       <c r="C21" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" s="26">
         <v>2</v>
@@ -18154,10 +18170,10 @@
     <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="123"/>
       <c r="B22" s="116" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D22" s="15">
         <f>SUM(D23:D25)</f>
@@ -18228,7 +18244,7 @@
       <c r="A23" s="123"/>
       <c r="B23" s="117"/>
       <c r="C23" s="77" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D23" s="24">
         <v>3</v>
@@ -18256,7 +18272,7 @@
       <c r="A24" s="123"/>
       <c r="B24" s="117"/>
       <c r="C24" s="77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D24" s="24">
         <v>5</v>
@@ -18286,7 +18302,7 @@
       <c r="A25" s="123"/>
       <c r="B25" s="118"/>
       <c r="C25" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D25" s="26"/>
       <c r="E25" s="18"/>
@@ -18311,10 +18327,10 @@
     <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="123"/>
       <c r="B26" s="119" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C26" s="47" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D26" s="10">
         <f>SUM(D27:D29)</f>
@@ -18385,7 +18401,7 @@
       <c r="A27" s="123"/>
       <c r="B27" s="120"/>
       <c r="C27" s="77" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D27" s="24"/>
       <c r="E27" s="17"/>
@@ -18411,7 +18427,7 @@
       <c r="A28" s="123"/>
       <c r="B28" s="120"/>
       <c r="C28" s="77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D28" s="24">
         <v>7</v>
@@ -18441,7 +18457,7 @@
       <c r="A29" s="123"/>
       <c r="B29" s="121"/>
       <c r="C29" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D29" s="26"/>
       <c r="E29" s="18"/>
@@ -18469,7 +18485,7 @@
         <v>40</v>
       </c>
       <c r="C30" s="60" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D30" s="10">
         <f>SUM(D31:D33)</f>
@@ -18540,7 +18556,7 @@
       <c r="A31" s="123"/>
       <c r="B31" s="120"/>
       <c r="C31" s="77" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D31" s="24"/>
       <c r="E31" s="17"/>
@@ -18566,7 +18582,7 @@
       <c r="A32" s="123"/>
       <c r="B32" s="120"/>
       <c r="C32" s="77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D32" s="24">
         <v>2</v>
@@ -18596,7 +18612,7 @@
       <c r="A33" s="123"/>
       <c r="B33" s="121"/>
       <c r="C33" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D33" s="26">
         <v>6</v>
@@ -18628,7 +18644,7 @@
         <v>41</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D34" s="10">
         <f>SUM(D35:D37)</f>
@@ -18699,7 +18715,7 @@
       <c r="A35" s="123"/>
       <c r="B35" s="120"/>
       <c r="C35" s="77" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D35" s="24">
         <v>6</v>
@@ -18727,7 +18743,7 @@
       <c r="A36" s="123"/>
       <c r="B36" s="120"/>
       <c r="C36" s="77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D36" s="24"/>
       <c r="E36" s="17"/>
@@ -18753,7 +18769,7 @@
       <c r="A37" s="123"/>
       <c r="B37" s="121"/>
       <c r="C37" s="46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D37" s="26"/>
       <c r="E37" s="18"/>
@@ -18777,10 +18793,10 @@
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="75"/>
-      <c r="B38" s="113" t="s">
-        <v>26</v>
-      </c>
-      <c r="C38" s="113"/>
+      <c r="B38" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" s="107"/>
       <c r="D38" s="2">
         <f t="shared" ref="D38:S38" si="12">SUM(D6,D10,D14,D18, D22, D26, D30, D34)</f>
         <v>47</v>
@@ -18901,6 +18917,7 @@
     <row r="72" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A6:A37"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="E2:K2"/>
     <mergeCell ref="L2:R2"/>
@@ -18912,7 +18929,6 @@
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A6:A37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>